<commit_message>
penilaian sampai link dan blade system
</commit_message>
<xml_diff>
--- a/XIIRPL2(❁´◡`❁)(❁´◡`❁)(❁´◡`❁)(u‿ฺu✿ฺ)/DATA PRAKTIK XII RPl 2.xlsx
+++ b/XIIRPL2(❁´◡`❁)(❁´◡`❁)(❁´◡`❁)(u‿ฺu✿ฺ)/DATA PRAKTIK XII RPl 2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AdeSetiyawan)(✿◡‿◡)(✿◡‿◡)\XIIRPL2(❁´◡`❁)(❁´◡`❁)(❁´◡`❁)(u‿ฺu✿ฺ)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FDDAC92-0464-482B-8E0E-D62F494AAE77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DB3B05D-367F-4A8D-A52F-DDCF44A5D58C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7A470BEC-FF9B-4C58-B3A9-6A89F2B6EB46}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="68">
   <si>
     <t xml:space="preserve">Nama </t>
   </si>
@@ -192,13 +192,6 @@
     <t>Blade</t>
   </si>
   <si>
-    <t>ULANGAN 2</t>
-  </si>
-  <si>
-    <t>ULANGAN
-1</t>
-  </si>
-  <si>
     <t>1. BANNER</t>
   </si>
   <si>
@@ -208,20 +201,58 @@
     <t>3. @yield('sidebar')</t>
   </si>
   <si>
-    <t>4. @yield('contentutama')</t>
-  </si>
-  <si>
     <t>5. copyright © 2023 maryoko</t>
   </si>
   <si>
     <t>natasya</t>
+  </si>
+  <si>
+    <t>DropOut</t>
+  </si>
+  <si>
+    <t>SESI ULANGAN</t>
+  </si>
+  <si>
+    <t>DIV</t>
+  </si>
+  <si>
+    <t>DIV
+DIV</t>
+  </si>
+  <si>
+    <t>banner</t>
+  </si>
+  <si>
+    <t>navbar</t>
+  </si>
+  <si>
+    <t>sidebar</t>
+  </si>
+  <si>
+    <t>isi</t>
+  </si>
+  <si>
+    <t>4. @yield('isi')</t>
+  </si>
+  <si>
+    <t>footer</t>
+  </si>
+  <si>
+    <t>ULANGAN 1
+(18-01-2023)
+100 point</t>
+  </si>
+  <si>
+    <t>ULANGAN2
+( nunggu )
+100 point</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -247,6 +278,22 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="30"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -290,7 +337,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -455,9 +502,31 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color indexed="64"/>
       </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -468,9 +537,7 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
+      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -479,9 +546,7 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
+      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -492,24 +557,24 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -519,7 +584,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -550,13 +615,13 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -568,6 +633,15 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -589,15 +663,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -607,21 +672,49 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -936,35 +1029,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E8966E4-2275-4E9F-82CA-974F40DBA593}">
-  <dimension ref="D1:R1048576"/>
+  <dimension ref="C1:R1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="M14" sqref="M14"/>
+      <selection pane="bottomLeft" activeCell="R10" sqref="R10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="9.140625" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" customWidth="1"/>
     <col min="4" max="4" width="6.5703125" style="2" customWidth="1"/>
     <col min="5" max="5" width="15.28515625" customWidth="1"/>
     <col min="6" max="6" width="5.5703125" style="2" customWidth="1"/>
     <col min="7" max="9" width="12.7109375" style="2" customWidth="1"/>
     <col min="10" max="10" width="12.7109375" style="1" customWidth="1"/>
     <col min="11" max="16" width="12.7109375" customWidth="1"/>
-    <col min="17" max="17" width="10.5703125" customWidth="1"/>
-    <col min="18" max="18" width="10" customWidth="1"/>
+    <col min="17" max="17" width="19" customWidth="1"/>
+    <col min="18" max="18" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D1" s="31" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" s="25" t="s">
+    <row r="1" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C1" s="40" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" s="34" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="18" t="s">
         <v>12</v>
       </c>
       <c r="G1" s="28" t="s">
@@ -975,25 +1071,26 @@
       </c>
       <c r="I1" s="30"/>
       <c r="J1" s="30"/>
-      <c r="K1" s="23" t="s">
+      <c r="K1" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="L1" s="24"/>
-      <c r="M1" s="24"/>
-      <c r="N1" s="24"/>
-      <c r="O1" s="24"/>
-      <c r="P1" s="24"/>
-      <c r="Q1" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="R1" s="18" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="2" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D2" s="32"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
+      <c r="L1" s="27"/>
+      <c r="M1" s="27"/>
+      <c r="N1" s="27"/>
+      <c r="O1" s="27"/>
+      <c r="P1" s="27"/>
+      <c r="Q1" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="R1" s="21" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C2" s="40"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
       <c r="G2" s="29"/>
       <c r="H2" s="15" t="s">
         <v>10</v>
@@ -1022,32 +1119,36 @@
       <c r="P2" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="Q2" s="19"/>
-      <c r="R2" s="18"/>
-    </row>
-    <row r="3" spans="4:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D3" s="33"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
+      <c r="Q2" s="22"/>
+      <c r="R2" s="21"/>
+    </row>
+    <row r="3" spans="3:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C3" s="40"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
       <c r="G3" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="H3" s="20" t="s">
+      <c r="H3" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="I3" s="21"/>
-      <c r="J3" s="22"/>
+      <c r="I3" s="24"/>
+      <c r="J3" s="25"/>
       <c r="K3" s="8"/>
       <c r="L3" s="8"/>
       <c r="M3" s="8"/>
       <c r="N3" s="8"/>
       <c r="O3" s="8"/>
       <c r="P3" s="13"/>
-      <c r="Q3" s="19"/>
-      <c r="R3" s="18"/>
-    </row>
-    <row r="4" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D4" s="6">
+      <c r="Q3" s="22"/>
+      <c r="R3" s="21"/>
+    </row>
+    <row r="4" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C4" s="3">
+        <v>1</v>
+      </c>
+      <c r="D4" s="37">
         <v>1</v>
       </c>
       <c r="E4" s="7" t="s">
@@ -1055,7 +1156,7 @@
       </c>
       <c r="F4" s="6">
         <f t="shared" ref="F4:F38" si="0">((SUM(G4:P4)*10)*70%)+(AVERAGE(Q4:R4)*30%)</f>
-        <v>14</v>
+        <v>22.75</v>
       </c>
       <c r="G4" s="10">
         <v>1</v>
@@ -1063,8 +1164,12 @@
       <c r="H4" s="10">
         <v>1</v>
       </c>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
+      <c r="I4" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="J4" s="10">
+        <v>0.75</v>
+      </c>
       <c r="K4" s="10"/>
       <c r="L4" s="10"/>
       <c r="M4" s="10"/>
@@ -1078,8 +1183,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D5" s="3">
+    <row r="5" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C5" s="3">
+        <v>2</v>
+      </c>
+      <c r="D5" s="38">
         <v>2</v>
       </c>
       <c r="E5" s="4" t="s">
@@ -1087,7 +1195,7 @@
       </c>
       <c r="F5" s="6">
         <f t="shared" si="0"/>
-        <v>19.25</v>
+        <v>26.25</v>
       </c>
       <c r="G5" s="10">
         <v>1</v>
@@ -1098,7 +1206,9 @@
       <c r="I5" s="10">
         <v>0.75</v>
       </c>
-      <c r="J5" s="10"/>
+      <c r="J5" s="10">
+        <v>1</v>
+      </c>
       <c r="K5" s="10"/>
       <c r="L5" s="10"/>
       <c r="M5" s="10"/>
@@ -1112,8 +1222,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D6" s="3">
+    <row r="6" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C6" s="41">
+        <v>1</v>
+      </c>
+      <c r="D6" s="38">
         <v>3</v>
       </c>
       <c r="E6" s="4" t="s">
@@ -1132,7 +1245,9 @@
       <c r="I6" s="10">
         <v>0</v>
       </c>
-      <c r="J6" s="10"/>
+      <c r="J6" s="10">
+        <v>0</v>
+      </c>
       <c r="K6" s="10"/>
       <c r="L6" s="10"/>
       <c r="M6" s="10"/>
@@ -1146,8 +1261,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D7" s="3">
+    <row r="7" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C7" s="3">
+        <v>2</v>
+      </c>
+      <c r="D7" s="38">
         <v>4</v>
       </c>
       <c r="E7" s="4" t="s">
@@ -1155,7 +1273,7 @@
       </c>
       <c r="F7" s="6">
         <f t="shared" si="0"/>
-        <v>19.25</v>
+        <v>26.25</v>
       </c>
       <c r="G7" s="10">
         <v>1</v>
@@ -1166,7 +1284,9 @@
       <c r="I7" s="10">
         <v>0.75</v>
       </c>
-      <c r="J7" s="10"/>
+      <c r="J7" s="10">
+        <v>1</v>
+      </c>
       <c r="K7" s="10"/>
       <c r="L7" s="10"/>
       <c r="M7" s="10"/>
@@ -1180,8 +1300,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D8" s="3">
+    <row r="8" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C8" s="3">
+        <v>1</v>
+      </c>
+      <c r="D8" s="38">
         <v>5</v>
       </c>
       <c r="E8" s="4" t="s">
@@ -1189,7 +1312,7 @@
       </c>
       <c r="F8" s="6">
         <f>((SUM(G8:P8)*10)*70%)+(AVERAGE(Q8:R8)*30%)</f>
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="G8" s="10">
         <v>1</v>
@@ -1200,13 +1323,27 @@
       <c r="I8" s="10">
         <v>1</v>
       </c>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
-      <c r="L8" s="10"/>
-      <c r="M8" s="10"/>
-      <c r="N8" s="10"/>
-      <c r="O8" s="10"/>
-      <c r="P8" s="14"/>
+      <c r="J8" s="10">
+        <v>1</v>
+      </c>
+      <c r="K8" s="10">
+        <v>0</v>
+      </c>
+      <c r="L8" s="10">
+        <v>0</v>
+      </c>
+      <c r="M8" s="10">
+        <v>0</v>
+      </c>
+      <c r="N8" s="10">
+        <v>0</v>
+      </c>
+      <c r="O8" s="10">
+        <v>0</v>
+      </c>
+      <c r="P8" s="14">
+        <v>0</v>
+      </c>
       <c r="Q8" s="5">
         <v>0</v>
       </c>
@@ -1214,14 +1351,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D9" s="3">
+    <row r="9" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C9" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D9" s="39">
         <v>6</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="45" t="s">
         <v>44</v>
       </c>
-      <c r="F9" s="6">
+      <c r="F9" s="33">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1234,7 +1374,9 @@
       <c r="I9" s="10">
         <v>0</v>
       </c>
-      <c r="J9" s="10"/>
+      <c r="J9" s="10">
+        <v>0</v>
+      </c>
       <c r="K9" s="10"/>
       <c r="L9" s="10"/>
       <c r="M9" s="10"/>
@@ -1248,8 +1390,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D10" s="3">
+    <row r="10" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C10" s="3">
+        <v>1</v>
+      </c>
+      <c r="D10" s="38">
         <v>7</v>
       </c>
       <c r="E10" s="4" t="s">
@@ -1257,7 +1402,7 @@
       </c>
       <c r="F10" s="6">
         <f t="shared" si="0"/>
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="G10" s="10">
         <v>1</v>
@@ -1268,7 +1413,9 @@
       <c r="I10" s="10">
         <v>1</v>
       </c>
-      <c r="J10" s="10"/>
+      <c r="J10" s="10">
+        <v>1</v>
+      </c>
       <c r="K10" s="10"/>
       <c r="L10" s="10"/>
       <c r="M10" s="10"/>
@@ -1282,8 +1429,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D11" s="3">
+    <row r="11" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C11" s="3">
+        <v>2</v>
+      </c>
+      <c r="D11" s="38">
         <v>8</v>
       </c>
       <c r="E11" s="4" t="s">
@@ -1291,7 +1441,7 @@
       </c>
       <c r="F11" s="6">
         <f t="shared" si="0"/>
-        <v>19.25</v>
+        <v>26.25</v>
       </c>
       <c r="G11" s="10">
         <v>1</v>
@@ -1302,7 +1452,9 @@
       <c r="I11" s="10">
         <v>0.75</v>
       </c>
-      <c r="J11" s="10"/>
+      <c r="J11" s="10">
+        <v>1</v>
+      </c>
       <c r="K11" s="10"/>
       <c r="L11" s="10"/>
       <c r="M11" s="10"/>
@@ -1316,8 +1468,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D12" s="3">
+    <row r="12" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C12" s="41">
+        <v>1</v>
+      </c>
+      <c r="D12" s="38">
         <v>9</v>
       </c>
       <c r="E12" s="4" t="s">
@@ -1336,7 +1491,9 @@
       <c r="I12" s="10">
         <v>0</v>
       </c>
-      <c r="J12" s="10"/>
+      <c r="J12" s="10">
+        <v>0</v>
+      </c>
       <c r="K12" s="10"/>
       <c r="L12" s="10"/>
       <c r="M12" s="10"/>
@@ -1350,8 +1507,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D13" s="3">
+    <row r="13" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C13" s="3">
+        <v>2</v>
+      </c>
+      <c r="D13" s="38">
         <v>10</v>
       </c>
       <c r="E13" s="4" t="s">
@@ -1359,7 +1519,7 @@
       </c>
       <c r="F13" s="6">
         <f t="shared" si="0"/>
-        <v>19.25</v>
+        <v>26.25</v>
       </c>
       <c r="G13" s="10">
         <v>1</v>
@@ -1370,7 +1530,9 @@
       <c r="I13" s="10">
         <v>0.75</v>
       </c>
-      <c r="J13" s="10"/>
+      <c r="J13" s="10">
+        <v>1</v>
+      </c>
       <c r="K13" s="10"/>
       <c r="L13" s="10"/>
       <c r="M13" s="10"/>
@@ -1384,8 +1546,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D14" s="3">
+    <row r="14" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C14" s="3">
+        <v>1</v>
+      </c>
+      <c r="D14" s="38">
         <v>11</v>
       </c>
       <c r="E14" s="4" t="s">
@@ -1393,7 +1558,7 @@
       </c>
       <c r="F14" s="6">
         <f t="shared" si="0"/>
-        <v>19.25</v>
+        <v>26.25</v>
       </c>
       <c r="G14" s="10">
         <v>1</v>
@@ -1404,7 +1569,9 @@
       <c r="I14" s="10">
         <v>0.75</v>
       </c>
-      <c r="J14" s="10"/>
+      <c r="J14" s="10">
+        <v>1</v>
+      </c>
       <c r="K14" s="10"/>
       <c r="L14" s="10"/>
       <c r="M14" s="10"/>
@@ -1418,8 +1585,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D15" s="3">
+    <row r="15" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C15" s="3">
+        <v>2</v>
+      </c>
+      <c r="D15" s="38">
         <v>12</v>
       </c>
       <c r="E15" s="4" t="s">
@@ -1427,7 +1597,7 @@
       </c>
       <c r="F15" s="6">
         <f t="shared" si="0"/>
-        <v>19.25</v>
+        <v>26.25</v>
       </c>
       <c r="G15" s="10">
         <v>1</v>
@@ -1438,7 +1608,9 @@
       <c r="I15" s="10">
         <v>0.75</v>
       </c>
-      <c r="J15" s="10"/>
+      <c r="J15" s="10">
+        <v>1</v>
+      </c>
       <c r="K15" s="10"/>
       <c r="L15" s="10"/>
       <c r="M15" s="10"/>
@@ -1452,8 +1624,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D16" s="3">
+    <row r="16" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C16" s="3">
+        <v>1</v>
+      </c>
+      <c r="D16" s="38">
         <v>13</v>
       </c>
       <c r="E16" s="4" t="s">
@@ -1461,7 +1636,7 @@
       </c>
       <c r="F16" s="6">
         <f t="shared" si="0"/>
-        <v>19.25</v>
+        <v>26.25</v>
       </c>
       <c r="G16" s="10">
         <v>1</v>
@@ -1472,7 +1647,9 @@
       <c r="I16" s="10">
         <v>0.75</v>
       </c>
-      <c r="J16" s="10"/>
+      <c r="J16" s="10">
+        <v>1</v>
+      </c>
       <c r="K16" s="10"/>
       <c r="L16" s="10"/>
       <c r="M16" s="10"/>
@@ -1486,8 +1663,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D17" s="3">
+    <row r="17" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C17" s="3">
+        <v>2</v>
+      </c>
+      <c r="D17" s="38">
         <v>14</v>
       </c>
       <c r="E17" s="4" t="s">
@@ -1495,7 +1675,7 @@
       </c>
       <c r="F17" s="6">
         <f t="shared" si="0"/>
-        <v>19.25</v>
+        <v>26.25</v>
       </c>
       <c r="G17" s="10">
         <v>1</v>
@@ -1506,7 +1686,9 @@
       <c r="I17" s="10">
         <v>0.75</v>
       </c>
-      <c r="J17" s="10"/>
+      <c r="J17" s="10">
+        <v>1</v>
+      </c>
       <c r="K17" s="10"/>
       <c r="L17" s="10"/>
       <c r="M17" s="10"/>
@@ -1520,8 +1702,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D18" s="3">
+    <row r="18" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C18" s="41">
+        <v>1</v>
+      </c>
+      <c r="D18" s="38">
         <v>15</v>
       </c>
       <c r="E18" s="4" t="s">
@@ -1540,7 +1725,9 @@
       <c r="I18" s="10">
         <v>0</v>
       </c>
-      <c r="J18" s="10"/>
+      <c r="J18" s="10">
+        <v>0</v>
+      </c>
       <c r="K18" s="10"/>
       <c r="L18" s="10"/>
       <c r="M18" s="10"/>
@@ -1554,8 +1741,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D19" s="3">
+    <row r="19" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C19" s="3">
+        <v>2</v>
+      </c>
+      <c r="D19" s="38">
         <v>16</v>
       </c>
       <c r="E19" s="4" t="s">
@@ -1563,7 +1753,7 @@
       </c>
       <c r="F19" s="6">
         <f t="shared" si="0"/>
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="G19" s="10">
         <v>1</v>
@@ -1574,7 +1764,9 @@
       <c r="I19" s="10">
         <v>1</v>
       </c>
-      <c r="J19" s="10"/>
+      <c r="J19" s="10">
+        <v>1</v>
+      </c>
       <c r="K19" s="10"/>
       <c r="L19" s="10"/>
       <c r="M19" s="10"/>
@@ -1588,8 +1780,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D20" s="3">
+    <row r="20" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C20" s="41">
+        <v>1</v>
+      </c>
+      <c r="D20" s="38">
         <v>17</v>
       </c>
       <c r="E20" s="4" t="s">
@@ -1608,7 +1803,9 @@
       <c r="I20" s="10">
         <v>0</v>
       </c>
-      <c r="J20" s="10"/>
+      <c r="J20" s="10">
+        <v>0</v>
+      </c>
       <c r="K20" s="10"/>
       <c r="L20" s="10"/>
       <c r="M20" s="10"/>
@@ -1622,8 +1819,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D21" s="3">
+    <row r="21" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C21" s="3">
+        <v>2</v>
+      </c>
+      <c r="D21" s="38">
         <v>18</v>
       </c>
       <c r="E21" s="4" t="s">
@@ -1631,7 +1831,7 @@
       </c>
       <c r="F21" s="6">
         <f t="shared" si="0"/>
-        <v>19.25</v>
+        <v>26.25</v>
       </c>
       <c r="G21" s="10">
         <v>1</v>
@@ -1642,7 +1842,9 @@
       <c r="I21" s="10">
         <v>0.75</v>
       </c>
-      <c r="J21" s="10"/>
+      <c r="J21" s="10">
+        <v>1</v>
+      </c>
       <c r="K21" s="10"/>
       <c r="L21" s="10"/>
       <c r="M21" s="10"/>
@@ -1656,8 +1858,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D22" s="3">
+    <row r="22" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C22" s="3">
+        <v>1</v>
+      </c>
+      <c r="D22" s="38">
         <v>19</v>
       </c>
       <c r="E22" s="4" t="s">
@@ -1665,7 +1870,7 @@
       </c>
       <c r="F22" s="6">
         <f t="shared" si="0"/>
-        <v>19.25</v>
+        <v>26.25</v>
       </c>
       <c r="G22" s="10">
         <v>1</v>
@@ -1676,7 +1881,9 @@
       <c r="I22" s="10">
         <v>0.75</v>
       </c>
-      <c r="J22" s="10"/>
+      <c r="J22" s="10">
+        <v>1</v>
+      </c>
       <c r="K22" s="10"/>
       <c r="L22" s="10"/>
       <c r="M22" s="10"/>
@@ -1690,8 +1897,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D23" s="3">
+    <row r="23" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C23" s="41">
+        <v>2</v>
+      </c>
+      <c r="D23" s="38">
         <v>20</v>
       </c>
       <c r="E23" s="4" t="s">
@@ -1710,7 +1920,9 @@
       <c r="I23" s="10">
         <v>0</v>
       </c>
-      <c r="J23" s="10"/>
+      <c r="J23" s="10">
+        <v>0</v>
+      </c>
       <c r="K23" s="10"/>
       <c r="L23" s="10"/>
       <c r="M23" s="10"/>
@@ -1724,8 +1936,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D24" s="3">
+    <row r="24" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C24" s="3">
+        <v>1</v>
+      </c>
+      <c r="D24" s="38">
         <v>21</v>
       </c>
       <c r="E24" s="4" t="s">
@@ -1733,7 +1948,7 @@
       </c>
       <c r="F24" s="6">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>24.5</v>
       </c>
       <c r="G24" s="10">
         <v>1</v>
@@ -1741,8 +1956,12 @@
       <c r="H24" s="10">
         <v>1</v>
       </c>
-      <c r="I24" s="10"/>
-      <c r="J24" s="10"/>
+      <c r="I24" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="J24" s="10">
+        <v>1</v>
+      </c>
       <c r="K24" s="10"/>
       <c r="L24" s="10"/>
       <c r="M24" s="10"/>
@@ -1756,8 +1975,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D25" s="3">
+    <row r="25" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C25" s="3">
+        <v>2</v>
+      </c>
+      <c r="D25" s="38">
         <v>22</v>
       </c>
       <c r="E25" s="4" t="s">
@@ -1765,7 +1987,7 @@
       </c>
       <c r="F25" s="6">
         <f t="shared" si="0"/>
-        <v>19.25</v>
+        <v>26.25</v>
       </c>
       <c r="G25" s="10">
         <v>1</v>
@@ -1776,7 +1998,9 @@
       <c r="I25" s="10">
         <v>0.75</v>
       </c>
-      <c r="J25" s="10"/>
+      <c r="J25" s="10">
+        <v>1</v>
+      </c>
       <c r="K25" s="10"/>
       <c r="L25" s="10"/>
       <c r="M25" s="10"/>
@@ -1790,8 +2014,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D26" s="3">
+    <row r="26" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C26" s="3">
+        <v>1</v>
+      </c>
+      <c r="D26" s="38">
         <v>23</v>
       </c>
       <c r="E26" s="4" t="s">
@@ -1799,7 +2026,7 @@
       </c>
       <c r="F26" s="6">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>24.5</v>
       </c>
       <c r="G26" s="10">
         <v>1</v>
@@ -1807,8 +2034,12 @@
       <c r="H26" s="10">
         <v>1</v>
       </c>
-      <c r="I26" s="10"/>
-      <c r="J26" s="10"/>
+      <c r="I26" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="J26" s="10">
+        <v>1</v>
+      </c>
       <c r="K26" s="10"/>
       <c r="L26" s="10"/>
       <c r="M26" s="10"/>
@@ -1822,8 +2053,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D27" s="3">
+    <row r="27" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C27" s="3">
+        <v>2</v>
+      </c>
+      <c r="D27" s="38">
         <v>24</v>
       </c>
       <c r="E27" s="4" t="s">
@@ -1831,7 +2065,7 @@
       </c>
       <c r="F27" s="6">
         <f t="shared" si="0"/>
-        <v>19.25</v>
+        <v>26.25</v>
       </c>
       <c r="G27" s="10">
         <v>1</v>
@@ -1842,7 +2076,9 @@
       <c r="I27" s="10">
         <v>0.75</v>
       </c>
-      <c r="J27" s="10"/>
+      <c r="J27" s="10">
+        <v>1</v>
+      </c>
       <c r="K27" s="10"/>
       <c r="L27" s="10"/>
       <c r="M27" s="10"/>
@@ -1856,16 +2092,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D28" s="3">
+    <row r="28" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C28" s="3">
+        <v>1</v>
+      </c>
+      <c r="D28" s="38">
         <v>25</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F28" s="6">
         <f t="shared" si="0"/>
-        <v>19.25</v>
+        <v>26.25</v>
       </c>
       <c r="G28" s="10">
         <v>1</v>
@@ -1876,7 +2115,9 @@
       <c r="I28" s="10">
         <v>0.75</v>
       </c>
-      <c r="J28" s="10"/>
+      <c r="J28" s="10">
+        <v>1</v>
+      </c>
       <c r="K28" s="10"/>
       <c r="L28" s="10"/>
       <c r="M28" s="10"/>
@@ -1890,8 +2131,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D29" s="3">
+    <row r="29" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C29" s="3">
+        <v>2</v>
+      </c>
+      <c r="D29" s="38">
         <v>26</v>
       </c>
       <c r="E29" s="4" t="s">
@@ -1899,7 +2143,7 @@
       </c>
       <c r="F29" s="6">
         <f t="shared" si="0"/>
-        <v>19.25</v>
+        <v>26.25</v>
       </c>
       <c r="G29" s="11">
         <v>1</v>
@@ -1910,7 +2154,9 @@
       <c r="I29" s="10">
         <v>0.75</v>
       </c>
-      <c r="J29" s="10"/>
+      <c r="J29" s="10">
+        <v>1</v>
+      </c>
       <c r="K29" s="10"/>
       <c r="L29" s="10"/>
       <c r="M29" s="10"/>
@@ -1924,8 +2170,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D30" s="3">
+    <row r="30" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C30" s="3">
+        <v>1</v>
+      </c>
+      <c r="D30" s="38">
         <v>27</v>
       </c>
       <c r="E30" s="4" t="s">
@@ -1933,7 +2182,7 @@
       </c>
       <c r="F30" s="6">
         <f t="shared" si="0"/>
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="G30" s="10">
         <v>1</v>
@@ -1944,7 +2193,9 @@
       <c r="I30" s="10">
         <v>1</v>
       </c>
-      <c r="J30" s="10"/>
+      <c r="J30" s="10">
+        <v>1</v>
+      </c>
       <c r="K30" s="10"/>
       <c r="L30" s="10"/>
       <c r="M30" s="10"/>
@@ -1958,8 +2209,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D31" s="3">
+    <row r="31" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C31" s="3">
+        <v>2</v>
+      </c>
+      <c r="D31" s="38">
         <v>28</v>
       </c>
       <c r="E31" s="4" t="s">
@@ -1967,7 +2221,7 @@
       </c>
       <c r="F31" s="6">
         <f t="shared" si="0"/>
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="G31" s="10">
         <v>1</v>
@@ -1978,7 +2232,9 @@
       <c r="I31" s="10">
         <v>1</v>
       </c>
-      <c r="J31" s="10"/>
+      <c r="J31" s="10">
+        <v>1</v>
+      </c>
       <c r="K31" s="10"/>
       <c r="L31" s="10"/>
       <c r="M31" s="10"/>
@@ -1992,8 +2248,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D32" s="3">
+    <row r="32" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C32" s="3">
+        <v>1</v>
+      </c>
+      <c r="D32" s="38">
         <v>29</v>
       </c>
       <c r="E32" s="4" t="s">
@@ -2001,7 +2260,7 @@
       </c>
       <c r="F32" s="6">
         <f t="shared" si="0"/>
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="G32" s="10">
         <v>1</v>
@@ -2012,7 +2271,9 @@
       <c r="I32" s="10">
         <v>1</v>
       </c>
-      <c r="J32" s="10"/>
+      <c r="J32" s="10">
+        <v>1</v>
+      </c>
       <c r="K32" s="10"/>
       <c r="L32" s="10"/>
       <c r="M32" s="10"/>
@@ -2026,8 +2287,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D33" s="3">
+    <row r="33" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C33" s="3">
+        <v>2</v>
+      </c>
+      <c r="D33" s="38">
         <v>30</v>
       </c>
       <c r="E33" s="4" t="s">
@@ -2035,7 +2299,7 @@
       </c>
       <c r="F33" s="6">
         <f t="shared" si="0"/>
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="G33" s="10">
         <v>1</v>
@@ -2046,7 +2310,9 @@
       <c r="I33" s="10">
         <v>1</v>
       </c>
-      <c r="J33" s="10"/>
+      <c r="J33" s="10">
+        <v>1</v>
+      </c>
       <c r="K33" s="10"/>
       <c r="L33" s="10"/>
       <c r="M33" s="10"/>
@@ -2060,8 +2326,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D34" s="3">
+    <row r="34" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C34" s="3">
+        <v>1</v>
+      </c>
+      <c r="D34" s="38">
         <v>31</v>
       </c>
       <c r="E34" s="4" t="s">
@@ -2069,7 +2338,7 @@
       </c>
       <c r="F34" s="6">
         <f t="shared" si="0"/>
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="G34" s="10">
         <v>1</v>
@@ -2080,7 +2349,9 @@
       <c r="I34" s="10">
         <v>1</v>
       </c>
-      <c r="J34" s="10"/>
+      <c r="J34" s="10">
+        <v>1</v>
+      </c>
       <c r="K34" s="10"/>
       <c r="L34" s="10"/>
       <c r="M34" s="10"/>
@@ -2094,8 +2365,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D35" s="3">
+    <row r="35" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C35" s="3">
+        <v>2</v>
+      </c>
+      <c r="D35" s="38">
         <v>32</v>
       </c>
       <c r="E35" s="4" t="s">
@@ -2103,7 +2377,7 @@
       </c>
       <c r="F35" s="6">
         <f t="shared" si="0"/>
-        <v>19.25</v>
+        <v>26.25</v>
       </c>
       <c r="G35" s="10">
         <v>1</v>
@@ -2114,7 +2388,9 @@
       <c r="I35" s="10">
         <v>0.75</v>
       </c>
-      <c r="J35" s="10"/>
+      <c r="J35" s="10">
+        <v>1</v>
+      </c>
       <c r="K35" s="10"/>
       <c r="L35" s="10"/>
       <c r="M35" s="10"/>
@@ -2128,8 +2404,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D36" s="3">
+    <row r="36" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C36" s="3">
+        <v>1</v>
+      </c>
+      <c r="D36" s="38">
         <v>33</v>
       </c>
       <c r="E36" s="4" t="s">
@@ -2137,7 +2416,7 @@
       </c>
       <c r="F36" s="6">
         <f t="shared" si="0"/>
-        <v>19.25</v>
+        <v>26.25</v>
       </c>
       <c r="G36" s="10">
         <v>1</v>
@@ -2148,7 +2427,9 @@
       <c r="I36" s="10">
         <v>0.75</v>
       </c>
-      <c r="J36" s="10"/>
+      <c r="J36" s="10">
+        <v>1</v>
+      </c>
       <c r="K36" s="10"/>
       <c r="L36" s="10"/>
       <c r="M36" s="10"/>
@@ -2162,8 +2443,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D37" s="3">
+    <row r="37" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C37" s="3">
+        <v>2</v>
+      </c>
+      <c r="D37" s="38">
         <v>34</v>
       </c>
       <c r="E37" s="4" t="s">
@@ -2171,7 +2455,7 @@
       </c>
       <c r="F37" s="6">
         <f t="shared" si="0"/>
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="G37" s="10">
         <v>1</v>
@@ -2182,7 +2466,9 @@
       <c r="I37" s="10">
         <v>1</v>
       </c>
-      <c r="J37" s="10"/>
+      <c r="J37" s="10">
+        <v>1</v>
+      </c>
       <c r="K37" s="10"/>
       <c r="L37" s="10"/>
       <c r="M37" s="10"/>
@@ -2196,8 +2482,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="4:18" x14ac:dyDescent="0.25">
-      <c r="D38" s="3">
+    <row r="38" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="C38" s="41">
+        <v>1</v>
+      </c>
+      <c r="D38" s="38">
         <v>35</v>
       </c>
       <c r="E38" s="4" t="s">
@@ -2216,7 +2505,9 @@
       <c r="I38" s="10">
         <v>0</v>
       </c>
-      <c r="J38" s="10"/>
+      <c r="J38" s="10">
+        <v>0</v>
+      </c>
       <c r="K38" s="10"/>
       <c r="L38" s="10"/>
       <c r="M38" s="10"/>
@@ -2234,7 +2525,8 @@
       <c r="G1048576" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="10">
+    <mergeCell ref="C1:C3"/>
     <mergeCell ref="D1:D3"/>
     <mergeCell ref="E1:E3"/>
     <mergeCell ref="Q1:Q3"/>
@@ -2288,18 +2580,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD728A97-A86D-4319-B892-289BC7014D66}">
-  <dimension ref="F2:Q30"/>
+  <dimension ref="E2:X30"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10:Q28"/>
+    <sheetView topLeftCell="E1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="S29" sqref="S29:U30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="8" max="8" width="21.7109375" customWidth="1"/>
+    <col min="23" max="24" width="30.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="6:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="5:24" x14ac:dyDescent="0.25">
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
@@ -2313,410 +2606,617 @@
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
     </row>
-    <row r="3" spans="6:17" x14ac:dyDescent="0.25">
-      <c r="F3" s="34" t="s">
+    <row r="3" spans="5:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E3" s="42">
+        <v>1</v>
+      </c>
+      <c r="F3" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
+      <c r="K3" s="32"/>
+      <c r="L3" s="32"/>
+      <c r="M3" s="32"/>
+      <c r="N3" s="32"/>
+      <c r="O3" s="32"/>
+      <c r="P3" s="32"/>
+      <c r="Q3" s="32"/>
+      <c r="S3" s="42" t="s">
+        <v>58</v>
+      </c>
+      <c r="T3" s="42"/>
+      <c r="U3" s="42"/>
+      <c r="W3" s="44" t="s">
+        <v>60</v>
+      </c>
+      <c r="X3" s="44"/>
+    </row>
+    <row r="4" spans="5:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E4" s="42"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="32"/>
+      <c r="I4" s="32"/>
+      <c r="J4" s="32"/>
+      <c r="K4" s="32"/>
+      <c r="L4" s="32"/>
+      <c r="M4" s="32"/>
+      <c r="N4" s="32"/>
+      <c r="O4" s="32"/>
+      <c r="P4" s="32"/>
+      <c r="Q4" s="32"/>
+      <c r="S4" s="42"/>
+      <c r="T4" s="42"/>
+      <c r="U4" s="42"/>
+      <c r="W4" s="44"/>
+      <c r="X4" s="44"/>
+    </row>
+    <row r="5" spans="5:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E5" s="42"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="32"/>
+      <c r="H5" s="32"/>
+      <c r="I5" s="32"/>
+      <c r="J5" s="32"/>
+      <c r="K5" s="32"/>
+      <c r="L5" s="32"/>
+      <c r="M5" s="32"/>
+      <c r="N5" s="32"/>
+      <c r="O5" s="32"/>
+      <c r="P5" s="32"/>
+      <c r="Q5" s="32"/>
+      <c r="S5" s="42"/>
+      <c r="T5" s="42"/>
+      <c r="U5" s="42"/>
+      <c r="W5" s="44"/>
+      <c r="X5" s="44"/>
+    </row>
+    <row r="6" spans="5:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E6" s="42"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="32"/>
+      <c r="H6" s="32"/>
+      <c r="I6" s="32"/>
+      <c r="J6" s="32"/>
+      <c r="K6" s="32"/>
+      <c r="L6" s="32"/>
+      <c r="M6" s="32"/>
+      <c r="N6" s="32"/>
+      <c r="O6" s="32"/>
+      <c r="P6" s="32"/>
+      <c r="Q6" s="32"/>
+      <c r="S6" s="42"/>
+      <c r="T6" s="42"/>
+      <c r="U6" s="42"/>
+      <c r="W6" s="44"/>
+      <c r="X6" s="44"/>
+    </row>
+    <row r="7" spans="5:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E7" s="42"/>
+      <c r="F7" s="32"/>
+      <c r="G7" s="32"/>
+      <c r="H7" s="32"/>
+      <c r="I7" s="32"/>
+      <c r="J7" s="32"/>
+      <c r="K7" s="32"/>
+      <c r="L7" s="32"/>
+      <c r="M7" s="32"/>
+      <c r="N7" s="32"/>
+      <c r="O7" s="32"/>
+      <c r="P7" s="32"/>
+      <c r="Q7" s="32"/>
+      <c r="S7" s="42"/>
+      <c r="T7" s="42"/>
+      <c r="U7" s="42"/>
+      <c r="W7" s="44"/>
+      <c r="X7" s="44"/>
+    </row>
+    <row r="8" spans="5:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E8" s="42">
+        <v>2</v>
+      </c>
+      <c r="F8" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="G8" s="32"/>
+      <c r="H8" s="32"/>
+      <c r="I8" s="32"/>
+      <c r="J8" s="32"/>
+      <c r="K8" s="32"/>
+      <c r="L8" s="32"/>
+      <c r="M8" s="32"/>
+      <c r="N8" s="32"/>
+      <c r="O8" s="32"/>
+      <c r="P8" s="32"/>
+      <c r="Q8" s="32"/>
+      <c r="S8" s="42" t="s">
+        <v>58</v>
+      </c>
+      <c r="T8" s="42"/>
+      <c r="U8" s="42"/>
+      <c r="W8" s="44" t="s">
+        <v>61</v>
+      </c>
+      <c r="X8" s="44"/>
+    </row>
+    <row r="9" spans="5:24" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E9" s="42"/>
+      <c r="F9" s="32"/>
+      <c r="G9" s="32"/>
+      <c r="H9" s="32"/>
+      <c r="I9" s="32"/>
+      <c r="J9" s="32"/>
+      <c r="K9" s="32"/>
+      <c r="L9" s="32"/>
+      <c r="M9" s="32"/>
+      <c r="N9" s="32"/>
+      <c r="O9" s="32"/>
+      <c r="P9" s="32"/>
+      <c r="Q9" s="32"/>
+      <c r="S9" s="42"/>
+      <c r="T9" s="42"/>
+      <c r="U9" s="42"/>
+      <c r="W9" s="44"/>
+      <c r="X9" s="44"/>
+    </row>
+    <row r="10" spans="5:24" x14ac:dyDescent="0.25">
+      <c r="E10" s="42">
+        <v>3</v>
+      </c>
+      <c r="F10" s="31" t="s">
         <v>53</v>
       </c>
-      <c r="G3" s="35"/>
-      <c r="H3" s="35"/>
-      <c r="I3" s="35"/>
-      <c r="J3" s="35"/>
-      <c r="K3" s="35"/>
-      <c r="L3" s="35"/>
-      <c r="M3" s="35"/>
-      <c r="N3" s="35"/>
-      <c r="O3" s="35"/>
-      <c r="P3" s="35"/>
-      <c r="Q3" s="35"/>
-    </row>
-    <row r="4" spans="6:17" x14ac:dyDescent="0.25">
-      <c r="F4" s="35"/>
-      <c r="G4" s="35"/>
-      <c r="H4" s="35"/>
-      <c r="I4" s="35"/>
-      <c r="J4" s="35"/>
-      <c r="K4" s="35"/>
-      <c r="L4" s="35"/>
-      <c r="M4" s="35"/>
-      <c r="N4" s="35"/>
-      <c r="O4" s="35"/>
-      <c r="P4" s="35"/>
-      <c r="Q4" s="35"/>
-    </row>
-    <row r="5" spans="6:17" x14ac:dyDescent="0.25">
-      <c r="F5" s="35"/>
-      <c r="G5" s="35"/>
-      <c r="H5" s="35"/>
-      <c r="I5" s="35"/>
-      <c r="J5" s="35"/>
-      <c r="K5" s="35"/>
-      <c r="L5" s="35"/>
-      <c r="M5" s="35"/>
-      <c r="N5" s="35"/>
-      <c r="O5" s="35"/>
-      <c r="P5" s="35"/>
-      <c r="Q5" s="35"/>
-    </row>
-    <row r="6" spans="6:17" x14ac:dyDescent="0.25">
-      <c r="F6" s="35"/>
-      <c r="G6" s="35"/>
-      <c r="H6" s="35"/>
-      <c r="I6" s="35"/>
-      <c r="J6" s="35"/>
-      <c r="K6" s="35"/>
-      <c r="L6" s="35"/>
-      <c r="M6" s="35"/>
-      <c r="N6" s="35"/>
-      <c r="O6" s="35"/>
-      <c r="P6" s="35"/>
-      <c r="Q6" s="35"/>
-    </row>
-    <row r="7" spans="6:17" x14ac:dyDescent="0.25">
-      <c r="F7" s="35"/>
-      <c r="G7" s="35"/>
-      <c r="H7" s="35"/>
-      <c r="I7" s="35"/>
-      <c r="J7" s="35"/>
-      <c r="K7" s="35"/>
-      <c r="L7" s="35"/>
-      <c r="M7" s="35"/>
-      <c r="N7" s="35"/>
-      <c r="O7" s="35"/>
-      <c r="P7" s="35"/>
-      <c r="Q7" s="35"/>
-    </row>
-    <row r="8" spans="6:17" x14ac:dyDescent="0.25">
-      <c r="F8" s="34" t="s">
+      <c r="G10" s="32"/>
+      <c r="H10" s="32"/>
+      <c r="I10" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="J10" s="32"/>
+      <c r="K10" s="32"/>
+      <c r="L10" s="32"/>
+      <c r="M10" s="32"/>
+      <c r="N10" s="32"/>
+      <c r="O10" s="32"/>
+      <c r="P10" s="32"/>
+      <c r="Q10" s="32"/>
+      <c r="S10" s="43" t="s">
+        <v>59</v>
+      </c>
+      <c r="T10" s="42"/>
+      <c r="U10" s="42"/>
+      <c r="W10" s="44" t="s">
+        <v>62</v>
+      </c>
+      <c r="X10" s="44" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="5:24" x14ac:dyDescent="0.25">
+      <c r="E11" s="42"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="32"/>
+      <c r="H11" s="32"/>
+      <c r="I11" s="32"/>
+      <c r="J11" s="32"/>
+      <c r="K11" s="32"/>
+      <c r="L11" s="32"/>
+      <c r="M11" s="32"/>
+      <c r="N11" s="32"/>
+      <c r="O11" s="32"/>
+      <c r="P11" s="32"/>
+      <c r="Q11" s="32"/>
+      <c r="S11" s="42"/>
+      <c r="T11" s="42"/>
+      <c r="U11" s="42"/>
+      <c r="W11" s="44"/>
+      <c r="X11" s="44"/>
+    </row>
+    <row r="12" spans="5:24" x14ac:dyDescent="0.25">
+      <c r="E12" s="42"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="32"/>
+      <c r="H12" s="32"/>
+      <c r="I12" s="32"/>
+      <c r="J12" s="32"/>
+      <c r="K12" s="32"/>
+      <c r="L12" s="32"/>
+      <c r="M12" s="32"/>
+      <c r="N12" s="32"/>
+      <c r="O12" s="32"/>
+      <c r="P12" s="32"/>
+      <c r="Q12" s="32"/>
+      <c r="S12" s="42"/>
+      <c r="T12" s="42"/>
+      <c r="U12" s="42"/>
+      <c r="W12" s="44"/>
+      <c r="X12" s="44"/>
+    </row>
+    <row r="13" spans="5:24" x14ac:dyDescent="0.25">
+      <c r="E13" s="42"/>
+      <c r="F13" s="32"/>
+      <c r="G13" s="32"/>
+      <c r="H13" s="32"/>
+      <c r="I13" s="32"/>
+      <c r="J13" s="32"/>
+      <c r="K13" s="32"/>
+      <c r="L13" s="32"/>
+      <c r="M13" s="32"/>
+      <c r="N13" s="32"/>
+      <c r="O13" s="32"/>
+      <c r="P13" s="32"/>
+      <c r="Q13" s="32"/>
+      <c r="S13" s="42"/>
+      <c r="T13" s="42"/>
+      <c r="U13" s="42"/>
+      <c r="W13" s="44"/>
+      <c r="X13" s="44"/>
+    </row>
+    <row r="14" spans="5:24" x14ac:dyDescent="0.25">
+      <c r="E14" s="42"/>
+      <c r="F14" s="32"/>
+      <c r="G14" s="32"/>
+      <c r="H14" s="32"/>
+      <c r="I14" s="32"/>
+      <c r="J14" s="32"/>
+      <c r="K14" s="32"/>
+      <c r="L14" s="32"/>
+      <c r="M14" s="32"/>
+      <c r="N14" s="32"/>
+      <c r="O14" s="32"/>
+      <c r="P14" s="32"/>
+      <c r="Q14" s="32"/>
+      <c r="S14" s="42"/>
+      <c r="T14" s="42"/>
+      <c r="U14" s="42"/>
+      <c r="W14" s="44"/>
+      <c r="X14" s="44"/>
+    </row>
+    <row r="15" spans="5:24" x14ac:dyDescent="0.25">
+      <c r="E15" s="42"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="32"/>
+      <c r="H15" s="32"/>
+      <c r="I15" s="32"/>
+      <c r="J15" s="32"/>
+      <c r="K15" s="32"/>
+      <c r="L15" s="32"/>
+      <c r="M15" s="32"/>
+      <c r="N15" s="32"/>
+      <c r="O15" s="32"/>
+      <c r="P15" s="32"/>
+      <c r="Q15" s="32"/>
+      <c r="S15" s="42"/>
+      <c r="T15" s="42"/>
+      <c r="U15" s="42"/>
+      <c r="W15" s="44"/>
+      <c r="X15" s="44"/>
+    </row>
+    <row r="16" spans="5:24" x14ac:dyDescent="0.25">
+      <c r="E16" s="42"/>
+      <c r="F16" s="32"/>
+      <c r="G16" s="32"/>
+      <c r="H16" s="32"/>
+      <c r="I16" s="32"/>
+      <c r="J16" s="32"/>
+      <c r="K16" s="32"/>
+      <c r="L16" s="32"/>
+      <c r="M16" s="32"/>
+      <c r="N16" s="32"/>
+      <c r="O16" s="32"/>
+      <c r="P16" s="32"/>
+      <c r="Q16" s="32"/>
+      <c r="S16" s="42"/>
+      <c r="T16" s="42"/>
+      <c r="U16" s="42"/>
+      <c r="W16" s="44"/>
+      <c r="X16" s="44"/>
+    </row>
+    <row r="17" spans="5:24" x14ac:dyDescent="0.25">
+      <c r="E17" s="42"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="32"/>
+      <c r="H17" s="32"/>
+      <c r="I17" s="32"/>
+      <c r="J17" s="32"/>
+      <c r="K17" s="32"/>
+      <c r="L17" s="32"/>
+      <c r="M17" s="32"/>
+      <c r="N17" s="32"/>
+      <c r="O17" s="32"/>
+      <c r="P17" s="32"/>
+      <c r="Q17" s="32"/>
+      <c r="S17" s="42"/>
+      <c r="T17" s="42"/>
+      <c r="U17" s="42"/>
+      <c r="W17" s="44"/>
+      <c r="X17" s="44"/>
+    </row>
+    <row r="18" spans="5:24" x14ac:dyDescent="0.25">
+      <c r="E18" s="42"/>
+      <c r="F18" s="32"/>
+      <c r="G18" s="32"/>
+      <c r="H18" s="32"/>
+      <c r="I18" s="32"/>
+      <c r="J18" s="32"/>
+      <c r="K18" s="32"/>
+      <c r="L18" s="32"/>
+      <c r="M18" s="32"/>
+      <c r="N18" s="32"/>
+      <c r="O18" s="32"/>
+      <c r="P18" s="32"/>
+      <c r="Q18" s="32"/>
+      <c r="S18" s="42"/>
+      <c r="T18" s="42"/>
+      <c r="U18" s="42"/>
+      <c r="W18" s="44"/>
+      <c r="X18" s="44"/>
+    </row>
+    <row r="19" spans="5:24" x14ac:dyDescent="0.25">
+      <c r="E19" s="42"/>
+      <c r="F19" s="32"/>
+      <c r="G19" s="32"/>
+      <c r="H19" s="32"/>
+      <c r="I19" s="32"/>
+      <c r="J19" s="32"/>
+      <c r="K19" s="32"/>
+      <c r="L19" s="32"/>
+      <c r="M19" s="32"/>
+      <c r="N19" s="32"/>
+      <c r="O19" s="32"/>
+      <c r="P19" s="32"/>
+      <c r="Q19" s="32"/>
+      <c r="S19" s="42"/>
+      <c r="T19" s="42"/>
+      <c r="U19" s="42"/>
+      <c r="W19" s="44"/>
+      <c r="X19" s="44"/>
+    </row>
+    <row r="20" spans="5:24" x14ac:dyDescent="0.25">
+      <c r="E20" s="42"/>
+      <c r="F20" s="32"/>
+      <c r="G20" s="32"/>
+      <c r="H20" s="32"/>
+      <c r="I20" s="32"/>
+      <c r="J20" s="32"/>
+      <c r="K20" s="32"/>
+      <c r="L20" s="32"/>
+      <c r="M20" s="32"/>
+      <c r="N20" s="32"/>
+      <c r="O20" s="32"/>
+      <c r="P20" s="32"/>
+      <c r="Q20" s="32"/>
+      <c r="S20" s="42"/>
+      <c r="T20" s="42"/>
+      <c r="U20" s="42"/>
+      <c r="W20" s="44"/>
+      <c r="X20" s="44"/>
+    </row>
+    <row r="21" spans="5:24" x14ac:dyDescent="0.25">
+      <c r="E21" s="42"/>
+      <c r="F21" s="32"/>
+      <c r="G21" s="32"/>
+      <c r="H21" s="32"/>
+      <c r="I21" s="32"/>
+      <c r="J21" s="32"/>
+      <c r="K21" s="32"/>
+      <c r="L21" s="32"/>
+      <c r="M21" s="32"/>
+      <c r="N21" s="32"/>
+      <c r="O21" s="32"/>
+      <c r="P21" s="32"/>
+      <c r="Q21" s="32"/>
+      <c r="S21" s="42"/>
+      <c r="T21" s="42"/>
+      <c r="U21" s="42"/>
+      <c r="W21" s="44"/>
+      <c r="X21" s="44"/>
+    </row>
+    <row r="22" spans="5:24" x14ac:dyDescent="0.25">
+      <c r="E22" s="42"/>
+      <c r="F22" s="32"/>
+      <c r="G22" s="32"/>
+      <c r="H22" s="32"/>
+      <c r="I22" s="32"/>
+      <c r="J22" s="32"/>
+      <c r="K22" s="32"/>
+      <c r="L22" s="32"/>
+      <c r="M22" s="32"/>
+      <c r="N22" s="32"/>
+      <c r="O22" s="32"/>
+      <c r="P22" s="32"/>
+      <c r="Q22" s="32"/>
+      <c r="S22" s="42"/>
+      <c r="T22" s="42"/>
+      <c r="U22" s="42"/>
+      <c r="W22" s="44"/>
+      <c r="X22" s="44"/>
+    </row>
+    <row r="23" spans="5:24" x14ac:dyDescent="0.25">
+      <c r="E23" s="42"/>
+      <c r="F23" s="32"/>
+      <c r="G23" s="32"/>
+      <c r="H23" s="32"/>
+      <c r="I23" s="32"/>
+      <c r="J23" s="32"/>
+      <c r="K23" s="32"/>
+      <c r="L23" s="32"/>
+      <c r="M23" s="32"/>
+      <c r="N23" s="32"/>
+      <c r="O23" s="32"/>
+      <c r="P23" s="32"/>
+      <c r="Q23" s="32"/>
+      <c r="S23" s="42"/>
+      <c r="T23" s="42"/>
+      <c r="U23" s="42"/>
+      <c r="W23" s="44"/>
+      <c r="X23" s="44"/>
+    </row>
+    <row r="24" spans="5:24" x14ac:dyDescent="0.25">
+      <c r="E24" s="42"/>
+      <c r="F24" s="32"/>
+      <c r="G24" s="32"/>
+      <c r="H24" s="32"/>
+      <c r="I24" s="32"/>
+      <c r="J24" s="32"/>
+      <c r="K24" s="32"/>
+      <c r="L24" s="32"/>
+      <c r="M24" s="32"/>
+      <c r="N24" s="32"/>
+      <c r="O24" s="32"/>
+      <c r="P24" s="32"/>
+      <c r="Q24" s="32"/>
+      <c r="S24" s="42"/>
+      <c r="T24" s="42"/>
+      <c r="U24" s="42"/>
+      <c r="W24" s="44"/>
+      <c r="X24" s="44"/>
+    </row>
+    <row r="25" spans="5:24" x14ac:dyDescent="0.25">
+      <c r="E25" s="42"/>
+      <c r="F25" s="32"/>
+      <c r="G25" s="32"/>
+      <c r="H25" s="32"/>
+      <c r="I25" s="32"/>
+      <c r="J25" s="32"/>
+      <c r="K25" s="32"/>
+      <c r="L25" s="32"/>
+      <c r="M25" s="32"/>
+      <c r="N25" s="32"/>
+      <c r="O25" s="32"/>
+      <c r="P25" s="32"/>
+      <c r="Q25" s="32"/>
+      <c r="S25" s="42"/>
+      <c r="T25" s="42"/>
+      <c r="U25" s="42"/>
+      <c r="W25" s="44"/>
+      <c r="X25" s="44"/>
+    </row>
+    <row r="26" spans="5:24" x14ac:dyDescent="0.25">
+      <c r="E26" s="42"/>
+      <c r="F26" s="32"/>
+      <c r="G26" s="32"/>
+      <c r="H26" s="32"/>
+      <c r="I26" s="32"/>
+      <c r="J26" s="32"/>
+      <c r="K26" s="32"/>
+      <c r="L26" s="32"/>
+      <c r="M26" s="32"/>
+      <c r="N26" s="32"/>
+      <c r="O26" s="32"/>
+      <c r="P26" s="32"/>
+      <c r="Q26" s="32"/>
+      <c r="S26" s="42"/>
+      <c r="T26" s="42"/>
+      <c r="U26" s="42"/>
+      <c r="W26" s="44"/>
+      <c r="X26" s="44"/>
+    </row>
+    <row r="27" spans="5:24" x14ac:dyDescent="0.25">
+      <c r="E27" s="42"/>
+      <c r="F27" s="32"/>
+      <c r="G27" s="32"/>
+      <c r="H27" s="32"/>
+      <c r="I27" s="32"/>
+      <c r="J27" s="32"/>
+      <c r="K27" s="32"/>
+      <c r="L27" s="32"/>
+      <c r="M27" s="32"/>
+      <c r="N27" s="32"/>
+      <c r="O27" s="32"/>
+      <c r="P27" s="32"/>
+      <c r="Q27" s="32"/>
+      <c r="S27" s="42"/>
+      <c r="T27" s="42"/>
+      <c r="U27" s="42"/>
+      <c r="W27" s="44"/>
+      <c r="X27" s="44"/>
+    </row>
+    <row r="28" spans="5:24" x14ac:dyDescent="0.25">
+      <c r="E28" s="42"/>
+      <c r="F28" s="32"/>
+      <c r="G28" s="32"/>
+      <c r="H28" s="32"/>
+      <c r="I28" s="32"/>
+      <c r="J28" s="32"/>
+      <c r="K28" s="32"/>
+      <c r="L28" s="32"/>
+      <c r="M28" s="32"/>
+      <c r="N28" s="32"/>
+      <c r="O28" s="32"/>
+      <c r="P28" s="32"/>
+      <c r="Q28" s="32"/>
+      <c r="S28" s="42"/>
+      <c r="T28" s="42"/>
+      <c r="U28" s="42"/>
+      <c r="W28" s="44"/>
+      <c r="X28" s="44"/>
+    </row>
+    <row r="29" spans="5:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E29" s="42">
+        <v>4</v>
+      </c>
+      <c r="F29" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="G8" s="35"/>
-      <c r="H8" s="35"/>
-      <c r="I8" s="35"/>
-      <c r="J8" s="35"/>
-      <c r="K8" s="35"/>
-      <c r="L8" s="35"/>
-      <c r="M8" s="35"/>
-      <c r="N8" s="35"/>
-      <c r="O8" s="35"/>
-      <c r="P8" s="35"/>
-      <c r="Q8" s="35"/>
-    </row>
-    <row r="9" spans="6:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F9" s="35"/>
-      <c r="G9" s="35"/>
-      <c r="H9" s="35"/>
-      <c r="I9" s="35"/>
-      <c r="J9" s="35"/>
-      <c r="K9" s="35"/>
-      <c r="L9" s="35"/>
-      <c r="M9" s="35"/>
-      <c r="N9" s="35"/>
-      <c r="O9" s="35"/>
-      <c r="P9" s="35"/>
-      <c r="Q9" s="35"/>
-    </row>
-    <row r="10" spans="6:17" x14ac:dyDescent="0.25">
-      <c r="F10" s="34" t="s">
-        <v>55</v>
-      </c>
-      <c r="G10" s="35"/>
-      <c r="H10" s="35"/>
-      <c r="I10" s="34" t="s">
-        <v>56</v>
-      </c>
-      <c r="J10" s="35"/>
-      <c r="K10" s="35"/>
-      <c r="L10" s="35"/>
-      <c r="M10" s="35"/>
-      <c r="N10" s="35"/>
-      <c r="O10" s="35"/>
-      <c r="P10" s="35"/>
-      <c r="Q10" s="35"/>
-    </row>
-    <row r="11" spans="6:17" x14ac:dyDescent="0.25">
-      <c r="F11" s="35"/>
-      <c r="G11" s="35"/>
-      <c r="H11" s="35"/>
-      <c r="I11" s="35"/>
-      <c r="J11" s="35"/>
-      <c r="K11" s="35"/>
-      <c r="L11" s="35"/>
-      <c r="M11" s="35"/>
-      <c r="N11" s="35"/>
-      <c r="O11" s="35"/>
-      <c r="P11" s="35"/>
-      <c r="Q11" s="35"/>
-    </row>
-    <row r="12" spans="6:17" x14ac:dyDescent="0.25">
-      <c r="F12" s="35"/>
-      <c r="G12" s="35"/>
-      <c r="H12" s="35"/>
-      <c r="I12" s="35"/>
-      <c r="J12" s="35"/>
-      <c r="K12" s="35"/>
-      <c r="L12" s="35"/>
-      <c r="M12" s="35"/>
-      <c r="N12" s="35"/>
-      <c r="O12" s="35"/>
-      <c r="P12" s="35"/>
-      <c r="Q12" s="35"/>
-    </row>
-    <row r="13" spans="6:17" x14ac:dyDescent="0.25">
-      <c r="F13" s="35"/>
-      <c r="G13" s="35"/>
-      <c r="H13" s="35"/>
-      <c r="I13" s="35"/>
-      <c r="J13" s="35"/>
-      <c r="K13" s="35"/>
-      <c r="L13" s="35"/>
-      <c r="M13" s="35"/>
-      <c r="N13" s="35"/>
-      <c r="O13" s="35"/>
-      <c r="P13" s="35"/>
-      <c r="Q13" s="35"/>
-    </row>
-    <row r="14" spans="6:17" x14ac:dyDescent="0.25">
-      <c r="F14" s="35"/>
-      <c r="G14" s="35"/>
-      <c r="H14" s="35"/>
-      <c r="I14" s="35"/>
-      <c r="J14" s="35"/>
-      <c r="K14" s="35"/>
-      <c r="L14" s="35"/>
-      <c r="M14" s="35"/>
-      <c r="N14" s="35"/>
-      <c r="O14" s="35"/>
-      <c r="P14" s="35"/>
-      <c r="Q14" s="35"/>
-    </row>
-    <row r="15" spans="6:17" x14ac:dyDescent="0.25">
-      <c r="F15" s="35"/>
-      <c r="G15" s="35"/>
-      <c r="H15" s="35"/>
-      <c r="I15" s="35"/>
-      <c r="J15" s="35"/>
-      <c r="K15" s="35"/>
-      <c r="L15" s="35"/>
-      <c r="M15" s="35"/>
-      <c r="N15" s="35"/>
-      <c r="O15" s="35"/>
-      <c r="P15" s="35"/>
-      <c r="Q15" s="35"/>
-    </row>
-    <row r="16" spans="6:17" x14ac:dyDescent="0.25">
-      <c r="F16" s="35"/>
-      <c r="G16" s="35"/>
-      <c r="H16" s="35"/>
-      <c r="I16" s="35"/>
-      <c r="J16" s="35"/>
-      <c r="K16" s="35"/>
-      <c r="L16" s="35"/>
-      <c r="M16" s="35"/>
-      <c r="N16" s="35"/>
-      <c r="O16" s="35"/>
-      <c r="P16" s="35"/>
-      <c r="Q16" s="35"/>
-    </row>
-    <row r="17" spans="6:17" x14ac:dyDescent="0.25">
-      <c r="F17" s="35"/>
-      <c r="G17" s="35"/>
-      <c r="H17" s="35"/>
-      <c r="I17" s="35"/>
-      <c r="J17" s="35"/>
-      <c r="K17" s="35"/>
-      <c r="L17" s="35"/>
-      <c r="M17" s="35"/>
-      <c r="N17" s="35"/>
-      <c r="O17" s="35"/>
-      <c r="P17" s="35"/>
-      <c r="Q17" s="35"/>
-    </row>
-    <row r="18" spans="6:17" x14ac:dyDescent="0.25">
-      <c r="F18" s="35"/>
-      <c r="G18" s="35"/>
-      <c r="H18" s="35"/>
-      <c r="I18" s="35"/>
-      <c r="J18" s="35"/>
-      <c r="K18" s="35"/>
-      <c r="L18" s="35"/>
-      <c r="M18" s="35"/>
-      <c r="N18" s="35"/>
-      <c r="O18" s="35"/>
-      <c r="P18" s="35"/>
-      <c r="Q18" s="35"/>
-    </row>
-    <row r="19" spans="6:17" x14ac:dyDescent="0.25">
-      <c r="F19" s="35"/>
-      <c r="G19" s="35"/>
-      <c r="H19" s="35"/>
-      <c r="I19" s="35"/>
-      <c r="J19" s="35"/>
-      <c r="K19" s="35"/>
-      <c r="L19" s="35"/>
-      <c r="M19" s="35"/>
-      <c r="N19" s="35"/>
-      <c r="O19" s="35"/>
-      <c r="P19" s="35"/>
-      <c r="Q19" s="35"/>
-    </row>
-    <row r="20" spans="6:17" x14ac:dyDescent="0.25">
-      <c r="F20" s="35"/>
-      <c r="G20" s="35"/>
-      <c r="H20" s="35"/>
-      <c r="I20" s="35"/>
-      <c r="J20" s="35"/>
-      <c r="K20" s="35"/>
-      <c r="L20" s="35"/>
-      <c r="M20" s="35"/>
-      <c r="N20" s="35"/>
-      <c r="O20" s="35"/>
-      <c r="P20" s="35"/>
-      <c r="Q20" s="35"/>
-    </row>
-    <row r="21" spans="6:17" x14ac:dyDescent="0.25">
-      <c r="F21" s="35"/>
-      <c r="G21" s="35"/>
-      <c r="H21" s="35"/>
-      <c r="I21" s="35"/>
-      <c r="J21" s="35"/>
-      <c r="K21" s="35"/>
-      <c r="L21" s="35"/>
-      <c r="M21" s="35"/>
-      <c r="N21" s="35"/>
-      <c r="O21" s="35"/>
-      <c r="P21" s="35"/>
-      <c r="Q21" s="35"/>
-    </row>
-    <row r="22" spans="6:17" x14ac:dyDescent="0.25">
-      <c r="F22" s="35"/>
-      <c r="G22" s="35"/>
-      <c r="H22" s="35"/>
-      <c r="I22" s="35"/>
-      <c r="J22" s="35"/>
-      <c r="K22" s="35"/>
-      <c r="L22" s="35"/>
-      <c r="M22" s="35"/>
-      <c r="N22" s="35"/>
-      <c r="O22" s="35"/>
-      <c r="P22" s="35"/>
-      <c r="Q22" s="35"/>
-    </row>
-    <row r="23" spans="6:17" x14ac:dyDescent="0.25">
-      <c r="F23" s="35"/>
-      <c r="G23" s="35"/>
-      <c r="H23" s="35"/>
-      <c r="I23" s="35"/>
-      <c r="J23" s="35"/>
-      <c r="K23" s="35"/>
-      <c r="L23" s="35"/>
-      <c r="M23" s="35"/>
-      <c r="N23" s="35"/>
-      <c r="O23" s="35"/>
-      <c r="P23" s="35"/>
-      <c r="Q23" s="35"/>
-    </row>
-    <row r="24" spans="6:17" x14ac:dyDescent="0.25">
-      <c r="F24" s="35"/>
-      <c r="G24" s="35"/>
-      <c r="H24" s="35"/>
-      <c r="I24" s="35"/>
-      <c r="J24" s="35"/>
-      <c r="K24" s="35"/>
-      <c r="L24" s="35"/>
-      <c r="M24" s="35"/>
-      <c r="N24" s="35"/>
-      <c r="O24" s="35"/>
-      <c r="P24" s="35"/>
-      <c r="Q24" s="35"/>
-    </row>
-    <row r="25" spans="6:17" x14ac:dyDescent="0.25">
-      <c r="F25" s="35"/>
-      <c r="G25" s="35"/>
-      <c r="H25" s="35"/>
-      <c r="I25" s="35"/>
-      <c r="J25" s="35"/>
-      <c r="K25" s="35"/>
-      <c r="L25" s="35"/>
-      <c r="M25" s="35"/>
-      <c r="N25" s="35"/>
-      <c r="O25" s="35"/>
-      <c r="P25" s="35"/>
-      <c r="Q25" s="35"/>
-    </row>
-    <row r="26" spans="6:17" x14ac:dyDescent="0.25">
-      <c r="F26" s="35"/>
-      <c r="G26" s="35"/>
-      <c r="H26" s="35"/>
-      <c r="I26" s="35"/>
-      <c r="J26" s="35"/>
-      <c r="K26" s="35"/>
-      <c r="L26" s="35"/>
-      <c r="M26" s="35"/>
-      <c r="N26" s="35"/>
-      <c r="O26" s="35"/>
-      <c r="P26" s="35"/>
-      <c r="Q26" s="35"/>
-    </row>
-    <row r="27" spans="6:17" x14ac:dyDescent="0.25">
-      <c r="F27" s="35"/>
-      <c r="G27" s="35"/>
-      <c r="H27" s="35"/>
-      <c r="I27" s="35"/>
-      <c r="J27" s="35"/>
-      <c r="K27" s="35"/>
-      <c r="L27" s="35"/>
-      <c r="M27" s="35"/>
-      <c r="N27" s="35"/>
-      <c r="O27" s="35"/>
-      <c r="P27" s="35"/>
-      <c r="Q27" s="35"/>
-    </row>
-    <row r="28" spans="6:17" x14ac:dyDescent="0.25">
-      <c r="F28" s="35"/>
-      <c r="G28" s="35"/>
-      <c r="H28" s="35"/>
-      <c r="I28" s="35"/>
-      <c r="J28" s="35"/>
-      <c r="K28" s="35"/>
-      <c r="L28" s="35"/>
-      <c r="M28" s="35"/>
-      <c r="N28" s="35"/>
-      <c r="O28" s="35"/>
-      <c r="P28" s="35"/>
-      <c r="Q28" s="35"/>
-    </row>
-    <row r="29" spans="6:17" x14ac:dyDescent="0.25">
-      <c r="F29" s="34" t="s">
-        <v>57</v>
-      </c>
-      <c r="G29" s="35"/>
-      <c r="H29" s="35"/>
-      <c r="I29" s="35"/>
-      <c r="J29" s="35"/>
-      <c r="K29" s="35"/>
-      <c r="L29" s="35"/>
-      <c r="M29" s="35"/>
-      <c r="N29" s="35"/>
-      <c r="O29" s="35"/>
-      <c r="P29" s="35"/>
-      <c r="Q29" s="35"/>
-    </row>
-    <row r="30" spans="6:17" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F30" s="35"/>
-      <c r="G30" s="35"/>
-      <c r="H30" s="35"/>
-      <c r="I30" s="35"/>
-      <c r="J30" s="35"/>
-      <c r="K30" s="35"/>
-      <c r="L30" s="35"/>
-      <c r="M30" s="35"/>
-      <c r="N30" s="35"/>
-      <c r="O30" s="35"/>
-      <c r="P30" s="35"/>
-      <c r="Q30" s="35"/>
+      <c r="G29" s="32"/>
+      <c r="H29" s="32"/>
+      <c r="I29" s="32"/>
+      <c r="J29" s="32"/>
+      <c r="K29" s="32"/>
+      <c r="L29" s="32"/>
+      <c r="M29" s="32"/>
+      <c r="N29" s="32"/>
+      <c r="O29" s="32"/>
+      <c r="P29" s="32"/>
+      <c r="Q29" s="32"/>
+      <c r="S29" s="42" t="s">
+        <v>58</v>
+      </c>
+      <c r="T29" s="42"/>
+      <c r="U29" s="42"/>
+      <c r="W29" s="44" t="s">
+        <v>65</v>
+      </c>
+      <c r="X29" s="44"/>
+    </row>
+    <row r="30" spans="5:24" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E30" s="42"/>
+      <c r="F30" s="32"/>
+      <c r="G30" s="32"/>
+      <c r="H30" s="32"/>
+      <c r="I30" s="32"/>
+      <c r="J30" s="32"/>
+      <c r="K30" s="32"/>
+      <c r="L30" s="32"/>
+      <c r="M30" s="32"/>
+      <c r="N30" s="32"/>
+      <c r="O30" s="32"/>
+      <c r="P30" s="32"/>
+      <c r="Q30" s="32"/>
+      <c r="S30" s="42"/>
+      <c r="T30" s="42"/>
+      <c r="U30" s="42"/>
+      <c r="W30" s="44"/>
+      <c r="X30" s="44"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="18">
+    <mergeCell ref="W3:X7"/>
+    <mergeCell ref="W8:X9"/>
+    <mergeCell ref="W29:X30"/>
+    <mergeCell ref="W10:W28"/>
+    <mergeCell ref="X10:X28"/>
+    <mergeCell ref="S3:U7"/>
+    <mergeCell ref="S8:U9"/>
+    <mergeCell ref="S10:U28"/>
+    <mergeCell ref="S29:U30"/>
+    <mergeCell ref="E3:E7"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="E10:E28"/>
+    <mergeCell ref="E29:E30"/>
     <mergeCell ref="F3:Q7"/>
     <mergeCell ref="F8:Q9"/>
     <mergeCell ref="F10:H28"/>

</xml_diff>

<commit_message>
update nilai ulangan fix xii rpl 2
</commit_message>
<xml_diff>
--- a/XIIRPL2(❁´◡`❁)(❁´◡`❁)(❁´◡`❁)(u‿ฺu✿ฺ)/DATA PRAKTIK XII RPl 2.xlsx
+++ b/XIIRPL2(❁´◡`❁)(❁´◡`❁)(❁´◡`❁)(u‿ฺu✿ฺ)/DATA PRAKTIK XII RPl 2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AdeSetiyawan)(✿◡‿◡)(✿◡‿◡)\XIIRPL2(❁´◡`❁)(❁´◡`❁)(❁´◡`❁)(u‿ฺu✿ฺ)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA3EF9C2-99B7-45AC-8347-236DA37AD797}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02664C57-29FE-4E32-876B-D4E15C7CFC1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="375" yWindow="1395" windowWidth="21600" windowHeight="11295" xr2:uid="{7A470BEC-FF9B-4C58-B3A9-6A89F2B6EB46}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7A470BEC-FF9B-4C58-B3A9-6A89F2B6EB46}"/>
   </bookViews>
   <sheets>
     <sheet name="Nilai All" sheetId="1" r:id="rId1"/>
@@ -256,30 +256,12 @@
     <t>:</t>
   </si>
   <si>
-    <t>drive selain C</t>
-  </si>
-  <si>
-    <t>ulangan_1001_nama_absen</t>
-  </si>
-  <si>
     <t>Folder Utama:</t>
   </si>
   <si>
     <t xml:space="preserve">Nama project: </t>
   </si>
   <si>
-    <t>nama_absen_1001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Profil Perusahaan </t>
-  </si>
-  <si>
-    <t>Download</t>
-  </si>
-  <si>
-    <t>Kontak kami</t>
-  </si>
-  <si>
     <t>harus ada 1 (h1)</t>
   </si>
   <si>
@@ -296,6 +278,24 @@
   </si>
   <si>
     <t>Pengurangan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bebas mau dimana saja </t>
+  </si>
+  <si>
+    <t>ulangan_1002_nama_absen</t>
+  </si>
+  <si>
+    <t>nama_absen_1002</t>
+  </si>
+  <si>
+    <t>Biodata Siswa</t>
+  </si>
+  <si>
+    <t>Galeri Foto dan Video</t>
+  </si>
+  <si>
+    <t>Chat Dengan Kami</t>
   </si>
 </sst>
 </file>
@@ -356,7 +356,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -393,6 +393,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="21">
     <border>
@@ -650,7 +656,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -715,6 +721,17 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -766,8 +783,8 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -781,20 +798,21 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1113,8 +1131,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E8966E4-2275-4E9F-82CA-974F40DBA593}">
   <dimension ref="B1:T1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
+      <selection activeCell="E2" sqref="E2"/>
+      <selection pane="topRight" activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1129,54 +1149,56 @@
     <col min="11" max="16" width="12.7109375" customWidth="1"/>
     <col min="17" max="17" width="19" customWidth="1"/>
     <col min="18" max="18" width="13.140625" customWidth="1"/>
+    <col min="19" max="19" width="9.140625" style="2"/>
+    <col min="20" max="20" width="12.5703125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="D1" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="28" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" s="28" t="s">
+      <c r="D1" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="38" t="s">
+      <c r="G1" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="40" t="s">
+      <c r="H1" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="40"/>
-      <c r="J1" s="40"/>
-      <c r="K1" s="36" t="s">
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
+      <c r="K1" s="41" t="s">
         <v>49</v>
       </c>
-      <c r="L1" s="37"/>
-      <c r="M1" s="37"/>
-      <c r="N1" s="37"/>
-      <c r="O1" s="37"/>
-      <c r="P1" s="37"/>
-      <c r="Q1" s="31" t="s">
+      <c r="L1" s="42"/>
+      <c r="M1" s="42"/>
+      <c r="N1" s="42"/>
+      <c r="O1" s="42"/>
+      <c r="P1" s="42"/>
+      <c r="Q1" s="36" t="s">
         <v>66</v>
       </c>
-      <c r="R1" s="31" t="s">
+      <c r="R1" s="36" t="s">
         <v>67</v>
       </c>
-      <c r="S1" s="52" t="s">
-        <v>84</v>
-      </c>
-      <c r="T1" s="53"/>
+      <c r="S1" s="27" t="s">
+        <v>78</v>
+      </c>
+      <c r="T1" s="28"/>
     </row>
     <row r="2" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="C2" s="24"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="39"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="44"/>
       <c r="H2" s="15" t="s">
         <v>10</v>
       </c>
@@ -1204,37 +1226,37 @@
       <c r="P2" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="Q2" s="32"/>
-      <c r="R2" s="31"/>
-      <c r="S2" s="52"/>
-      <c r="T2" s="53"/>
+      <c r="Q2" s="37"/>
+      <c r="R2" s="36"/>
+      <c r="S2" s="27"/>
+      <c r="T2" s="28"/>
     </row>
     <row r="3" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="24"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
       <c r="G3" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="H3" s="33" t="s">
+      <c r="H3" s="38" t="s">
         <v>47</v>
       </c>
-      <c r="I3" s="34"/>
-      <c r="J3" s="35"/>
+      <c r="I3" s="39"/>
+      <c r="J3" s="40"/>
       <c r="K3" s="8"/>
       <c r="L3" s="8"/>
       <c r="M3" s="8"/>
       <c r="N3" s="8"/>
       <c r="O3" s="8"/>
       <c r="P3" s="13"/>
-      <c r="Q3" s="32"/>
-      <c r="R3" s="31"/>
-      <c r="S3" s="50" t="s">
-        <v>85</v>
-      </c>
-      <c r="T3" s="51" t="s">
-        <v>86</v>
+      <c r="Q3" s="37"/>
+      <c r="R3" s="36"/>
+      <c r="S3" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="2:20" x14ac:dyDescent="0.25">
@@ -1279,10 +1301,10 @@
       <c r="R4" s="5">
         <v>0</v>
       </c>
-      <c r="S4">
+      <c r="S4" s="52">
         <v>60</v>
       </c>
-      <c r="T4">
+      <c r="T4" s="2">
         <v>5</v>
       </c>
     </row>
@@ -1293,12 +1315,12 @@
       <c r="D5" s="20">
         <v>2</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="56" t="s">
         <v>18</v>
       </c>
       <c r="F5" s="6">
         <f t="shared" si="0"/>
-        <v>26.25</v>
+        <v>41.25</v>
       </c>
       <c r="G5" s="10">
         <v>1</v>
@@ -1318,11 +1340,17 @@
       <c r="N5" s="10"/>
       <c r="O5" s="10"/>
       <c r="P5" s="14"/>
-      <c r="Q5" s="5">
+      <c r="Q5" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="R5" s="5">
+        <v>0</v>
+      </c>
+      <c r="S5" s="52">
+        <v>100</v>
+      </c>
+      <c r="T5" s="2">
         <v>0</v>
       </c>
     </row>
@@ -1338,7 +1366,7 @@
       </c>
       <c r="F6" s="6">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>24.5</v>
       </c>
       <c r="G6" s="10">
         <v>1</v>
@@ -1347,10 +1375,10 @@
         <v>1</v>
       </c>
       <c r="I6" s="10">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="J6" s="10">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="K6" s="10"/>
       <c r="L6" s="10"/>
@@ -1365,6 +1393,12 @@
       <c r="R6" s="5">
         <v>0</v>
       </c>
+      <c r="S6" s="2">
+        <v>0</v>
+      </c>
+      <c r="T6" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="2:20" x14ac:dyDescent="0.25">
       <c r="C7" s="3">
@@ -1373,12 +1407,12 @@
       <c r="D7" s="20">
         <v>4</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="56" t="s">
         <v>17</v>
       </c>
       <c r="F7" s="6">
         <f t="shared" si="0"/>
-        <v>26.25</v>
+        <v>41.25</v>
       </c>
       <c r="G7" s="10">
         <v>1</v>
@@ -1398,11 +1432,17 @@
       <c r="N7" s="10"/>
       <c r="O7" s="10"/>
       <c r="P7" s="14"/>
-      <c r="Q7" s="5">
+      <c r="Q7" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="R7" s="5">
+        <v>0</v>
+      </c>
+      <c r="S7" s="52">
+        <v>100</v>
+      </c>
+      <c r="T7" s="2">
         <v>0</v>
       </c>
     </row>
@@ -1435,24 +1475,12 @@
       <c r="J8" s="10">
         <v>1</v>
       </c>
-      <c r="K8" s="10">
-        <v>0</v>
-      </c>
-      <c r="L8" s="10">
-        <v>0</v>
-      </c>
-      <c r="M8" s="10">
-        <v>0</v>
-      </c>
-      <c r="N8" s="10">
-        <v>0</v>
-      </c>
-      <c r="O8" s="10">
-        <v>0</v>
-      </c>
-      <c r="P8" s="14">
-        <v>0</v>
-      </c>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="10"/>
+      <c r="N8" s="10"/>
+      <c r="O8" s="10"/>
+      <c r="P8" s="14"/>
       <c r="Q8" s="9">
         <f t="shared" si="1"/>
         <v>75</v>
@@ -1460,15 +1488,16 @@
       <c r="R8" s="5">
         <v>0</v>
       </c>
-      <c r="S8" s="48">
+      <c r="S8" s="57">
         <v>80</v>
       </c>
-      <c r="T8" s="48">
+      <c r="T8" s="57">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="C9" s="5" t="s">
+    <row r="9" spans="2:20" s="55" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="53"/>
+      <c r="C9" s="54" t="s">
         <v>56</v>
       </c>
       <c r="D9" s="21">
@@ -1499,13 +1528,16 @@
       <c r="N9" s="10"/>
       <c r="O9" s="10"/>
       <c r="P9" s="14"/>
-      <c r="Q9" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R9" s="5">
-        <v>0</v>
-      </c>
+      <c r="Q9" s="54">
+        <v>0</v>
+      </c>
+      <c r="R9" s="54">
+        <v>0</v>
+      </c>
+      <c r="S9" s="53">
+        <v>100</v>
+      </c>
+      <c r="T9" s="53"/>
     </row>
     <row r="10" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
@@ -1549,8 +1581,11 @@
       <c r="R10" s="5">
         <v>0</v>
       </c>
-      <c r="S10">
+      <c r="S10" s="52">
         <v>100</v>
+      </c>
+      <c r="T10" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="2:20" x14ac:dyDescent="0.25">
@@ -1560,12 +1595,12 @@
       <c r="D11" s="20">
         <v>8</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E11" s="56" t="s">
         <v>43</v>
       </c>
       <c r="F11" s="6">
         <f t="shared" si="0"/>
-        <v>26.25</v>
+        <v>33.75</v>
       </c>
       <c r="G11" s="10">
         <v>1</v>
@@ -1585,12 +1620,18 @@
       <c r="N11" s="10"/>
       <c r="O11" s="10"/>
       <c r="P11" s="14"/>
-      <c r="Q11" s="5">
+      <c r="Q11" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="R11" s="5">
         <v>0</v>
+      </c>
+      <c r="S11" s="52">
+        <v>60</v>
+      </c>
+      <c r="T11" s="2">
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="2:20" x14ac:dyDescent="0.25">
@@ -1600,12 +1641,12 @@
       <c r="D12" s="20">
         <v>9</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E12" s="56" t="s">
         <v>15</v>
       </c>
       <c r="F12" s="6">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>36.5</v>
       </c>
       <c r="G12" s="10">
         <v>1</v>
@@ -1614,10 +1655,10 @@
         <v>1</v>
       </c>
       <c r="I12" s="10">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="J12" s="10">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="K12" s="10"/>
       <c r="L12" s="10"/>
@@ -1625,12 +1666,18 @@
       <c r="N12" s="10"/>
       <c r="O12" s="10"/>
       <c r="P12" s="14"/>
-      <c r="Q12" s="5">
+      <c r="Q12" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="R12" s="5">
         <v>0</v>
+      </c>
+      <c r="S12" s="52">
+        <v>90</v>
+      </c>
+      <c r="T12" s="2">
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="2:20" x14ac:dyDescent="0.25">
@@ -1640,12 +1687,12 @@
       <c r="D13" s="20">
         <v>10</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E13" s="56" t="s">
         <v>19</v>
       </c>
       <c r="F13" s="6">
         <f t="shared" si="0"/>
-        <v>26.25</v>
+        <v>40.5</v>
       </c>
       <c r="G13" s="10">
         <v>1</v>
@@ -1665,12 +1712,18 @@
       <c r="N13" s="10"/>
       <c r="O13" s="10"/>
       <c r="P13" s="14"/>
-      <c r="Q13" s="5">
+      <c r="Q13" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>95</v>
       </c>
       <c r="R13" s="5">
         <v>0</v>
+      </c>
+      <c r="S13" s="52">
+        <v>100</v>
+      </c>
+      <c r="T13" s="2">
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="2:20" x14ac:dyDescent="0.25">
@@ -1715,10 +1768,10 @@
       <c r="R14" s="5">
         <v>0</v>
       </c>
-      <c r="S14">
+      <c r="S14" s="52">
         <v>80</v>
       </c>
-      <c r="T14">
+      <c r="T14" s="2">
         <v>10</v>
       </c>
     </row>
@@ -1729,12 +1782,12 @@
       <c r="D15" s="20">
         <v>12</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="E15" s="56" t="s">
         <v>20</v>
       </c>
       <c r="F15" s="6">
         <f t="shared" si="0"/>
-        <v>26.25</v>
+        <v>38.25</v>
       </c>
       <c r="G15" s="10">
         <v>1</v>
@@ -1754,12 +1807,18 @@
       <c r="N15" s="10"/>
       <c r="O15" s="10"/>
       <c r="P15" s="14"/>
-      <c r="Q15" s="5">
+      <c r="Q15" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="R15" s="5">
         <v>0</v>
+      </c>
+      <c r="S15" s="52">
+        <v>90</v>
+      </c>
+      <c r="T15" s="2">
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="2:20" x14ac:dyDescent="0.25">
@@ -1804,8 +1863,11 @@
       <c r="R16" s="5">
         <v>0</v>
       </c>
-      <c r="S16">
+      <c r="S16" s="52">
         <v>100</v>
+      </c>
+      <c r="T16" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="2:20" x14ac:dyDescent="0.25">
@@ -1815,12 +1877,12 @@
       <c r="D17" s="20">
         <v>14</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="E17" s="56" t="s">
         <v>36</v>
       </c>
       <c r="F17" s="6">
         <f t="shared" si="0"/>
-        <v>26.25</v>
+        <v>40.950000000000003</v>
       </c>
       <c r="G17" s="10">
         <v>1</v>
@@ -1840,11 +1902,17 @@
       <c r="N17" s="10"/>
       <c r="O17" s="10"/>
       <c r="P17" s="14"/>
-      <c r="Q17" s="5">
+      <c r="Q17" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>98</v>
       </c>
       <c r="R17" s="5">
+        <v>0</v>
+      </c>
+      <c r="S17" s="52">
+        <v>98</v>
+      </c>
+      <c r="T17" s="2">
         <v>0</v>
       </c>
     </row>
@@ -1855,12 +1923,12 @@
       <c r="D18" s="20">
         <v>15</v>
       </c>
-      <c r="E18" s="4" t="s">
+      <c r="E18" s="56" t="s">
         <v>23</v>
       </c>
       <c r="F18" s="6">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>35.75</v>
       </c>
       <c r="G18" s="10">
         <v>1</v>
@@ -1869,10 +1937,10 @@
         <v>1</v>
       </c>
       <c r="I18" s="10">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="J18" s="10">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="K18" s="10"/>
       <c r="L18" s="10"/>
@@ -1880,12 +1948,18 @@
       <c r="N18" s="10"/>
       <c r="O18" s="10"/>
       <c r="P18" s="14"/>
-      <c r="Q18" s="5">
+      <c r="Q18" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="R18" s="5">
         <v>0</v>
+      </c>
+      <c r="S18" s="52">
+        <v>80</v>
+      </c>
+      <c r="T18" s="2">
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="2:20" x14ac:dyDescent="0.25">
@@ -1895,12 +1969,12 @@
       <c r="D19" s="20">
         <v>16</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="E19" s="56" t="s">
         <v>25</v>
       </c>
       <c r="F19" s="6">
         <f t="shared" si="0"/>
-        <v>28</v>
+        <v>40.75</v>
       </c>
       <c r="G19" s="10">
         <v>1</v>
@@ -1920,12 +1994,18 @@
       <c r="N19" s="10"/>
       <c r="O19" s="10"/>
       <c r="P19" s="14"/>
-      <c r="Q19" s="5">
+      <c r="Q19" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>85</v>
       </c>
       <c r="R19" s="5">
         <v>0</v>
+      </c>
+      <c r="S19" s="52">
+        <v>90</v>
+      </c>
+      <c r="T19" s="2">
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="2:20" x14ac:dyDescent="0.25">
@@ -1940,7 +2020,7 @@
       </c>
       <c r="F20" s="6">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>24.5</v>
       </c>
       <c r="G20" s="11">
         <v>1</v>
@@ -1949,10 +2029,10 @@
         <v>1</v>
       </c>
       <c r="I20" s="10">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="J20" s="10">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="K20" s="10"/>
       <c r="L20" s="10"/>
@@ -1967,6 +2047,12 @@
       <c r="R20" s="5">
         <v>0</v>
       </c>
+      <c r="S20" s="2">
+        <v>0</v>
+      </c>
+      <c r="T20" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="21" spans="2:20" x14ac:dyDescent="0.25">
       <c r="C21" s="3">
@@ -1975,12 +2061,12 @@
       <c r="D21" s="20">
         <v>18</v>
       </c>
-      <c r="E21" s="4" t="s">
+      <c r="E21" s="56" t="s">
         <v>21</v>
       </c>
       <c r="F21" s="6">
         <f t="shared" si="0"/>
-        <v>26.25</v>
+        <v>36.75</v>
       </c>
       <c r="G21" s="10">
         <v>1</v>
@@ -2000,12 +2086,18 @@
       <c r="N21" s="10"/>
       <c r="O21" s="10"/>
       <c r="P21" s="14"/>
-      <c r="Q21" s="5">
+      <c r="Q21" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="R21" s="5">
         <v>0</v>
+      </c>
+      <c r="S21" s="52">
+        <v>80</v>
+      </c>
+      <c r="T21" s="2">
+        <v>10</v>
       </c>
     </row>
     <row r="22" spans="2:20" x14ac:dyDescent="0.25">
@@ -2037,24 +2129,12 @@
       <c r="J22" s="10">
         <v>1</v>
       </c>
-      <c r="K22" s="10">
-        <v>0</v>
-      </c>
-      <c r="L22" s="10">
-        <v>0</v>
-      </c>
-      <c r="M22" s="10">
-        <v>0</v>
-      </c>
-      <c r="N22" s="10">
-        <v>0</v>
-      </c>
-      <c r="O22" s="10">
-        <v>0</v>
-      </c>
-      <c r="P22" s="14">
-        <v>0</v>
-      </c>
+      <c r="K22" s="10"/>
+      <c r="L22" s="10"/>
+      <c r="M22" s="10"/>
+      <c r="N22" s="10"/>
+      <c r="O22" s="10"/>
+      <c r="P22" s="14"/>
       <c r="Q22" s="9">
         <f t="shared" si="1"/>
         <v>55</v>
@@ -2062,10 +2142,10 @@
       <c r="R22" s="5">
         <v>40</v>
       </c>
-      <c r="S22">
+      <c r="S22" s="52">
         <v>60</v>
       </c>
-      <c r="T22">
+      <c r="T22" s="2">
         <v>5</v>
       </c>
     </row>
@@ -2076,12 +2156,12 @@
       <c r="D23" s="20">
         <v>20</v>
       </c>
-      <c r="E23" s="4" t="s">
+      <c r="E23" s="56" t="s">
         <v>42</v>
       </c>
       <c r="F23" s="6">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>34.25</v>
       </c>
       <c r="G23" s="11">
         <v>1</v>
@@ -2090,10 +2170,10 @@
         <v>1</v>
       </c>
       <c r="I23" s="10">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="J23" s="10">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="K23" s="10"/>
       <c r="L23" s="10"/>
@@ -2101,12 +2181,18 @@
       <c r="N23" s="10"/>
       <c r="O23" s="10"/>
       <c r="P23" s="14"/>
-      <c r="Q23" s="5">
+      <c r="Q23" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>65</v>
       </c>
       <c r="R23" s="5">
         <v>0</v>
+      </c>
+      <c r="S23" s="52">
+        <v>80</v>
+      </c>
+      <c r="T23" s="2">
+        <v>15</v>
       </c>
     </row>
     <row r="24" spans="2:20" x14ac:dyDescent="0.25">
@@ -2151,10 +2237,10 @@
       <c r="R24" s="5">
         <v>0</v>
       </c>
-      <c r="S24">
+      <c r="S24" s="52">
         <v>60</v>
       </c>
-      <c r="T24">
+      <c r="T24" s="2">
         <v>5</v>
       </c>
     </row>
@@ -2165,12 +2251,12 @@
       <c r="D25" s="20">
         <v>22</v>
       </c>
-      <c r="E25" s="4" t="s">
+      <c r="E25" s="56" t="s">
         <v>35</v>
       </c>
       <c r="F25" s="6">
         <f t="shared" si="0"/>
-        <v>26.25</v>
+        <v>36</v>
       </c>
       <c r="G25" s="10">
         <v>1</v>
@@ -2190,12 +2276,18 @@
       <c r="N25" s="10"/>
       <c r="O25" s="10"/>
       <c r="P25" s="14"/>
-      <c r="Q25" s="5">
+      <c r="Q25" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>65</v>
       </c>
       <c r="R25" s="5">
         <v>0</v>
+      </c>
+      <c r="S25" s="52">
+        <v>80</v>
+      </c>
+      <c r="T25" s="2">
+        <v>15</v>
       </c>
     </row>
     <row r="26" spans="2:20" x14ac:dyDescent="0.25">
@@ -2240,8 +2332,11 @@
       <c r="R26" s="5">
         <v>0</v>
       </c>
-      <c r="S26">
+      <c r="S26" s="52">
         <v>40</v>
+      </c>
+      <c r="T26" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="2:20" x14ac:dyDescent="0.25">
@@ -2251,12 +2346,12 @@
       <c r="D27" s="20">
         <v>24</v>
       </c>
-      <c r="E27" s="4" t="s">
+      <c r="E27" s="56" t="s">
         <v>41</v>
       </c>
       <c r="F27" s="6">
         <f t="shared" si="0"/>
-        <v>26.25</v>
+        <v>36.75</v>
       </c>
       <c r="G27" s="10">
         <v>1</v>
@@ -2276,12 +2371,18 @@
       <c r="N27" s="10"/>
       <c r="O27" s="10"/>
       <c r="P27" s="14"/>
-      <c r="Q27" s="5">
+      <c r="Q27" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="R27" s="5">
         <v>0</v>
+      </c>
+      <c r="S27" s="52">
+        <v>80</v>
+      </c>
+      <c r="T27" s="2">
+        <v>10</v>
       </c>
     </row>
     <row r="28" spans="2:20" x14ac:dyDescent="0.25">
@@ -2326,10 +2427,10 @@
       <c r="R28" s="5">
         <v>0</v>
       </c>
-      <c r="S28">
+      <c r="S28" s="52">
         <v>80</v>
       </c>
-      <c r="T28">
+      <c r="T28" s="2">
         <v>10</v>
       </c>
     </row>
@@ -2340,12 +2441,12 @@
       <c r="D29" s="20">
         <v>26</v>
       </c>
-      <c r="E29" s="4" t="s">
+      <c r="E29" s="56" t="s">
         <v>46</v>
       </c>
       <c r="F29" s="6">
         <f t="shared" si="0"/>
-        <v>26.25</v>
+        <v>34.5</v>
       </c>
       <c r="G29" s="11">
         <v>1</v>
@@ -2365,12 +2466,18 @@
       <c r="N29" s="10"/>
       <c r="O29" s="10"/>
       <c r="P29" s="14"/>
-      <c r="Q29" s="5">
+      <c r="Q29" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>55</v>
       </c>
       <c r="R29" s="5">
         <v>0</v>
+      </c>
+      <c r="S29" s="52">
+        <v>60</v>
+      </c>
+      <c r="T29" s="2">
+        <v>5</v>
       </c>
     </row>
     <row r="30" spans="2:20" x14ac:dyDescent="0.25">
@@ -2415,10 +2522,10 @@
       <c r="R30" s="5">
         <v>0</v>
       </c>
-      <c r="S30">
+      <c r="S30" s="52">
         <v>90</v>
       </c>
-      <c r="T30">
+      <c r="T30" s="2">
         <v>5</v>
       </c>
     </row>
@@ -2429,12 +2536,12 @@
       <c r="D31" s="20">
         <v>28</v>
       </c>
-      <c r="E31" s="4" t="s">
+      <c r="E31" s="56" t="s">
         <v>28</v>
       </c>
       <c r="F31" s="6">
         <f t="shared" si="0"/>
-        <v>28</v>
+        <v>41.5</v>
       </c>
       <c r="G31" s="10">
         <v>1</v>
@@ -2454,11 +2561,17 @@
       <c r="N31" s="10"/>
       <c r="O31" s="10"/>
       <c r="P31" s="14"/>
-      <c r="Q31" s="5">
+      <c r="Q31" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="R31" s="5">
+        <v>0</v>
+      </c>
+      <c r="S31" s="52">
+        <v>90</v>
+      </c>
+      <c r="T31" s="2">
         <v>0</v>
       </c>
     </row>
@@ -2497,33 +2610,33 @@
       <c r="N32" s="10"/>
       <c r="O32" s="10"/>
       <c r="P32" s="14"/>
-      <c r="Q32" s="5">
+      <c r="Q32" s="9">
         <f t="shared" si="1"/>
         <v>70</v>
       </c>
       <c r="R32" s="5">
         <v>0</v>
       </c>
-      <c r="S32">
+      <c r="S32" s="52">
         <v>80</v>
       </c>
-      <c r="T32">
+      <c r="T32" s="2">
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:20" x14ac:dyDescent="0.25">
       <c r="C33" s="3">
         <v>2</v>
       </c>
       <c r="D33" s="20">
         <v>30</v>
       </c>
-      <c r="E33" s="4" t="s">
+      <c r="E33" s="56" t="s">
         <v>39</v>
       </c>
       <c r="F33" s="6">
         <f t="shared" si="0"/>
-        <v>28</v>
+        <v>42.25</v>
       </c>
       <c r="G33" s="10">
         <v>1</v>
@@ -2543,15 +2656,21 @@
       <c r="N33" s="10"/>
       <c r="O33" s="10"/>
       <c r="P33" s="14"/>
-      <c r="Q33" s="5">
+      <c r="Q33" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>95</v>
       </c>
       <c r="R33" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="S33" s="52">
+        <v>100</v>
+      </c>
+      <c r="T33" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B34" s="2" t="s">
         <v>68</v>
       </c>
@@ -2593,23 +2712,26 @@
       <c r="R34" s="5">
         <v>0</v>
       </c>
-      <c r="S34">
+      <c r="S34" s="52">
         <v>100</v>
       </c>
-    </row>
-    <row r="35" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="T34" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="2:20" x14ac:dyDescent="0.25">
       <c r="C35" s="3">
         <v>2</v>
       </c>
       <c r="D35" s="20">
         <v>32</v>
       </c>
-      <c r="E35" s="4" t="s">
+      <c r="E35" s="56" t="s">
         <v>26</v>
       </c>
       <c r="F35" s="6">
         <f t="shared" si="0"/>
-        <v>26.25</v>
+        <v>34.5</v>
       </c>
       <c r="G35" s="10">
         <v>1</v>
@@ -2629,15 +2751,21 @@
       <c r="N35" s="10"/>
       <c r="O35" s="10"/>
       <c r="P35" s="14"/>
-      <c r="Q35" s="5">
+      <c r="Q35" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>55</v>
       </c>
       <c r="R35" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="S35" s="52">
+        <v>60</v>
+      </c>
+      <c r="T35" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B36" s="2" t="s">
         <v>69</v>
       </c>
@@ -2679,20 +2807,26 @@
       <c r="R36" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="S36" s="2">
+        <v>0</v>
+      </c>
+      <c r="T36" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="2:20" x14ac:dyDescent="0.25">
       <c r="C37" s="3">
         <v>2</v>
       </c>
       <c r="D37" s="20">
         <v>34</v>
       </c>
-      <c r="E37" s="4" t="s">
+      <c r="E37" s="56" t="s">
         <v>14</v>
       </c>
       <c r="F37" s="6">
         <f t="shared" si="0"/>
-        <v>28</v>
+        <v>38.5</v>
       </c>
       <c r="G37" s="10">
         <v>1</v>
@@ -2712,15 +2846,21 @@
       <c r="N37" s="10"/>
       <c r="O37" s="10"/>
       <c r="P37" s="14"/>
-      <c r="Q37" s="5">
+      <c r="Q37" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="R37" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="S37" s="52">
+        <v>70</v>
+      </c>
+      <c r="T37" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B38" s="2" t="s">
         <v>68</v>
       </c>
@@ -2735,7 +2875,7 @@
       </c>
       <c r="F38" s="6">
         <f t="shared" si="0"/>
-        <v>29</v>
+        <v>39.5</v>
       </c>
       <c r="G38" s="10">
         <v>1</v>
@@ -2744,10 +2884,10 @@
         <v>1</v>
       </c>
       <c r="I38" s="10">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="J38" s="10">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="K38" s="10"/>
       <c r="L38" s="10"/>
@@ -2762,41 +2902,44 @@
       <c r="R38" s="5">
         <v>0</v>
       </c>
-      <c r="S38">
+      <c r="S38" s="52">
         <v>100</v>
       </c>
-    </row>
-    <row r="39" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="K39" s="49"/>
-      <c r="L39" s="49"/>
-      <c r="M39" s="49"/>
-      <c r="N39" s="49"/>
-      <c r="O39" s="49"/>
-      <c r="P39" s="49"/>
-    </row>
-    <row r="40" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="K40" s="49"/>
-      <c r="L40" s="49"/>
-      <c r="M40" s="49"/>
-      <c r="N40" s="49"/>
-      <c r="O40" s="49"/>
-      <c r="P40" s="49"/>
-    </row>
-    <row r="41" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="K41" s="49"/>
-      <c r="L41" s="49"/>
-      <c r="M41" s="49"/>
-      <c r="N41" s="49"/>
-      <c r="O41" s="49"/>
-      <c r="P41" s="49"/>
-    </row>
-    <row r="42" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="K42" s="49"/>
-      <c r="L42" s="49"/>
-      <c r="M42" s="49"/>
-      <c r="N42" s="49"/>
-      <c r="O42" s="49"/>
-      <c r="P42" s="49"/>
+      <c r="T38" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="K39" s="25"/>
+      <c r="L39" s="25"/>
+      <c r="M39" s="25"/>
+      <c r="N39" s="25"/>
+      <c r="O39" s="25"/>
+      <c r="P39" s="25"/>
+    </row>
+    <row r="40" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="K40" s="25"/>
+      <c r="L40" s="25"/>
+      <c r="M40" s="25"/>
+      <c r="N40" s="25"/>
+      <c r="O40" s="25"/>
+      <c r="P40" s="25"/>
+    </row>
+    <row r="41" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="K41" s="25"/>
+      <c r="L41" s="25"/>
+      <c r="M41" s="25"/>
+      <c r="N41" s="25"/>
+      <c r="O41" s="25"/>
+      <c r="P41" s="25"/>
+    </row>
+    <row r="42" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="K42" s="25"/>
+      <c r="L42" s="25"/>
+      <c r="M42" s="25"/>
+      <c r="N42" s="25"/>
+      <c r="O42" s="25"/>
+      <c r="P42" s="25"/>
     </row>
     <row r="1048576" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G1048576" s="6"/>
@@ -2815,7 +2958,7 @@
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="H1:J1"/>
   </mergeCells>
-  <conditionalFormatting sqref="S8:T8 G4:P38">
+  <conditionalFormatting sqref="G4:P38">
     <cfRule type="dataBar" priority="1">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -2848,7 +2991,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>S8:T8 G4:P38</xm:sqref>
+          <xm:sqref>G4:P38</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -2860,13 +3003,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{153E42C8-D1FE-4E64-96D9-EED2206D80DB}">
   <dimension ref="A1:M10"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="46.5" x14ac:dyDescent="0.7"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="47"/>
+    <col min="1" max="16384" width="9.140625" style="24"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.7">
@@ -2887,84 +3030,84 @@
       <c r="M1" s="46"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.7">
-      <c r="A2" s="47">
-        <v>1</v>
-      </c>
-      <c r="B2" s="47" t="s">
+      <c r="A2" s="24">
+        <v>1</v>
+      </c>
+      <c r="B2" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="G2" s="47" t="s">
+      <c r="G2" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="H2" s="47" t="s">
+      <c r="H2" s="24" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.7">
+      <c r="C3" s="24" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.7">
-      <c r="C3" s="47" t="s">
+      <c r="H3" s="24" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.7">
+      <c r="C4" s="24" t="s">
+        <v>74</v>
+      </c>
+      <c r="H4" s="24" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.7">
+      <c r="A5" s="24">
+        <v>2</v>
+      </c>
+      <c r="B5" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="24" t="s">
+        <v>72</v>
+      </c>
+      <c r="H5" s="24">
+        <v>1</v>
+      </c>
+      <c r="I5" s="24" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.7">
+      <c r="H6" s="24">
+        <v>2</v>
+      </c>
+      <c r="I6" s="24" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.7">
+      <c r="H7" s="24">
+        <v>3</v>
+      </c>
+      <c r="I7" s="24" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.7">
+      <c r="C8" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="H3" s="47" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.7">
-      <c r="C4" s="47" t="s">
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.7">
+      <c r="C9" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="H4" s="47" t="s">
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.7">
+      <c r="A10" s="24">
+        <v>3</v>
+      </c>
+      <c r="B10" s="24" t="s">
         <v>77</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.7">
-      <c r="A5" s="47">
-        <v>2</v>
-      </c>
-      <c r="B5" s="47" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" s="47" t="s">
-        <v>72</v>
-      </c>
-      <c r="H5" s="47">
-        <v>1</v>
-      </c>
-      <c r="I5" s="47" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.7">
-      <c r="H6" s="47">
-        <v>2</v>
-      </c>
-      <c r="I6" s="47" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.7">
-      <c r="H7" s="47">
-        <v>3</v>
-      </c>
-      <c r="I7" s="47" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.7">
-      <c r="C8" s="47" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.7">
-      <c r="C9" s="47" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.7">
-      <c r="A10" s="47">
-        <v>3</v>
-      </c>
-      <c r="B10" s="47" t="s">
-        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -3005,603 +3148,608 @@
       <c r="Q2" s="2"/>
     </row>
     <row r="3" spans="5:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E3" s="42">
-        <v>1</v>
-      </c>
-      <c r="F3" s="44" t="s">
+      <c r="E3" s="47">
+        <v>1</v>
+      </c>
+      <c r="F3" s="49" t="s">
         <v>51</v>
       </c>
-      <c r="G3" s="45"/>
-      <c r="H3" s="45"/>
-      <c r="I3" s="45"/>
-      <c r="J3" s="45"/>
-      <c r="K3" s="45"/>
-      <c r="L3" s="45"/>
-      <c r="M3" s="45"/>
-      <c r="N3" s="45"/>
-      <c r="O3" s="45"/>
-      <c r="P3" s="45"/>
-      <c r="Q3" s="45"/>
-      <c r="S3" s="42" t="s">
+      <c r="G3" s="50"/>
+      <c r="H3" s="50"/>
+      <c r="I3" s="50"/>
+      <c r="J3" s="50"/>
+      <c r="K3" s="50"/>
+      <c r="L3" s="50"/>
+      <c r="M3" s="50"/>
+      <c r="N3" s="50"/>
+      <c r="O3" s="50"/>
+      <c r="P3" s="50"/>
+      <c r="Q3" s="50"/>
+      <c r="S3" s="47" t="s">
         <v>58</v>
       </c>
-      <c r="T3" s="42"/>
-      <c r="U3" s="42"/>
-      <c r="W3" s="41" t="s">
+      <c r="T3" s="47"/>
+      <c r="U3" s="47"/>
+      <c r="W3" s="51" t="s">
         <v>60</v>
       </c>
-      <c r="X3" s="41"/>
+      <c r="X3" s="51"/>
     </row>
     <row r="4" spans="5:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E4" s="42"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
-      <c r="H4" s="45"/>
-      <c r="I4" s="45"/>
-      <c r="J4" s="45"/>
-      <c r="K4" s="45"/>
-      <c r="L4" s="45"/>
-      <c r="M4" s="45"/>
-      <c r="N4" s="45"/>
-      <c r="O4" s="45"/>
-      <c r="P4" s="45"/>
-      <c r="Q4" s="45"/>
-      <c r="S4" s="42"/>
-      <c r="T4" s="42"/>
-      <c r="U4" s="42"/>
-      <c r="W4" s="41"/>
-      <c r="X4" s="41"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="50"/>
+      <c r="G4" s="50"/>
+      <c r="H4" s="50"/>
+      <c r="I4" s="50"/>
+      <c r="J4" s="50"/>
+      <c r="K4" s="50"/>
+      <c r="L4" s="50"/>
+      <c r="M4" s="50"/>
+      <c r="N4" s="50"/>
+      <c r="O4" s="50"/>
+      <c r="P4" s="50"/>
+      <c r="Q4" s="50"/>
+      <c r="S4" s="47"/>
+      <c r="T4" s="47"/>
+      <c r="U4" s="47"/>
+      <c r="W4" s="51"/>
+      <c r="X4" s="51"/>
     </row>
     <row r="5" spans="5:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E5" s="42"/>
-      <c r="F5" s="45"/>
-      <c r="G5" s="45"/>
-      <c r="H5" s="45"/>
-      <c r="I5" s="45"/>
-      <c r="J5" s="45"/>
-      <c r="K5" s="45"/>
-      <c r="L5" s="45"/>
-      <c r="M5" s="45"/>
-      <c r="N5" s="45"/>
-      <c r="O5" s="45"/>
-      <c r="P5" s="45"/>
-      <c r="Q5" s="45"/>
-      <c r="S5" s="42"/>
-      <c r="T5" s="42"/>
-      <c r="U5" s="42"/>
-      <c r="W5" s="41"/>
-      <c r="X5" s="41"/>
+      <c r="E5" s="47"/>
+      <c r="F5" s="50"/>
+      <c r="G5" s="50"/>
+      <c r="H5" s="50"/>
+      <c r="I5" s="50"/>
+      <c r="J5" s="50"/>
+      <c r="K5" s="50"/>
+      <c r="L5" s="50"/>
+      <c r="M5" s="50"/>
+      <c r="N5" s="50"/>
+      <c r="O5" s="50"/>
+      <c r="P5" s="50"/>
+      <c r="Q5" s="50"/>
+      <c r="S5" s="47"/>
+      <c r="T5" s="47"/>
+      <c r="U5" s="47"/>
+      <c r="W5" s="51"/>
+      <c r="X5" s="51"/>
     </row>
     <row r="6" spans="5:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E6" s="42"/>
-      <c r="F6" s="45"/>
-      <c r="G6" s="45"/>
-      <c r="H6" s="45"/>
-      <c r="I6" s="45"/>
-      <c r="J6" s="45"/>
-      <c r="K6" s="45"/>
-      <c r="L6" s="45"/>
-      <c r="M6" s="45"/>
-      <c r="N6" s="45"/>
-      <c r="O6" s="45"/>
-      <c r="P6" s="45"/>
-      <c r="Q6" s="45"/>
-      <c r="S6" s="42"/>
-      <c r="T6" s="42"/>
-      <c r="U6" s="42"/>
-      <c r="W6" s="41"/>
-      <c r="X6" s="41"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="50"/>
+      <c r="G6" s="50"/>
+      <c r="H6" s="50"/>
+      <c r="I6" s="50"/>
+      <c r="J6" s="50"/>
+      <c r="K6" s="50"/>
+      <c r="L6" s="50"/>
+      <c r="M6" s="50"/>
+      <c r="N6" s="50"/>
+      <c r="O6" s="50"/>
+      <c r="P6" s="50"/>
+      <c r="Q6" s="50"/>
+      <c r="S6" s="47"/>
+      <c r="T6" s="47"/>
+      <c r="U6" s="47"/>
+      <c r="W6" s="51"/>
+      <c r="X6" s="51"/>
     </row>
     <row r="7" spans="5:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E7" s="42"/>
-      <c r="F7" s="45"/>
-      <c r="G7" s="45"/>
-      <c r="H7" s="45"/>
-      <c r="I7" s="45"/>
-      <c r="J7" s="45"/>
-      <c r="K7" s="45"/>
-      <c r="L7" s="45"/>
-      <c r="M7" s="45"/>
-      <c r="N7" s="45"/>
-      <c r="O7" s="45"/>
-      <c r="P7" s="45"/>
-      <c r="Q7" s="45"/>
-      <c r="S7" s="42"/>
-      <c r="T7" s="42"/>
-      <c r="U7" s="42"/>
-      <c r="W7" s="41"/>
-      <c r="X7" s="41"/>
+      <c r="E7" s="47"/>
+      <c r="F7" s="50"/>
+      <c r="G7" s="50"/>
+      <c r="H7" s="50"/>
+      <c r="I7" s="50"/>
+      <c r="J7" s="50"/>
+      <c r="K7" s="50"/>
+      <c r="L7" s="50"/>
+      <c r="M7" s="50"/>
+      <c r="N7" s="50"/>
+      <c r="O7" s="50"/>
+      <c r="P7" s="50"/>
+      <c r="Q7" s="50"/>
+      <c r="S7" s="47"/>
+      <c r="T7" s="47"/>
+      <c r="U7" s="47"/>
+      <c r="W7" s="51"/>
+      <c r="X7" s="51"/>
     </row>
     <row r="8" spans="5:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E8" s="42">
+      <c r="E8" s="47">
         <v>2</v>
       </c>
-      <c r="F8" s="44" t="s">
+      <c r="F8" s="49" t="s">
         <v>52</v>
       </c>
-      <c r="G8" s="45"/>
-      <c r="H8" s="45"/>
-      <c r="I8" s="45"/>
-      <c r="J8" s="45"/>
-      <c r="K8" s="45"/>
-      <c r="L8" s="45"/>
-      <c r="M8" s="45"/>
-      <c r="N8" s="45"/>
-      <c r="O8" s="45"/>
-      <c r="P8" s="45"/>
-      <c r="Q8" s="45"/>
-      <c r="S8" s="42" t="s">
+      <c r="G8" s="50"/>
+      <c r="H8" s="50"/>
+      <c r="I8" s="50"/>
+      <c r="J8" s="50"/>
+      <c r="K8" s="50"/>
+      <c r="L8" s="50"/>
+      <c r="M8" s="50"/>
+      <c r="N8" s="50"/>
+      <c r="O8" s="50"/>
+      <c r="P8" s="50"/>
+      <c r="Q8" s="50"/>
+      <c r="S8" s="47" t="s">
         <v>58</v>
       </c>
-      <c r="T8" s="42"/>
-      <c r="U8" s="42"/>
-      <c r="W8" s="41" t="s">
+      <c r="T8" s="47"/>
+      <c r="U8" s="47"/>
+      <c r="W8" s="51" t="s">
         <v>61</v>
       </c>
-      <c r="X8" s="41"/>
+      <c r="X8" s="51"/>
     </row>
     <row r="9" spans="5:24" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E9" s="42"/>
-      <c r="F9" s="45"/>
-      <c r="G9" s="45"/>
-      <c r="H9" s="45"/>
-      <c r="I9" s="45"/>
-      <c r="J9" s="45"/>
-      <c r="K9" s="45"/>
-      <c r="L9" s="45"/>
-      <c r="M9" s="45"/>
-      <c r="N9" s="45"/>
-      <c r="O9" s="45"/>
-      <c r="P9" s="45"/>
-      <c r="Q9" s="45"/>
-      <c r="S9" s="42"/>
-      <c r="T9" s="42"/>
-      <c r="U9" s="42"/>
-      <c r="W9" s="41"/>
-      <c r="X9" s="41"/>
+      <c r="E9" s="47"/>
+      <c r="F9" s="50"/>
+      <c r="G9" s="50"/>
+      <c r="H9" s="50"/>
+      <c r="I9" s="50"/>
+      <c r="J9" s="50"/>
+      <c r="K9" s="50"/>
+      <c r="L9" s="50"/>
+      <c r="M9" s="50"/>
+      <c r="N9" s="50"/>
+      <c r="O9" s="50"/>
+      <c r="P9" s="50"/>
+      <c r="Q9" s="50"/>
+      <c r="S9" s="47"/>
+      <c r="T9" s="47"/>
+      <c r="U9" s="47"/>
+      <c r="W9" s="51"/>
+      <c r="X9" s="51"/>
     </row>
     <row r="10" spans="5:24" x14ac:dyDescent="0.25">
-      <c r="E10" s="42">
+      <c r="E10" s="47">
         <v>3</v>
       </c>
-      <c r="F10" s="44" t="s">
+      <c r="F10" s="49" t="s">
         <v>53</v>
       </c>
-      <c r="G10" s="45"/>
-      <c r="H10" s="45"/>
-      <c r="I10" s="44" t="s">
+      <c r="G10" s="50"/>
+      <c r="H10" s="50"/>
+      <c r="I10" s="49" t="s">
         <v>64</v>
       </c>
-      <c r="J10" s="45"/>
-      <c r="K10" s="45"/>
-      <c r="L10" s="45"/>
-      <c r="M10" s="45"/>
-      <c r="N10" s="45"/>
-      <c r="O10" s="45"/>
-      <c r="P10" s="45"/>
-      <c r="Q10" s="45"/>
-      <c r="S10" s="43" t="s">
+      <c r="J10" s="50"/>
+      <c r="K10" s="50"/>
+      <c r="L10" s="50"/>
+      <c r="M10" s="50"/>
+      <c r="N10" s="50"/>
+      <c r="O10" s="50"/>
+      <c r="P10" s="50"/>
+      <c r="Q10" s="50"/>
+      <c r="S10" s="48" t="s">
         <v>59</v>
       </c>
-      <c r="T10" s="42"/>
-      <c r="U10" s="42"/>
-      <c r="W10" s="41" t="s">
+      <c r="T10" s="47"/>
+      <c r="U10" s="47"/>
+      <c r="W10" s="51" t="s">
         <v>62</v>
       </c>
-      <c r="X10" s="41" t="s">
+      <c r="X10" s="51" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="11" spans="5:24" x14ac:dyDescent="0.25">
-      <c r="E11" s="42"/>
-      <c r="F11" s="45"/>
-      <c r="G11" s="45"/>
-      <c r="H11" s="45"/>
-      <c r="I11" s="45"/>
-      <c r="J11" s="45"/>
-      <c r="K11" s="45"/>
-      <c r="L11" s="45"/>
-      <c r="M11" s="45"/>
-      <c r="N11" s="45"/>
-      <c r="O11" s="45"/>
-      <c r="P11" s="45"/>
-      <c r="Q11" s="45"/>
-      <c r="S11" s="42"/>
-      <c r="T11" s="42"/>
-      <c r="U11" s="42"/>
-      <c r="W11" s="41"/>
-      <c r="X11" s="41"/>
+      <c r="E11" s="47"/>
+      <c r="F11" s="50"/>
+      <c r="G11" s="50"/>
+      <c r="H11" s="50"/>
+      <c r="I11" s="50"/>
+      <c r="J11" s="50"/>
+      <c r="K11" s="50"/>
+      <c r="L11" s="50"/>
+      <c r="M11" s="50"/>
+      <c r="N11" s="50"/>
+      <c r="O11" s="50"/>
+      <c r="P11" s="50"/>
+      <c r="Q11" s="50"/>
+      <c r="S11" s="47"/>
+      <c r="T11" s="47"/>
+      <c r="U11" s="47"/>
+      <c r="W11" s="51"/>
+      <c r="X11" s="51"/>
     </row>
     <row r="12" spans="5:24" x14ac:dyDescent="0.25">
-      <c r="E12" s="42"/>
-      <c r="F12" s="45"/>
-      <c r="G12" s="45"/>
-      <c r="H12" s="45"/>
-      <c r="I12" s="45"/>
-      <c r="J12" s="45"/>
-      <c r="K12" s="45"/>
-      <c r="L12" s="45"/>
-      <c r="M12" s="45"/>
-      <c r="N12" s="45"/>
-      <c r="O12" s="45"/>
-      <c r="P12" s="45"/>
-      <c r="Q12" s="45"/>
-      <c r="S12" s="42"/>
-      <c r="T12" s="42"/>
-      <c r="U12" s="42"/>
-      <c r="W12" s="41"/>
-      <c r="X12" s="41"/>
+      <c r="E12" s="47"/>
+      <c r="F12" s="50"/>
+      <c r="G12" s="50"/>
+      <c r="H12" s="50"/>
+      <c r="I12" s="50"/>
+      <c r="J12" s="50"/>
+      <c r="K12" s="50"/>
+      <c r="L12" s="50"/>
+      <c r="M12" s="50"/>
+      <c r="N12" s="50"/>
+      <c r="O12" s="50"/>
+      <c r="P12" s="50"/>
+      <c r="Q12" s="50"/>
+      <c r="S12" s="47"/>
+      <c r="T12" s="47"/>
+      <c r="U12" s="47"/>
+      <c r="W12" s="51"/>
+      <c r="X12" s="51"/>
     </row>
     <row r="13" spans="5:24" x14ac:dyDescent="0.25">
-      <c r="E13" s="42"/>
-      <c r="F13" s="45"/>
-      <c r="G13" s="45"/>
-      <c r="H13" s="45"/>
-      <c r="I13" s="45"/>
-      <c r="J13" s="45"/>
-      <c r="K13" s="45"/>
-      <c r="L13" s="45"/>
-      <c r="M13" s="45"/>
-      <c r="N13" s="45"/>
-      <c r="O13" s="45"/>
-      <c r="P13" s="45"/>
-      <c r="Q13" s="45"/>
-      <c r="S13" s="42"/>
-      <c r="T13" s="42"/>
-      <c r="U13" s="42"/>
-      <c r="W13" s="41"/>
-      <c r="X13" s="41"/>
+      <c r="E13" s="47"/>
+      <c r="F13" s="50"/>
+      <c r="G13" s="50"/>
+      <c r="H13" s="50"/>
+      <c r="I13" s="50"/>
+      <c r="J13" s="50"/>
+      <c r="K13" s="50"/>
+      <c r="L13" s="50"/>
+      <c r="M13" s="50"/>
+      <c r="N13" s="50"/>
+      <c r="O13" s="50"/>
+      <c r="P13" s="50"/>
+      <c r="Q13" s="50"/>
+      <c r="S13" s="47"/>
+      <c r="T13" s="47"/>
+      <c r="U13" s="47"/>
+      <c r="W13" s="51"/>
+      <c r="X13" s="51"/>
     </row>
     <row r="14" spans="5:24" x14ac:dyDescent="0.25">
-      <c r="E14" s="42"/>
-      <c r="F14" s="45"/>
-      <c r="G14" s="45"/>
-      <c r="H14" s="45"/>
-      <c r="I14" s="45"/>
-      <c r="J14" s="45"/>
-      <c r="K14" s="45"/>
-      <c r="L14" s="45"/>
-      <c r="M14" s="45"/>
-      <c r="N14" s="45"/>
-      <c r="O14" s="45"/>
-      <c r="P14" s="45"/>
-      <c r="Q14" s="45"/>
-      <c r="S14" s="42"/>
-      <c r="T14" s="42"/>
-      <c r="U14" s="42"/>
-      <c r="W14" s="41"/>
-      <c r="X14" s="41"/>
+      <c r="E14" s="47"/>
+      <c r="F14" s="50"/>
+      <c r="G14" s="50"/>
+      <c r="H14" s="50"/>
+      <c r="I14" s="50"/>
+      <c r="J14" s="50"/>
+      <c r="K14" s="50"/>
+      <c r="L14" s="50"/>
+      <c r="M14" s="50"/>
+      <c r="N14" s="50"/>
+      <c r="O14" s="50"/>
+      <c r="P14" s="50"/>
+      <c r="Q14" s="50"/>
+      <c r="S14" s="47"/>
+      <c r="T14" s="47"/>
+      <c r="U14" s="47"/>
+      <c r="W14" s="51"/>
+      <c r="X14" s="51"/>
     </row>
     <row r="15" spans="5:24" x14ac:dyDescent="0.25">
-      <c r="E15" s="42"/>
-      <c r="F15" s="45"/>
-      <c r="G15" s="45"/>
-      <c r="H15" s="45"/>
-      <c r="I15" s="45"/>
-      <c r="J15" s="45"/>
-      <c r="K15" s="45"/>
-      <c r="L15" s="45"/>
-      <c r="M15" s="45"/>
-      <c r="N15" s="45"/>
-      <c r="O15" s="45"/>
-      <c r="P15" s="45"/>
-      <c r="Q15" s="45"/>
-      <c r="S15" s="42"/>
-      <c r="T15" s="42"/>
-      <c r="U15" s="42"/>
-      <c r="W15" s="41"/>
-      <c r="X15" s="41"/>
+      <c r="E15" s="47"/>
+      <c r="F15" s="50"/>
+      <c r="G15" s="50"/>
+      <c r="H15" s="50"/>
+      <c r="I15" s="50"/>
+      <c r="J15" s="50"/>
+      <c r="K15" s="50"/>
+      <c r="L15" s="50"/>
+      <c r="M15" s="50"/>
+      <c r="N15" s="50"/>
+      <c r="O15" s="50"/>
+      <c r="P15" s="50"/>
+      <c r="Q15" s="50"/>
+      <c r="S15" s="47"/>
+      <c r="T15" s="47"/>
+      <c r="U15" s="47"/>
+      <c r="W15" s="51"/>
+      <c r="X15" s="51"/>
     </row>
     <row r="16" spans="5:24" x14ac:dyDescent="0.25">
-      <c r="E16" s="42"/>
-      <c r="F16" s="45"/>
-      <c r="G16" s="45"/>
-      <c r="H16" s="45"/>
-      <c r="I16" s="45"/>
-      <c r="J16" s="45"/>
-      <c r="K16" s="45"/>
-      <c r="L16" s="45"/>
-      <c r="M16" s="45"/>
-      <c r="N16" s="45"/>
-      <c r="O16" s="45"/>
-      <c r="P16" s="45"/>
-      <c r="Q16" s="45"/>
-      <c r="S16" s="42"/>
-      <c r="T16" s="42"/>
-      <c r="U16" s="42"/>
-      <c r="W16" s="41"/>
-      <c r="X16" s="41"/>
+      <c r="E16" s="47"/>
+      <c r="F16" s="50"/>
+      <c r="G16" s="50"/>
+      <c r="H16" s="50"/>
+      <c r="I16" s="50"/>
+      <c r="J16" s="50"/>
+      <c r="K16" s="50"/>
+      <c r="L16" s="50"/>
+      <c r="M16" s="50"/>
+      <c r="N16" s="50"/>
+      <c r="O16" s="50"/>
+      <c r="P16" s="50"/>
+      <c r="Q16" s="50"/>
+      <c r="S16" s="47"/>
+      <c r="T16" s="47"/>
+      <c r="U16" s="47"/>
+      <c r="W16" s="51"/>
+      <c r="X16" s="51"/>
     </row>
     <row r="17" spans="5:24" x14ac:dyDescent="0.25">
-      <c r="E17" s="42"/>
-      <c r="F17" s="45"/>
-      <c r="G17" s="45"/>
-      <c r="H17" s="45"/>
-      <c r="I17" s="45"/>
-      <c r="J17" s="45"/>
-      <c r="K17" s="45"/>
-      <c r="L17" s="45"/>
-      <c r="M17" s="45"/>
-      <c r="N17" s="45"/>
-      <c r="O17" s="45"/>
-      <c r="P17" s="45"/>
-      <c r="Q17" s="45"/>
-      <c r="S17" s="42"/>
-      <c r="T17" s="42"/>
-      <c r="U17" s="42"/>
-      <c r="W17" s="41"/>
-      <c r="X17" s="41"/>
+      <c r="E17" s="47"/>
+      <c r="F17" s="50"/>
+      <c r="G17" s="50"/>
+      <c r="H17" s="50"/>
+      <c r="I17" s="50"/>
+      <c r="J17" s="50"/>
+      <c r="K17" s="50"/>
+      <c r="L17" s="50"/>
+      <c r="M17" s="50"/>
+      <c r="N17" s="50"/>
+      <c r="O17" s="50"/>
+      <c r="P17" s="50"/>
+      <c r="Q17" s="50"/>
+      <c r="S17" s="47"/>
+      <c r="T17" s="47"/>
+      <c r="U17" s="47"/>
+      <c r="W17" s="51"/>
+      <c r="X17" s="51"/>
     </row>
     <row r="18" spans="5:24" x14ac:dyDescent="0.25">
-      <c r="E18" s="42"/>
-      <c r="F18" s="45"/>
-      <c r="G18" s="45"/>
-      <c r="H18" s="45"/>
-      <c r="I18" s="45"/>
-      <c r="J18" s="45"/>
-      <c r="K18" s="45"/>
-      <c r="L18" s="45"/>
-      <c r="M18" s="45"/>
-      <c r="N18" s="45"/>
-      <c r="O18" s="45"/>
-      <c r="P18" s="45"/>
-      <c r="Q18" s="45"/>
-      <c r="S18" s="42"/>
-      <c r="T18" s="42"/>
-      <c r="U18" s="42"/>
-      <c r="W18" s="41"/>
-      <c r="X18" s="41"/>
+      <c r="E18" s="47"/>
+      <c r="F18" s="50"/>
+      <c r="G18" s="50"/>
+      <c r="H18" s="50"/>
+      <c r="I18" s="50"/>
+      <c r="J18" s="50"/>
+      <c r="K18" s="50"/>
+      <c r="L18" s="50"/>
+      <c r="M18" s="50"/>
+      <c r="N18" s="50"/>
+      <c r="O18" s="50"/>
+      <c r="P18" s="50"/>
+      <c r="Q18" s="50"/>
+      <c r="S18" s="47"/>
+      <c r="T18" s="47"/>
+      <c r="U18" s="47"/>
+      <c r="W18" s="51"/>
+      <c r="X18" s="51"/>
     </row>
     <row r="19" spans="5:24" x14ac:dyDescent="0.25">
-      <c r="E19" s="42"/>
-      <c r="F19" s="45"/>
-      <c r="G19" s="45"/>
-      <c r="H19" s="45"/>
-      <c r="I19" s="45"/>
-      <c r="J19" s="45"/>
-      <c r="K19" s="45"/>
-      <c r="L19" s="45"/>
-      <c r="M19" s="45"/>
-      <c r="N19" s="45"/>
-      <c r="O19" s="45"/>
-      <c r="P19" s="45"/>
-      <c r="Q19" s="45"/>
-      <c r="S19" s="42"/>
-      <c r="T19" s="42"/>
-      <c r="U19" s="42"/>
-      <c r="W19" s="41"/>
-      <c r="X19" s="41"/>
+      <c r="E19" s="47"/>
+      <c r="F19" s="50"/>
+      <c r="G19" s="50"/>
+      <c r="H19" s="50"/>
+      <c r="I19" s="50"/>
+      <c r="J19" s="50"/>
+      <c r="K19" s="50"/>
+      <c r="L19" s="50"/>
+      <c r="M19" s="50"/>
+      <c r="N19" s="50"/>
+      <c r="O19" s="50"/>
+      <c r="P19" s="50"/>
+      <c r="Q19" s="50"/>
+      <c r="S19" s="47"/>
+      <c r="T19" s="47"/>
+      <c r="U19" s="47"/>
+      <c r="W19" s="51"/>
+      <c r="X19" s="51"/>
     </row>
     <row r="20" spans="5:24" x14ac:dyDescent="0.25">
-      <c r="E20" s="42"/>
-      <c r="F20" s="45"/>
-      <c r="G20" s="45"/>
-      <c r="H20" s="45"/>
-      <c r="I20" s="45"/>
-      <c r="J20" s="45"/>
-      <c r="K20" s="45"/>
-      <c r="L20" s="45"/>
-      <c r="M20" s="45"/>
-      <c r="N20" s="45"/>
-      <c r="O20" s="45"/>
-      <c r="P20" s="45"/>
-      <c r="Q20" s="45"/>
-      <c r="S20" s="42"/>
-      <c r="T20" s="42"/>
-      <c r="U20" s="42"/>
-      <c r="W20" s="41"/>
-      <c r="X20" s="41"/>
+      <c r="E20" s="47"/>
+      <c r="F20" s="50"/>
+      <c r="G20" s="50"/>
+      <c r="H20" s="50"/>
+      <c r="I20" s="50"/>
+      <c r="J20" s="50"/>
+      <c r="K20" s="50"/>
+      <c r="L20" s="50"/>
+      <c r="M20" s="50"/>
+      <c r="N20" s="50"/>
+      <c r="O20" s="50"/>
+      <c r="P20" s="50"/>
+      <c r="Q20" s="50"/>
+      <c r="S20" s="47"/>
+      <c r="T20" s="47"/>
+      <c r="U20" s="47"/>
+      <c r="W20" s="51"/>
+      <c r="X20" s="51"/>
     </row>
     <row r="21" spans="5:24" x14ac:dyDescent="0.25">
-      <c r="E21" s="42"/>
-      <c r="F21" s="45"/>
-      <c r="G21" s="45"/>
-      <c r="H21" s="45"/>
-      <c r="I21" s="45"/>
-      <c r="J21" s="45"/>
-      <c r="K21" s="45"/>
-      <c r="L21" s="45"/>
-      <c r="M21" s="45"/>
-      <c r="N21" s="45"/>
-      <c r="O21" s="45"/>
-      <c r="P21" s="45"/>
-      <c r="Q21" s="45"/>
-      <c r="S21" s="42"/>
-      <c r="T21" s="42"/>
-      <c r="U21" s="42"/>
-      <c r="W21" s="41"/>
-      <c r="X21" s="41"/>
+      <c r="E21" s="47"/>
+      <c r="F21" s="50"/>
+      <c r="G21" s="50"/>
+      <c r="H21" s="50"/>
+      <c r="I21" s="50"/>
+      <c r="J21" s="50"/>
+      <c r="K21" s="50"/>
+      <c r="L21" s="50"/>
+      <c r="M21" s="50"/>
+      <c r="N21" s="50"/>
+      <c r="O21" s="50"/>
+      <c r="P21" s="50"/>
+      <c r="Q21" s="50"/>
+      <c r="S21" s="47"/>
+      <c r="T21" s="47"/>
+      <c r="U21" s="47"/>
+      <c r="W21" s="51"/>
+      <c r="X21" s="51"/>
     </row>
     <row r="22" spans="5:24" x14ac:dyDescent="0.25">
-      <c r="E22" s="42"/>
-      <c r="F22" s="45"/>
-      <c r="G22" s="45"/>
-      <c r="H22" s="45"/>
-      <c r="I22" s="45"/>
-      <c r="J22" s="45"/>
-      <c r="K22" s="45"/>
-      <c r="L22" s="45"/>
-      <c r="M22" s="45"/>
-      <c r="N22" s="45"/>
-      <c r="O22" s="45"/>
-      <c r="P22" s="45"/>
-      <c r="Q22" s="45"/>
-      <c r="S22" s="42"/>
-      <c r="T22" s="42"/>
-      <c r="U22" s="42"/>
-      <c r="W22" s="41"/>
-      <c r="X22" s="41"/>
+      <c r="E22" s="47"/>
+      <c r="F22" s="50"/>
+      <c r="G22" s="50"/>
+      <c r="H22" s="50"/>
+      <c r="I22" s="50"/>
+      <c r="J22" s="50"/>
+      <c r="K22" s="50"/>
+      <c r="L22" s="50"/>
+      <c r="M22" s="50"/>
+      <c r="N22" s="50"/>
+      <c r="O22" s="50"/>
+      <c r="P22" s="50"/>
+      <c r="Q22" s="50"/>
+      <c r="S22" s="47"/>
+      <c r="T22" s="47"/>
+      <c r="U22" s="47"/>
+      <c r="W22" s="51"/>
+      <c r="X22" s="51"/>
     </row>
     <row r="23" spans="5:24" x14ac:dyDescent="0.25">
-      <c r="E23" s="42"/>
-      <c r="F23" s="45"/>
-      <c r="G23" s="45"/>
-      <c r="H23" s="45"/>
-      <c r="I23" s="45"/>
-      <c r="J23" s="45"/>
-      <c r="K23" s="45"/>
-      <c r="L23" s="45"/>
-      <c r="M23" s="45"/>
-      <c r="N23" s="45"/>
-      <c r="O23" s="45"/>
-      <c r="P23" s="45"/>
-      <c r="Q23" s="45"/>
-      <c r="S23" s="42"/>
-      <c r="T23" s="42"/>
-      <c r="U23" s="42"/>
-      <c r="W23" s="41"/>
-      <c r="X23" s="41"/>
+      <c r="E23" s="47"/>
+      <c r="F23" s="50"/>
+      <c r="G23" s="50"/>
+      <c r="H23" s="50"/>
+      <c r="I23" s="50"/>
+      <c r="J23" s="50"/>
+      <c r="K23" s="50"/>
+      <c r="L23" s="50"/>
+      <c r="M23" s="50"/>
+      <c r="N23" s="50"/>
+      <c r="O23" s="50"/>
+      <c r="P23" s="50"/>
+      <c r="Q23" s="50"/>
+      <c r="S23" s="47"/>
+      <c r="T23" s="47"/>
+      <c r="U23" s="47"/>
+      <c r="W23" s="51"/>
+      <c r="X23" s="51"/>
     </row>
     <row r="24" spans="5:24" x14ac:dyDescent="0.25">
-      <c r="E24" s="42"/>
-      <c r="F24" s="45"/>
-      <c r="G24" s="45"/>
-      <c r="H24" s="45"/>
-      <c r="I24" s="45"/>
-      <c r="J24" s="45"/>
-      <c r="K24" s="45"/>
-      <c r="L24" s="45"/>
-      <c r="M24" s="45"/>
-      <c r="N24" s="45"/>
-      <c r="O24" s="45"/>
-      <c r="P24" s="45"/>
-      <c r="Q24" s="45"/>
-      <c r="S24" s="42"/>
-      <c r="T24" s="42"/>
-      <c r="U24" s="42"/>
-      <c r="W24" s="41"/>
-      <c r="X24" s="41"/>
+      <c r="E24" s="47"/>
+      <c r="F24" s="50"/>
+      <c r="G24" s="50"/>
+      <c r="H24" s="50"/>
+      <c r="I24" s="50"/>
+      <c r="J24" s="50"/>
+      <c r="K24" s="50"/>
+      <c r="L24" s="50"/>
+      <c r="M24" s="50"/>
+      <c r="N24" s="50"/>
+      <c r="O24" s="50"/>
+      <c r="P24" s="50"/>
+      <c r="Q24" s="50"/>
+      <c r="S24" s="47"/>
+      <c r="T24" s="47"/>
+      <c r="U24" s="47"/>
+      <c r="W24" s="51"/>
+      <c r="X24" s="51"/>
     </row>
     <row r="25" spans="5:24" x14ac:dyDescent="0.25">
-      <c r="E25" s="42"/>
-      <c r="F25" s="45"/>
-      <c r="G25" s="45"/>
-      <c r="H25" s="45"/>
-      <c r="I25" s="45"/>
-      <c r="J25" s="45"/>
-      <c r="K25" s="45"/>
-      <c r="L25" s="45"/>
-      <c r="M25" s="45"/>
-      <c r="N25" s="45"/>
-      <c r="O25" s="45"/>
-      <c r="P25" s="45"/>
-      <c r="Q25" s="45"/>
-      <c r="S25" s="42"/>
-      <c r="T25" s="42"/>
-      <c r="U25" s="42"/>
-      <c r="W25" s="41"/>
-      <c r="X25" s="41"/>
+      <c r="E25" s="47"/>
+      <c r="F25" s="50"/>
+      <c r="G25" s="50"/>
+      <c r="H25" s="50"/>
+      <c r="I25" s="50"/>
+      <c r="J25" s="50"/>
+      <c r="K25" s="50"/>
+      <c r="L25" s="50"/>
+      <c r="M25" s="50"/>
+      <c r="N25" s="50"/>
+      <c r="O25" s="50"/>
+      <c r="P25" s="50"/>
+      <c r="Q25" s="50"/>
+      <c r="S25" s="47"/>
+      <c r="T25" s="47"/>
+      <c r="U25" s="47"/>
+      <c r="W25" s="51"/>
+      <c r="X25" s="51"/>
     </row>
     <row r="26" spans="5:24" x14ac:dyDescent="0.25">
-      <c r="E26" s="42"/>
-      <c r="F26" s="45"/>
-      <c r="G26" s="45"/>
-      <c r="H26" s="45"/>
-      <c r="I26" s="45"/>
-      <c r="J26" s="45"/>
-      <c r="K26" s="45"/>
-      <c r="L26" s="45"/>
-      <c r="M26" s="45"/>
-      <c r="N26" s="45"/>
-      <c r="O26" s="45"/>
-      <c r="P26" s="45"/>
-      <c r="Q26" s="45"/>
-      <c r="S26" s="42"/>
-      <c r="T26" s="42"/>
-      <c r="U26" s="42"/>
-      <c r="W26" s="41"/>
-      <c r="X26" s="41"/>
+      <c r="E26" s="47"/>
+      <c r="F26" s="50"/>
+      <c r="G26" s="50"/>
+      <c r="H26" s="50"/>
+      <c r="I26" s="50"/>
+      <c r="J26" s="50"/>
+      <c r="K26" s="50"/>
+      <c r="L26" s="50"/>
+      <c r="M26" s="50"/>
+      <c r="N26" s="50"/>
+      <c r="O26" s="50"/>
+      <c r="P26" s="50"/>
+      <c r="Q26" s="50"/>
+      <c r="S26" s="47"/>
+      <c r="T26" s="47"/>
+      <c r="U26" s="47"/>
+      <c r="W26" s="51"/>
+      <c r="X26" s="51"/>
     </row>
     <row r="27" spans="5:24" x14ac:dyDescent="0.25">
-      <c r="E27" s="42"/>
-      <c r="F27" s="45"/>
-      <c r="G27" s="45"/>
-      <c r="H27" s="45"/>
-      <c r="I27" s="45"/>
-      <c r="J27" s="45"/>
-      <c r="K27" s="45"/>
-      <c r="L27" s="45"/>
-      <c r="M27" s="45"/>
-      <c r="N27" s="45"/>
-      <c r="O27" s="45"/>
-      <c r="P27" s="45"/>
-      <c r="Q27" s="45"/>
-      <c r="S27" s="42"/>
-      <c r="T27" s="42"/>
-      <c r="U27" s="42"/>
-      <c r="W27" s="41"/>
-      <c r="X27" s="41"/>
+      <c r="E27" s="47"/>
+      <c r="F27" s="50"/>
+      <c r="G27" s="50"/>
+      <c r="H27" s="50"/>
+      <c r="I27" s="50"/>
+      <c r="J27" s="50"/>
+      <c r="K27" s="50"/>
+      <c r="L27" s="50"/>
+      <c r="M27" s="50"/>
+      <c r="N27" s="50"/>
+      <c r="O27" s="50"/>
+      <c r="P27" s="50"/>
+      <c r="Q27" s="50"/>
+      <c r="S27" s="47"/>
+      <c r="T27" s="47"/>
+      <c r="U27" s="47"/>
+      <c r="W27" s="51"/>
+      <c r="X27" s="51"/>
     </row>
     <row r="28" spans="5:24" x14ac:dyDescent="0.25">
-      <c r="E28" s="42"/>
-      <c r="F28" s="45"/>
-      <c r="G28" s="45"/>
-      <c r="H28" s="45"/>
-      <c r="I28" s="45"/>
-      <c r="J28" s="45"/>
-      <c r="K28" s="45"/>
-      <c r="L28" s="45"/>
-      <c r="M28" s="45"/>
-      <c r="N28" s="45"/>
-      <c r="O28" s="45"/>
-      <c r="P28" s="45"/>
-      <c r="Q28" s="45"/>
-      <c r="S28" s="42"/>
-      <c r="T28" s="42"/>
-      <c r="U28" s="42"/>
-      <c r="W28" s="41"/>
-      <c r="X28" s="41"/>
+      <c r="E28" s="47"/>
+      <c r="F28" s="50"/>
+      <c r="G28" s="50"/>
+      <c r="H28" s="50"/>
+      <c r="I28" s="50"/>
+      <c r="J28" s="50"/>
+      <c r="K28" s="50"/>
+      <c r="L28" s="50"/>
+      <c r="M28" s="50"/>
+      <c r="N28" s="50"/>
+      <c r="O28" s="50"/>
+      <c r="P28" s="50"/>
+      <c r="Q28" s="50"/>
+      <c r="S28" s="47"/>
+      <c r="T28" s="47"/>
+      <c r="U28" s="47"/>
+      <c r="W28" s="51"/>
+      <c r="X28" s="51"/>
     </row>
     <row r="29" spans="5:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E29" s="42">
+      <c r="E29" s="47">
         <v>4</v>
       </c>
-      <c r="F29" s="44" t="s">
+      <c r="F29" s="49" t="s">
         <v>54</v>
       </c>
-      <c r="G29" s="45"/>
-      <c r="H29" s="45"/>
-      <c r="I29" s="45"/>
-      <c r="J29" s="45"/>
-      <c r="K29" s="45"/>
-      <c r="L29" s="45"/>
-      <c r="M29" s="45"/>
-      <c r="N29" s="45"/>
-      <c r="O29" s="45"/>
-      <c r="P29" s="45"/>
-      <c r="Q29" s="45"/>
-      <c r="S29" s="42" t="s">
+      <c r="G29" s="50"/>
+      <c r="H29" s="50"/>
+      <c r="I29" s="50"/>
+      <c r="J29" s="50"/>
+      <c r="K29" s="50"/>
+      <c r="L29" s="50"/>
+      <c r="M29" s="50"/>
+      <c r="N29" s="50"/>
+      <c r="O29" s="50"/>
+      <c r="P29" s="50"/>
+      <c r="Q29" s="50"/>
+      <c r="S29" s="47" t="s">
         <v>58</v>
       </c>
-      <c r="T29" s="42"/>
-      <c r="U29" s="42"/>
-      <c r="W29" s="41" t="s">
+      <c r="T29" s="47"/>
+      <c r="U29" s="47"/>
+      <c r="W29" s="51" t="s">
         <v>65</v>
       </c>
-      <c r="X29" s="41"/>
+      <c r="X29" s="51"/>
     </row>
     <row r="30" spans="5:24" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E30" s="42"/>
-      <c r="F30" s="45"/>
-      <c r="G30" s="45"/>
-      <c r="H30" s="45"/>
-      <c r="I30" s="45"/>
-      <c r="J30" s="45"/>
-      <c r="K30" s="45"/>
-      <c r="L30" s="45"/>
-      <c r="M30" s="45"/>
-      <c r="N30" s="45"/>
-      <c r="O30" s="45"/>
-      <c r="P30" s="45"/>
-      <c r="Q30" s="45"/>
-      <c r="S30" s="42"/>
-      <c r="T30" s="42"/>
-      <c r="U30" s="42"/>
-      <c r="W30" s="41"/>
-      <c r="X30" s="41"/>
+      <c r="E30" s="47"/>
+      <c r="F30" s="50"/>
+      <c r="G30" s="50"/>
+      <c r="H30" s="50"/>
+      <c r="I30" s="50"/>
+      <c r="J30" s="50"/>
+      <c r="K30" s="50"/>
+      <c r="L30" s="50"/>
+      <c r="M30" s="50"/>
+      <c r="N30" s="50"/>
+      <c r="O30" s="50"/>
+      <c r="P30" s="50"/>
+      <c r="Q30" s="50"/>
+      <c r="S30" s="47"/>
+      <c r="T30" s="47"/>
+      <c r="U30" s="47"/>
+      <c r="W30" s="51"/>
+      <c r="X30" s="51"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="W3:X7"/>
+    <mergeCell ref="W8:X9"/>
+    <mergeCell ref="W29:X30"/>
+    <mergeCell ref="W10:W28"/>
+    <mergeCell ref="X10:X28"/>
     <mergeCell ref="S3:U7"/>
     <mergeCell ref="S8:U9"/>
     <mergeCell ref="S10:U28"/>
@@ -3615,11 +3763,6 @@
     <mergeCell ref="F10:H28"/>
     <mergeCell ref="I10:Q28"/>
     <mergeCell ref="F29:Q30"/>
-    <mergeCell ref="W3:X7"/>
-    <mergeCell ref="W8:X9"/>
-    <mergeCell ref="W29:X30"/>
-    <mergeCell ref="W10:W28"/>
-    <mergeCell ref="X10:X28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
penilaian migration kelas XII RPL 2
</commit_message>
<xml_diff>
--- a/XIIRPL2(❁´◡`❁)(❁´◡`❁)(❁´◡`❁)(u‿ฺu✿ฺ)/DATA PRAKTIK XII RPl 2.xlsx
+++ b/XIIRPL2(❁´◡`❁)(❁´◡`❁)(❁´◡`❁)(u‿ฺu✿ฺ)/DATA PRAKTIK XII RPl 2.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AdeSetiyawan)(✿◡‿◡)(✿◡‿◡)\XIIRPL2(❁´◡`❁)(❁´◡`❁)(❁´◡`❁)(u‿ฺu✿ฺ)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12A6920E-380D-47FF-AF7E-C9CFC06DC677}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B29C6C9-4862-4374-84FA-92A132247505}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7A470BEC-FF9B-4C58-B3A9-6A89F2B6EB46}"/>
   </bookViews>
   <sheets>
     <sheet name="Nilai All" sheetId="1" r:id="rId1"/>
-    <sheet name="Sesi 1" sheetId="3" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
+    <sheet name="Soal Migration" sheetId="5" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId3"/>
+    <sheet name="Sesi 1" sheetId="3" r:id="rId4"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Nilai All'!$E$1:$G$38</definedName>
@@ -30,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="106">
   <si>
     <t xml:space="preserve">Nama </t>
   </si>
@@ -241,12 +243,6 @@
 100 point</t>
   </si>
   <si>
-    <t>✓</t>
-  </si>
-  <si>
-    <t>🚫</t>
-  </si>
-  <si>
     <t>SOAL sesi 1</t>
   </si>
   <si>
@@ -296,6 +292,69 @@
   </si>
   <si>
     <t>Chat Dengan Kami</t>
+  </si>
+  <si>
+    <t>&gt; 71</t>
+  </si>
+  <si>
+    <t>&lt;71</t>
+  </si>
+  <si>
+    <t xml:space="preserve">migrate </t>
+  </si>
+  <si>
+    <t>class array</t>
+  </si>
+  <si>
+    <t>25.01.2023</t>
+  </si>
+  <si>
+    <t>25,01,23 (sakit)</t>
+  </si>
+  <si>
+    <t>25,01,23 Ijin Kelas Karir</t>
+  </si>
+  <si>
+    <t xml:space="preserve">letak migration </t>
+  </si>
+  <si>
+    <t>-database -&gt; migrations</t>
+  </si>
+  <si>
+    <t>Cara membuat migration:</t>
+  </si>
+  <si>
+    <t>- php artisan make:migration create_namatable(s)_table [enter]</t>
+  </si>
+  <si>
+    <t>Cara mengeksekusi migration :</t>
+  </si>
+  <si>
+    <t>cara menghapus semua migration :</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cara untuk menghapus 3 kali migration : </t>
+  </si>
+  <si>
+    <t>- php artisan migrate:rollback dilakukan sebanyak 3 kali</t>
+  </si>
+  <si>
+    <t>- INGAT TIDAK BOLEH ADA NAMA MIGRATION YANG SAMA !!!!</t>
+  </si>
+  <si>
+    <t>=====================</t>
+  </si>
+  <si>
+    <t>=  tb_ukuranbarang  =</t>
+  </si>
+  <si>
+    <t>=</t>
+  </si>
+  <si>
+    <t>keterangan (text)</t>
+  </si>
+  <si>
+    <t>=  tbjual_kaos_bola  =</t>
   </si>
 </sst>
 </file>
@@ -303,7 +362,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="0&quot;%&quot;"/>
+    <numFmt numFmtId="164" formatCode="0&quot;%&quot;"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -359,7 +418,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -402,6 +461,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="21">
     <border>
@@ -740,6 +805,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -800,6 +874,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -812,19 +889,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1132,7 +1201,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1142,15 +1211,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E8966E4-2275-4E9F-82CA-974F40DBA593}">
   <dimension ref="B1:T1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
-      <selection activeCell="E2" sqref="E2"/>
-      <selection pane="topRight" activeCell="L17" sqref="L17"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T17" sqref="T17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="9.140625" style="2"/>
+    <col min="2" max="2" width="21.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.28515625" customWidth="1"/>
     <col min="4" max="4" width="6.5703125" style="2" customWidth="1"/>
     <col min="5" max="5" width="15.28515625" customWidth="1"/>
@@ -1165,51 +1232,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="C1" s="34" t="s">
+      <c r="C1" s="37" t="s">
         <v>57</v>
       </c>
-      <c r="D1" s="35" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="38" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" s="38" t="s">
+      <c r="D1" s="38" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="48" t="s">
+      <c r="G1" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="50" t="s">
+      <c r="H1" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="50"/>
-      <c r="J1" s="50"/>
-      <c r="K1" s="46" t="s">
+      <c r="I1" s="53"/>
+      <c r="J1" s="53"/>
+      <c r="K1" s="49" t="s">
         <v>49</v>
       </c>
-      <c r="L1" s="47"/>
-      <c r="M1" s="47"/>
-      <c r="N1" s="47"/>
-      <c r="O1" s="47"/>
-      <c r="P1" s="47"/>
-      <c r="Q1" s="41" t="s">
+      <c r="L1" s="50"/>
+      <c r="M1" s="50"/>
+      <c r="N1" s="50"/>
+      <c r="O1" s="50"/>
+      <c r="P1" s="50"/>
+      <c r="Q1" s="44" t="s">
         <v>66</v>
       </c>
-      <c r="R1" s="41" t="s">
+      <c r="R1" s="44" t="s">
         <v>67</v>
       </c>
-      <c r="S1" s="32" t="s">
-        <v>78</v>
-      </c>
-      <c r="T1" s="33"/>
-    </row>
-    <row r="2" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="C2" s="34"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="49"/>
+      <c r="S1" s="35" t="s">
+        <v>76</v>
+      </c>
+      <c r="T1" s="36"/>
+    </row>
+    <row r="2" spans="2:20" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C2" s="37"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="52"/>
       <c r="H2" s="15" t="s">
         <v>10</v>
       </c>
@@ -1219,10 +1286,10 @@
       <c r="J2" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="9" t="s">
+      <c r="K2" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="L2" s="9" t="s">
+      <c r="L2" s="60" t="s">
         <v>5</v>
       </c>
       <c r="M2" s="9" t="s">
@@ -1237,43 +1304,42 @@
       <c r="P2" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="Q2" s="42"/>
-      <c r="R2" s="41"/>
-      <c r="S2" s="32"/>
-      <c r="T2" s="33"/>
+      <c r="Q2" s="45"/>
+      <c r="R2" s="44"/>
+      <c r="S2" s="35"/>
+      <c r="T2" s="36"/>
     </row>
     <row r="3" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="34"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="40"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
       <c r="G3" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="H3" s="43" t="s">
+      <c r="H3" s="46" t="s">
         <v>47</v>
       </c>
-      <c r="I3" s="44"/>
-      <c r="J3" s="45"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
+      <c r="I3" s="47"/>
+      <c r="J3" s="48"/>
+      <c r="K3" s="61" t="s">
+        <v>89</v>
+      </c>
+      <c r="L3" s="61"/>
       <c r="M3" s="8"/>
       <c r="N3" s="8"/>
       <c r="O3" s="8"/>
       <c r="P3" s="13"/>
-      <c r="Q3" s="42"/>
-      <c r="R3" s="41"/>
+      <c r="Q3" s="45"/>
+      <c r="R3" s="44"/>
       <c r="S3" s="26" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="T3" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B4" s="2" t="s">
-        <v>68</v>
-      </c>
       <c r="C4" s="3">
         <v>1</v>
       </c>
@@ -1285,7 +1351,7 @@
       </c>
       <c r="F4" s="6">
         <f t="shared" ref="F4:F38" si="0">((SUM(G4:P4)*10)*70%)+(AVERAGE(Q4:R4)*30%)</f>
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="G4" s="10">
         <v>1</v>
@@ -1299,7 +1365,9 @@
       <c r="J4" s="10">
         <v>0.75</v>
       </c>
-      <c r="K4" s="10"/>
+      <c r="K4" s="10">
+        <v>1</v>
+      </c>
       <c r="L4" s="10"/>
       <c r="M4" s="10"/>
       <c r="N4" s="10"/>
@@ -1331,7 +1399,7 @@
       </c>
       <c r="F5" s="6">
         <f t="shared" si="0"/>
-        <v>41.25</v>
+        <v>48.25</v>
       </c>
       <c r="G5" s="10">
         <v>1</v>
@@ -1345,7 +1413,9 @@
       <c r="J5" s="10">
         <v>1</v>
       </c>
-      <c r="K5" s="10"/>
+      <c r="K5" s="10">
+        <v>1</v>
+      </c>
       <c r="L5" s="10"/>
       <c r="M5" s="10"/>
       <c r="N5" s="10"/>
@@ -1366,6 +1436,9 @@
       </c>
     </row>
     <row r="6" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="C6" s="22">
         <v>1</v>
       </c>
@@ -1391,16 +1464,15 @@
       <c r="J6" s="10">
         <v>0.75</v>
       </c>
-      <c r="K6" s="10"/>
+      <c r="K6" s="10">
+        <v>0</v>
+      </c>
       <c r="L6" s="10"/>
       <c r="M6" s="10"/>
       <c r="N6" s="10"/>
       <c r="O6" s="10"/>
       <c r="P6" s="14"/>
-      <c r="Q6" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="Q6" s="5"/>
       <c r="R6" s="5">
         <v>0</v>
       </c>
@@ -1423,7 +1495,7 @@
       </c>
       <c r="F7" s="6">
         <f t="shared" si="0"/>
-        <v>41.25</v>
+        <v>48.25</v>
       </c>
       <c r="G7" s="10">
         <v>1</v>
@@ -1437,7 +1509,9 @@
       <c r="J7" s="10">
         <v>1</v>
       </c>
-      <c r="K7" s="10"/>
+      <c r="K7" s="10">
+        <v>1</v>
+      </c>
       <c r="L7" s="10"/>
       <c r="M7" s="10"/>
       <c r="N7" s="10"/>
@@ -1458,9 +1532,6 @@
       </c>
     </row>
     <row r="8" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B8" s="2" t="s">
-        <v>68</v>
-      </c>
       <c r="C8" s="3">
         <v>1</v>
       </c>
@@ -1472,7 +1543,7 @@
       </c>
       <c r="F8" s="6">
         <f>((SUM(G8:P8)*10)*70%)+(AVERAGE(Q8:R8)*30%)</f>
-        <v>39.25</v>
+        <v>46.25</v>
       </c>
       <c r="G8" s="10">
         <v>1</v>
@@ -1486,7 +1557,9 @@
       <c r="J8" s="10">
         <v>1</v>
       </c>
-      <c r="K8" s="10"/>
+      <c r="K8" s="10">
+        <v>1</v>
+      </c>
       <c r="L8" s="10"/>
       <c r="M8" s="10"/>
       <c r="N8" s="10"/>
@@ -1531,9 +1604,7 @@
       <c r="N9" s="10"/>
       <c r="O9" s="10"/>
       <c r="P9" s="14"/>
-      <c r="Q9" s="29">
-        <v>0</v>
-      </c>
+      <c r="Q9" s="29"/>
       <c r="R9" s="29">
         <v>0</v>
       </c>
@@ -1543,9 +1614,6 @@
       <c r="T9" s="28"/>
     </row>
     <row r="10" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B10" s="2" t="s">
-        <v>68</v>
-      </c>
       <c r="C10" s="3">
         <v>1</v>
       </c>
@@ -1557,7 +1625,7 @@
       </c>
       <c r="F10" s="6">
         <f t="shared" si="0"/>
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="G10" s="10">
         <v>1</v>
@@ -1571,7 +1639,9 @@
       <c r="J10" s="10">
         <v>1</v>
       </c>
-      <c r="K10" s="10"/>
+      <c r="K10" s="10">
+        <v>1</v>
+      </c>
       <c r="L10" s="10"/>
       <c r="M10" s="10"/>
       <c r="N10" s="10"/>
@@ -1603,7 +1673,7 @@
       </c>
       <c r="F11" s="6">
         <f t="shared" si="0"/>
-        <v>33.75</v>
+        <v>40.75</v>
       </c>
       <c r="G11" s="10">
         <v>1</v>
@@ -1617,7 +1687,9 @@
       <c r="J11" s="10">
         <v>1</v>
       </c>
-      <c r="K11" s="10"/>
+      <c r="K11" s="10">
+        <v>1</v>
+      </c>
       <c r="L11" s="10"/>
       <c r="M11" s="10"/>
       <c r="N11" s="10"/>
@@ -1638,6 +1710,9 @@
       </c>
     </row>
     <row r="12" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B12" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="C12" s="22">
         <v>1</v>
       </c>
@@ -1663,7 +1738,9 @@
       <c r="J12" s="10">
         <v>0.75</v>
       </c>
-      <c r="K12" s="10"/>
+      <c r="K12" s="10">
+        <v>0</v>
+      </c>
       <c r="L12" s="10"/>
       <c r="M12" s="10"/>
       <c r="N12" s="10"/>
@@ -1695,7 +1772,7 @@
       </c>
       <c r="F13" s="6">
         <f t="shared" si="0"/>
-        <v>40.5</v>
+        <v>47.5</v>
       </c>
       <c r="G13" s="10">
         <v>1</v>
@@ -1709,7 +1786,9 @@
       <c r="J13" s="10">
         <v>1</v>
       </c>
-      <c r="K13" s="10"/>
+      <c r="K13" s="10">
+        <v>1</v>
+      </c>
       <c r="L13" s="10"/>
       <c r="M13" s="10"/>
       <c r="N13" s="10"/>
@@ -1730,9 +1809,6 @@
       </c>
     </row>
     <row r="14" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B14" s="2" t="s">
-        <v>68</v>
-      </c>
       <c r="C14" s="3">
         <v>1</v>
       </c>
@@ -1744,7 +1820,7 @@
       </c>
       <c r="F14" s="6">
         <f t="shared" si="0"/>
-        <v>36.75</v>
+        <v>43.75</v>
       </c>
       <c r="G14" s="10">
         <v>1</v>
@@ -1758,7 +1834,9 @@
       <c r="J14" s="10">
         <v>1</v>
       </c>
-      <c r="K14" s="10"/>
+      <c r="K14" s="10">
+        <v>1</v>
+      </c>
       <c r="L14" s="10"/>
       <c r="M14" s="10"/>
       <c r="N14" s="10"/>
@@ -1790,7 +1868,7 @@
       </c>
       <c r="F15" s="6">
         <f t="shared" si="0"/>
-        <v>38.25</v>
+        <v>45.25</v>
       </c>
       <c r="G15" s="10">
         <v>1</v>
@@ -1804,7 +1882,9 @@
       <c r="J15" s="10">
         <v>1</v>
       </c>
-      <c r="K15" s="10"/>
+      <c r="K15" s="10">
+        <v>1</v>
+      </c>
       <c r="L15" s="10"/>
       <c r="M15" s="10"/>
       <c r="N15" s="10"/>
@@ -1826,7 +1906,7 @@
     </row>
     <row r="16" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
-        <v>68</v>
+        <v>90</v>
       </c>
       <c r="C16" s="3">
         <v>1</v>
@@ -1853,7 +1933,9 @@
       <c r="J16" s="10">
         <v>1</v>
       </c>
-      <c r="K16" s="10"/>
+      <c r="K16" s="10">
+        <v>0</v>
+      </c>
       <c r="L16" s="10"/>
       <c r="M16" s="10"/>
       <c r="N16" s="10"/>
@@ -1885,7 +1967,7 @@
       </c>
       <c r="F17" s="6">
         <f t="shared" si="0"/>
-        <v>40.950000000000003</v>
+        <v>47.95</v>
       </c>
       <c r="G17" s="10">
         <v>1</v>
@@ -1899,7 +1981,9 @@
       <c r="J17" s="10">
         <v>1</v>
       </c>
-      <c r="K17" s="10"/>
+      <c r="K17" s="10">
+        <v>1</v>
+      </c>
       <c r="L17" s="10"/>
       <c r="M17" s="10"/>
       <c r="N17" s="10"/>
@@ -1920,6 +2004,9 @@
       </c>
     </row>
     <row r="18" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B18" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="C18" s="22">
         <v>1</v>
       </c>
@@ -1945,7 +2032,9 @@
       <c r="J18" s="10">
         <v>0.75</v>
       </c>
-      <c r="K18" s="10"/>
+      <c r="K18" s="10">
+        <v>0</v>
+      </c>
       <c r="L18" s="10"/>
       <c r="M18" s="10"/>
       <c r="N18" s="10"/>
@@ -1977,7 +2066,7 @@
       </c>
       <c r="F19" s="6">
         <f t="shared" si="0"/>
-        <v>40.75</v>
+        <v>47.75</v>
       </c>
       <c r="G19" s="10">
         <v>1</v>
@@ -1991,7 +2080,9 @@
       <c r="J19" s="10">
         <v>1</v>
       </c>
-      <c r="K19" s="10"/>
+      <c r="K19" s="10">
+        <v>1</v>
+      </c>
       <c r="L19" s="10"/>
       <c r="M19" s="10"/>
       <c r="N19" s="10"/>
@@ -2012,6 +2103,9 @@
       </c>
     </row>
     <row r="20" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B20" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="C20" s="22">
         <v>1</v>
       </c>
@@ -2037,16 +2131,15 @@
       <c r="J20" s="10">
         <v>0.75</v>
       </c>
-      <c r="K20" s="10"/>
+      <c r="K20" s="10">
+        <v>0</v>
+      </c>
       <c r="L20" s="10"/>
       <c r="M20" s="10"/>
       <c r="N20" s="10"/>
       <c r="O20" s="10"/>
       <c r="P20" s="14"/>
-      <c r="Q20" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="Q20" s="5"/>
       <c r="R20" s="5">
         <v>0</v>
       </c>
@@ -2069,7 +2162,7 @@
       </c>
       <c r="F21" s="6">
         <f t="shared" si="0"/>
-        <v>36.75</v>
+        <v>43.75</v>
       </c>
       <c r="G21" s="10">
         <v>1</v>
@@ -2083,7 +2176,9 @@
       <c r="J21" s="10">
         <v>1</v>
       </c>
-      <c r="K21" s="10"/>
+      <c r="K21" s="10">
+        <v>1</v>
+      </c>
       <c r="L21" s="10"/>
       <c r="M21" s="10"/>
       <c r="N21" s="10"/>
@@ -2104,9 +2199,6 @@
       </c>
     </row>
     <row r="22" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B22" s="2" t="s">
-        <v>68</v>
-      </c>
       <c r="C22" s="3">
         <v>1</v>
       </c>
@@ -2118,7 +2210,7 @@
       </c>
       <c r="F22" s="6">
         <f t="shared" si="0"/>
-        <v>34.5</v>
+        <v>38</v>
       </c>
       <c r="G22" s="10">
         <v>1</v>
@@ -2132,7 +2224,9 @@
       <c r="J22" s="10">
         <v>1</v>
       </c>
-      <c r="K22" s="10"/>
+      <c r="K22" s="10">
+        <v>0.5</v>
+      </c>
       <c r="L22" s="10"/>
       <c r="M22" s="10"/>
       <c r="N22" s="10"/>
@@ -2153,6 +2247,9 @@
       </c>
     </row>
     <row r="23" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B23" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="C23" s="22">
         <v>2</v>
       </c>
@@ -2178,7 +2275,9 @@
       <c r="J23" s="10">
         <v>0.75</v>
       </c>
-      <c r="K23" s="10"/>
+      <c r="K23" s="10">
+        <v>0</v>
+      </c>
       <c r="L23" s="10"/>
       <c r="M23" s="10"/>
       <c r="N23" s="10"/>
@@ -2199,9 +2298,6 @@
       </c>
     </row>
     <row r="24" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B24" s="2" t="s">
-        <v>68</v>
-      </c>
       <c r="C24" s="3">
         <v>1</v>
       </c>
@@ -2213,7 +2309,7 @@
       </c>
       <c r="F24" s="6">
         <f t="shared" si="0"/>
-        <v>32.75</v>
+        <v>38</v>
       </c>
       <c r="G24" s="10">
         <v>1</v>
@@ -2227,7 +2323,9 @@
       <c r="J24" s="10">
         <v>1</v>
       </c>
-      <c r="K24" s="10"/>
+      <c r="K24" s="10">
+        <v>0.75</v>
+      </c>
       <c r="L24" s="10"/>
       <c r="M24" s="10"/>
       <c r="N24" s="10"/>
@@ -2259,7 +2357,7 @@
       </c>
       <c r="F25" s="6">
         <f t="shared" si="0"/>
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="G25" s="10">
         <v>1</v>
@@ -2273,7 +2371,9 @@
       <c r="J25" s="10">
         <v>1</v>
       </c>
-      <c r="K25" s="10"/>
+      <c r="K25" s="10">
+        <v>1</v>
+      </c>
       <c r="L25" s="10"/>
       <c r="M25" s="10"/>
       <c r="N25" s="10"/>
@@ -2294,9 +2394,6 @@
       </c>
     </row>
     <row r="26" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B26" s="2" t="s">
-        <v>68</v>
-      </c>
       <c r="C26" s="3">
         <v>1</v>
       </c>
@@ -2308,7 +2405,7 @@
       </c>
       <c r="F26" s="6">
         <f t="shared" si="0"/>
-        <v>30.5</v>
+        <v>34</v>
       </c>
       <c r="G26" s="10">
         <v>1</v>
@@ -2322,7 +2419,9 @@
       <c r="J26" s="10">
         <v>1</v>
       </c>
-      <c r="K26" s="10"/>
+      <c r="K26" s="10">
+        <v>0.5</v>
+      </c>
       <c r="L26" s="10"/>
       <c r="M26" s="10"/>
       <c r="N26" s="10"/>
@@ -2354,7 +2453,7 @@
       </c>
       <c r="F27" s="6">
         <f t="shared" si="0"/>
-        <v>36.75</v>
+        <v>43.75</v>
       </c>
       <c r="G27" s="10">
         <v>1</v>
@@ -2368,7 +2467,9 @@
       <c r="J27" s="10">
         <v>1</v>
       </c>
-      <c r="K27" s="10"/>
+      <c r="K27" s="10">
+        <v>1</v>
+      </c>
       <c r="L27" s="10"/>
       <c r="M27" s="10"/>
       <c r="N27" s="10"/>
@@ -2389,9 +2490,6 @@
       </c>
     </row>
     <row r="28" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B28" s="2" t="s">
-        <v>68</v>
-      </c>
       <c r="C28" s="3">
         <v>1</v>
       </c>
@@ -2403,7 +2501,7 @@
       </c>
       <c r="F28" s="6">
         <f t="shared" si="0"/>
-        <v>36.75</v>
+        <v>43.75</v>
       </c>
       <c r="G28" s="10">
         <v>1</v>
@@ -2417,7 +2515,9 @@
       <c r="J28" s="10">
         <v>1</v>
       </c>
-      <c r="K28" s="10"/>
+      <c r="K28" s="10">
+        <v>1</v>
+      </c>
       <c r="L28" s="10"/>
       <c r="M28" s="10"/>
       <c r="N28" s="10"/>
@@ -2449,7 +2549,7 @@
       </c>
       <c r="F29" s="6">
         <f t="shared" si="0"/>
-        <v>34.5</v>
+        <v>39.75</v>
       </c>
       <c r="G29" s="11">
         <v>1</v>
@@ -2463,7 +2563,9 @@
       <c r="J29" s="10">
         <v>1</v>
       </c>
-      <c r="K29" s="10"/>
+      <c r="K29" s="10">
+        <v>0.75</v>
+      </c>
       <c r="L29" s="10"/>
       <c r="M29" s="10"/>
       <c r="N29" s="10"/>
@@ -2484,9 +2586,6 @@
       </c>
     </row>
     <row r="30" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B30" s="2" t="s">
-        <v>68</v>
-      </c>
       <c r="C30" s="3">
         <v>1</v>
       </c>
@@ -2498,7 +2597,7 @@
       </c>
       <c r="F30" s="6">
         <f t="shared" si="0"/>
-        <v>40.75</v>
+        <v>47.75</v>
       </c>
       <c r="G30" s="10">
         <v>1</v>
@@ -2512,7 +2611,9 @@
       <c r="J30" s="10">
         <v>1</v>
       </c>
-      <c r="K30" s="10"/>
+      <c r="K30" s="10">
+        <v>1</v>
+      </c>
       <c r="L30" s="10"/>
       <c r="M30" s="10"/>
       <c r="N30" s="10"/>
@@ -2544,7 +2645,7 @@
       </c>
       <c r="F31" s="6">
         <f t="shared" si="0"/>
-        <v>41.5</v>
+        <v>48.5</v>
       </c>
       <c r="G31" s="10">
         <v>1</v>
@@ -2558,7 +2659,9 @@
       <c r="J31" s="10">
         <v>1</v>
       </c>
-      <c r="K31" s="10"/>
+      <c r="K31" s="10">
+        <v>1</v>
+      </c>
       <c r="L31" s="10"/>
       <c r="M31" s="10"/>
       <c r="N31" s="10"/>
@@ -2579,9 +2682,6 @@
       </c>
     </row>
     <row r="32" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B32" s="2" t="s">
-        <v>68</v>
-      </c>
       <c r="C32" s="3">
         <v>1</v>
       </c>
@@ -2593,7 +2693,7 @@
       </c>
       <c r="F32" s="6">
         <f t="shared" si="0"/>
-        <v>38.5</v>
+        <v>45.5</v>
       </c>
       <c r="G32" s="10">
         <v>1</v>
@@ -2607,7 +2707,9 @@
       <c r="J32" s="10">
         <v>1</v>
       </c>
-      <c r="K32" s="10"/>
+      <c r="K32" s="10">
+        <v>1</v>
+      </c>
       <c r="L32" s="10"/>
       <c r="M32" s="10"/>
       <c r="N32" s="10"/>
@@ -2639,7 +2741,7 @@
       </c>
       <c r="F33" s="6">
         <f t="shared" si="0"/>
-        <v>42.25</v>
+        <v>49.25</v>
       </c>
       <c r="G33" s="10">
         <v>1</v>
@@ -2653,7 +2755,9 @@
       <c r="J33" s="10">
         <v>1</v>
       </c>
-      <c r="K33" s="10"/>
+      <c r="K33" s="10">
+        <v>1</v>
+      </c>
       <c r="L33" s="10"/>
       <c r="M33" s="10"/>
       <c r="N33" s="10"/>
@@ -2674,9 +2778,6 @@
       </c>
     </row>
     <row r="34" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B34" s="2" t="s">
-        <v>68</v>
-      </c>
       <c r="C34" s="3">
         <v>1</v>
       </c>
@@ -2688,7 +2789,7 @@
       </c>
       <c r="F34" s="6">
         <f t="shared" si="0"/>
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="G34" s="10">
         <v>1</v>
@@ -2702,7 +2803,9 @@
       <c r="J34" s="10">
         <v>1</v>
       </c>
-      <c r="K34" s="10"/>
+      <c r="K34" s="10">
+        <v>1</v>
+      </c>
       <c r="L34" s="10"/>
       <c r="M34" s="10"/>
       <c r="N34" s="10"/>
@@ -2734,7 +2837,7 @@
       </c>
       <c r="F35" s="6">
         <f t="shared" si="0"/>
-        <v>34.5</v>
+        <v>39.75</v>
       </c>
       <c r="G35" s="10">
         <v>1</v>
@@ -2748,7 +2851,9 @@
       <c r="J35" s="10">
         <v>1</v>
       </c>
-      <c r="K35" s="10"/>
+      <c r="K35" s="10">
+        <v>0.75</v>
+      </c>
       <c r="L35" s="10"/>
       <c r="M35" s="10"/>
       <c r="N35" s="10"/>
@@ -2769,9 +2874,6 @@
       </c>
     </row>
     <row r="36" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B36" s="2" t="s">
-        <v>69</v>
-      </c>
       <c r="C36" s="3">
         <v>1</v>
       </c>
@@ -2783,7 +2885,7 @@
       </c>
       <c r="F36" s="6">
         <f t="shared" si="0"/>
-        <v>26.25</v>
+        <v>33.25</v>
       </c>
       <c r="G36" s="10">
         <v>1</v>
@@ -2797,16 +2899,15 @@
       <c r="J36" s="10">
         <v>1</v>
       </c>
-      <c r="K36" s="10"/>
+      <c r="K36" s="10">
+        <v>1</v>
+      </c>
       <c r="L36" s="10"/>
       <c r="M36" s="10"/>
       <c r="N36" s="10"/>
       <c r="O36" s="10"/>
       <c r="P36" s="14"/>
-      <c r="Q36" s="5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="Q36" s="5"/>
       <c r="R36" s="5">
         <v>0</v>
       </c>
@@ -2829,7 +2930,7 @@
       </c>
       <c r="F37" s="6">
         <f t="shared" si="0"/>
-        <v>38.5</v>
+        <v>43.75</v>
       </c>
       <c r="G37" s="10">
         <v>1</v>
@@ -2843,7 +2944,9 @@
       <c r="J37" s="10">
         <v>1</v>
       </c>
-      <c r="K37" s="10"/>
+      <c r="K37" s="10">
+        <v>0.75</v>
+      </c>
       <c r="L37" s="10"/>
       <c r="M37" s="10"/>
       <c r="N37" s="10"/>
@@ -2865,7 +2968,7 @@
     </row>
     <row r="38" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B38" s="2" t="s">
-        <v>68</v>
+        <v>91</v>
       </c>
       <c r="C38" s="22">
         <v>1</v>
@@ -2892,7 +2995,9 @@
       <c r="J38" s="10">
         <v>0.75</v>
       </c>
-      <c r="K38" s="10"/>
+      <c r="K38" s="10">
+        <v>0</v>
+      </c>
       <c r="L38" s="10"/>
       <c r="M38" s="10"/>
       <c r="N38" s="10"/>
@@ -2913,39 +3018,63 @@
       </c>
     </row>
     <row r="39" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="G39" s="59">
+      <c r="G39" s="32">
         <f>(AVERAGE(G4:G38)*100)</f>
         <v>100</v>
       </c>
-      <c r="H39" s="59">
-        <f t="shared" ref="H39:J39" si="2">(AVERAGE(H4:H38)*100)</f>
+      <c r="H39" s="32">
+        <f t="shared" ref="H39:R39" si="2">(AVERAGE(H4:H38)*100)</f>
         <v>100</v>
       </c>
-      <c r="I39" s="59">
+      <c r="I39" s="32">
         <f t="shared" si="2"/>
         <v>79.411764705882348</v>
       </c>
-      <c r="J39" s="59">
+      <c r="J39" s="32">
         <f t="shared" si="2"/>
         <v>94.85294117647058</v>
       </c>
-      <c r="K39" s="57"/>
-      <c r="L39" s="57"/>
-      <c r="M39" s="57"/>
-      <c r="N39" s="57"/>
-      <c r="O39" s="57"/>
-      <c r="P39" s="57"/>
-      <c r="Q39" s="58"/>
-      <c r="R39" s="58"/>
+      <c r="K39" s="32">
+        <f t="shared" si="2"/>
+        <v>73.529411764705884</v>
+      </c>
+      <c r="L39" s="32" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M39" s="32" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N39" s="32" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O39" s="32" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P39" s="32" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q39" s="32">
+        <f>(AVERAGE(Q4:Q38)*1)</f>
+        <v>76.548387096774192</v>
+      </c>
+      <c r="R39" s="32">
+        <f>(AVERAGE(R4:R38)*1)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="40" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="G40" s="60">
+      <c r="G40" s="33">
         <f>AVERAGE(G39:J39)</f>
         <v>93.566176470588232</v>
       </c>
-      <c r="H40" s="61"/>
-      <c r="I40" s="61"/>
-      <c r="J40" s="61"/>
+      <c r="H40" s="34"/>
+      <c r="I40" s="34"/>
+      <c r="J40" s="34"/>
       <c r="K40" s="25"/>
       <c r="L40" s="25"/>
       <c r="M40" s="25"/>
@@ -2968,6 +3097,38 @@
       <c r="N42" s="25"/>
       <c r="O42" s="25"/>
       <c r="P42" s="25"/>
+    </row>
+    <row r="44" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="G44" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H44" s="2">
+        <v>91</v>
+      </c>
+      <c r="I44" s="2">
+        <f>H44*10%</f>
+        <v>9.1</v>
+      </c>
+      <c r="J44" s="1">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="45" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="I45" s="2">
+        <f>H44+I44</f>
+        <v>100.1</v>
+      </c>
+    </row>
+    <row r="46" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="G46" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="H46" s="2">
+        <v>69</v>
+      </c>
+      <c r="I46" s="2">
+        <v>71</v>
+      </c>
     </row>
     <row r="1048576" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G1048576" s="6"/>
@@ -3029,6 +3190,207 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F32B9B9-AE73-473C-AE26-D53E54D53E5A}">
+  <dimension ref="A1:B38"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M26" sqref="M25:M26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="e">
+        <f>- php artisan migrate</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="e">
+        <f>- php artisan migrate:rollback</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="e">
+        <f xml:space="preserve"> id (PK)</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="e">
+        <f xml:space="preserve"> namaUkuran (string)</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="e">
+        <f xml:space="preserve"> lebarDada (string)</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="e">
+        <f xml:space="preserve"> tinggiBadan (string)</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>103</v>
+      </c>
+      <c r="B25" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="e">
+        <f xml:space="preserve"> id (PK)</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="e">
+        <f xml:space="preserve"> nama_baju (string)</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="e">
+        <f xml:space="preserve"> warna_baju (string)</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="e">
+        <f xml:space="preserve"> ukuran_baju (string)</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>103</v>
+      </c>
+      <c r="B36" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>101</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{715B0C13-179F-4FD8-B66D-ED38FCC03D1C}">
+  <dimension ref="B5:B6"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" zoomScale="280" zoomScaleNormal="280" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{153E42C8-D1FE-4E64-96D9-EED2206D80DB}">
   <dimension ref="A1:M10"/>
   <sheetViews>
@@ -3042,50 +3404,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.7">
-      <c r="A1" s="51" t="s">
-        <v>70</v>
-      </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="51"/>
-      <c r="H1" s="51"/>
-      <c r="I1" s="51"/>
-      <c r="J1" s="51"/>
-      <c r="K1" s="51"/>
-      <c r="L1" s="51"/>
-      <c r="M1" s="51"/>
+      <c r="A1" s="54" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="54"/>
+      <c r="M1" s="54"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.7">
       <c r="A2" s="24">
         <v>1</v>
       </c>
       <c r="B2" s="24" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G2" s="24" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H2" s="24" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.7">
       <c r="C3" s="24" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H3" s="24" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.7">
       <c r="C4" s="24" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H4" s="24" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.7">
@@ -3096,13 +3458,13 @@
         <v>10</v>
       </c>
       <c r="G5" s="24" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H5" s="24">
         <v>1</v>
       </c>
       <c r="I5" s="24" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.7">
@@ -3110,7 +3472,7 @@
         <v>2</v>
       </c>
       <c r="I6" s="24" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.7">
@@ -3118,17 +3480,17 @@
         <v>3</v>
       </c>
       <c r="I7" s="24" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.7">
       <c r="C8" s="24" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.7">
       <c r="C9" s="24" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.7">
@@ -3136,7 +3498,7 @@
         <v>3</v>
       </c>
       <c r="B10" s="24" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -3148,7 +3510,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD728A97-A86D-4319-B892-289BC7014D66}">
   <dimension ref="E2:X30"/>
   <sheetViews>
@@ -3177,608 +3539,603 @@
       <c r="Q2" s="2"/>
     </row>
     <row r="3" spans="5:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E3" s="52">
-        <v>1</v>
-      </c>
-      <c r="F3" s="54" t="s">
+      <c r="E3" s="56">
+        <v>1</v>
+      </c>
+      <c r="F3" s="58" t="s">
         <v>51</v>
       </c>
-      <c r="G3" s="55"/>
-      <c r="H3" s="55"/>
-      <c r="I3" s="55"/>
-      <c r="J3" s="55"/>
-      <c r="K3" s="55"/>
-      <c r="L3" s="55"/>
-      <c r="M3" s="55"/>
-      <c r="N3" s="55"/>
-      <c r="O3" s="55"/>
-      <c r="P3" s="55"/>
-      <c r="Q3" s="55"/>
-      <c r="S3" s="52" t="s">
+      <c r="G3" s="59"/>
+      <c r="H3" s="59"/>
+      <c r="I3" s="59"/>
+      <c r="J3" s="59"/>
+      <c r="K3" s="59"/>
+      <c r="L3" s="59"/>
+      <c r="M3" s="59"/>
+      <c r="N3" s="59"/>
+      <c r="O3" s="59"/>
+      <c r="P3" s="59"/>
+      <c r="Q3" s="59"/>
+      <c r="S3" s="56" t="s">
         <v>58</v>
       </c>
-      <c r="T3" s="52"/>
-      <c r="U3" s="52"/>
-      <c r="W3" s="56" t="s">
+      <c r="T3" s="56"/>
+      <c r="U3" s="56"/>
+      <c r="W3" s="55" t="s">
         <v>60</v>
       </c>
-      <c r="X3" s="56"/>
+      <c r="X3" s="55"/>
     </row>
     <row r="4" spans="5:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E4" s="52"/>
-      <c r="F4" s="55"/>
-      <c r="G4" s="55"/>
-      <c r="H4" s="55"/>
-      <c r="I4" s="55"/>
-      <c r="J4" s="55"/>
-      <c r="K4" s="55"/>
-      <c r="L4" s="55"/>
-      <c r="M4" s="55"/>
-      <c r="N4" s="55"/>
-      <c r="O4" s="55"/>
-      <c r="P4" s="55"/>
-      <c r="Q4" s="55"/>
-      <c r="S4" s="52"/>
-      <c r="T4" s="52"/>
-      <c r="U4" s="52"/>
-      <c r="W4" s="56"/>
-      <c r="X4" s="56"/>
+      <c r="E4" s="56"/>
+      <c r="F4" s="59"/>
+      <c r="G4" s="59"/>
+      <c r="H4" s="59"/>
+      <c r="I4" s="59"/>
+      <c r="J4" s="59"/>
+      <c r="K4" s="59"/>
+      <c r="L4" s="59"/>
+      <c r="M4" s="59"/>
+      <c r="N4" s="59"/>
+      <c r="O4" s="59"/>
+      <c r="P4" s="59"/>
+      <c r="Q4" s="59"/>
+      <c r="S4" s="56"/>
+      <c r="T4" s="56"/>
+      <c r="U4" s="56"/>
+      <c r="W4" s="55"/>
+      <c r="X4" s="55"/>
     </row>
     <row r="5" spans="5:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E5" s="52"/>
-      <c r="F5" s="55"/>
-      <c r="G5" s="55"/>
-      <c r="H5" s="55"/>
-      <c r="I5" s="55"/>
-      <c r="J5" s="55"/>
-      <c r="K5" s="55"/>
-      <c r="L5" s="55"/>
-      <c r="M5" s="55"/>
-      <c r="N5" s="55"/>
-      <c r="O5" s="55"/>
-      <c r="P5" s="55"/>
-      <c r="Q5" s="55"/>
-      <c r="S5" s="52"/>
-      <c r="T5" s="52"/>
-      <c r="U5" s="52"/>
-      <c r="W5" s="56"/>
-      <c r="X5" s="56"/>
+      <c r="E5" s="56"/>
+      <c r="F5" s="59"/>
+      <c r="G5" s="59"/>
+      <c r="H5" s="59"/>
+      <c r="I5" s="59"/>
+      <c r="J5" s="59"/>
+      <c r="K5" s="59"/>
+      <c r="L5" s="59"/>
+      <c r="M5" s="59"/>
+      <c r="N5" s="59"/>
+      <c r="O5" s="59"/>
+      <c r="P5" s="59"/>
+      <c r="Q5" s="59"/>
+      <c r="S5" s="56"/>
+      <c r="T5" s="56"/>
+      <c r="U5" s="56"/>
+      <c r="W5" s="55"/>
+      <c r="X5" s="55"/>
     </row>
     <row r="6" spans="5:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E6" s="52"/>
-      <c r="F6" s="55"/>
-      <c r="G6" s="55"/>
-      <c r="H6" s="55"/>
-      <c r="I6" s="55"/>
-      <c r="J6" s="55"/>
-      <c r="K6" s="55"/>
-      <c r="L6" s="55"/>
-      <c r="M6" s="55"/>
-      <c r="N6" s="55"/>
-      <c r="O6" s="55"/>
-      <c r="P6" s="55"/>
-      <c r="Q6" s="55"/>
-      <c r="S6" s="52"/>
-      <c r="T6" s="52"/>
-      <c r="U6" s="52"/>
-      <c r="W6" s="56"/>
-      <c r="X6" s="56"/>
+      <c r="E6" s="56"/>
+      <c r="F6" s="59"/>
+      <c r="G6" s="59"/>
+      <c r="H6" s="59"/>
+      <c r="I6" s="59"/>
+      <c r="J6" s="59"/>
+      <c r="K6" s="59"/>
+      <c r="L6" s="59"/>
+      <c r="M6" s="59"/>
+      <c r="N6" s="59"/>
+      <c r="O6" s="59"/>
+      <c r="P6" s="59"/>
+      <c r="Q6" s="59"/>
+      <c r="S6" s="56"/>
+      <c r="T6" s="56"/>
+      <c r="U6" s="56"/>
+      <c r="W6" s="55"/>
+      <c r="X6" s="55"/>
     </row>
     <row r="7" spans="5:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E7" s="52"/>
-      <c r="F7" s="55"/>
-      <c r="G7" s="55"/>
-      <c r="H7" s="55"/>
-      <c r="I7" s="55"/>
-      <c r="J7" s="55"/>
-      <c r="K7" s="55"/>
-      <c r="L7" s="55"/>
-      <c r="M7" s="55"/>
-      <c r="N7" s="55"/>
-      <c r="O7" s="55"/>
-      <c r="P7" s="55"/>
-      <c r="Q7" s="55"/>
-      <c r="S7" s="52"/>
-      <c r="T7" s="52"/>
-      <c r="U7" s="52"/>
-      <c r="W7" s="56"/>
-      <c r="X7" s="56"/>
+      <c r="E7" s="56"/>
+      <c r="F7" s="59"/>
+      <c r="G7" s="59"/>
+      <c r="H7" s="59"/>
+      <c r="I7" s="59"/>
+      <c r="J7" s="59"/>
+      <c r="K7" s="59"/>
+      <c r="L7" s="59"/>
+      <c r="M7" s="59"/>
+      <c r="N7" s="59"/>
+      <c r="O7" s="59"/>
+      <c r="P7" s="59"/>
+      <c r="Q7" s="59"/>
+      <c r="S7" s="56"/>
+      <c r="T7" s="56"/>
+      <c r="U7" s="56"/>
+      <c r="W7" s="55"/>
+      <c r="X7" s="55"/>
     </row>
     <row r="8" spans="5:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E8" s="52">
+      <c r="E8" s="56">
         <v>2</v>
       </c>
-      <c r="F8" s="54" t="s">
+      <c r="F8" s="58" t="s">
         <v>52</v>
       </c>
-      <c r="G8" s="55"/>
-      <c r="H8" s="55"/>
-      <c r="I8" s="55"/>
-      <c r="J8" s="55"/>
-      <c r="K8" s="55"/>
-      <c r="L8" s="55"/>
-      <c r="M8" s="55"/>
-      <c r="N8" s="55"/>
-      <c r="O8" s="55"/>
-      <c r="P8" s="55"/>
-      <c r="Q8" s="55"/>
-      <c r="S8" s="52" t="s">
+      <c r="G8" s="59"/>
+      <c r="H8" s="59"/>
+      <c r="I8" s="59"/>
+      <c r="J8" s="59"/>
+      <c r="K8" s="59"/>
+      <c r="L8" s="59"/>
+      <c r="M8" s="59"/>
+      <c r="N8" s="59"/>
+      <c r="O8" s="59"/>
+      <c r="P8" s="59"/>
+      <c r="Q8" s="59"/>
+      <c r="S8" s="56" t="s">
         <v>58</v>
       </c>
-      <c r="T8" s="52"/>
-      <c r="U8" s="52"/>
-      <c r="W8" s="56" t="s">
+      <c r="T8" s="56"/>
+      <c r="U8" s="56"/>
+      <c r="W8" s="55" t="s">
         <v>61</v>
       </c>
-      <c r="X8" s="56"/>
+      <c r="X8" s="55"/>
     </row>
     <row r="9" spans="5:24" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E9" s="52"/>
-      <c r="F9" s="55"/>
-      <c r="G9" s="55"/>
-      <c r="H9" s="55"/>
-      <c r="I9" s="55"/>
-      <c r="J9" s="55"/>
-      <c r="K9" s="55"/>
-      <c r="L9" s="55"/>
-      <c r="M9" s="55"/>
-      <c r="N9" s="55"/>
-      <c r="O9" s="55"/>
-      <c r="P9" s="55"/>
-      <c r="Q9" s="55"/>
-      <c r="S9" s="52"/>
-      <c r="T9" s="52"/>
-      <c r="U9" s="52"/>
-      <c r="W9" s="56"/>
-      <c r="X9" s="56"/>
+      <c r="E9" s="56"/>
+      <c r="F9" s="59"/>
+      <c r="G9" s="59"/>
+      <c r="H9" s="59"/>
+      <c r="I9" s="59"/>
+      <c r="J9" s="59"/>
+      <c r="K9" s="59"/>
+      <c r="L9" s="59"/>
+      <c r="M9" s="59"/>
+      <c r="N9" s="59"/>
+      <c r="O9" s="59"/>
+      <c r="P9" s="59"/>
+      <c r="Q9" s="59"/>
+      <c r="S9" s="56"/>
+      <c r="T9" s="56"/>
+      <c r="U9" s="56"/>
+      <c r="W9" s="55"/>
+      <c r="X9" s="55"/>
     </row>
     <row r="10" spans="5:24" x14ac:dyDescent="0.25">
-      <c r="E10" s="52">
+      <c r="E10" s="56">
         <v>3</v>
       </c>
-      <c r="F10" s="54" t="s">
+      <c r="F10" s="58" t="s">
         <v>53</v>
       </c>
-      <c r="G10" s="55"/>
-      <c r="H10" s="55"/>
-      <c r="I10" s="54" t="s">
+      <c r="G10" s="59"/>
+      <c r="H10" s="59"/>
+      <c r="I10" s="58" t="s">
         <v>64</v>
       </c>
-      <c r="J10" s="55"/>
-      <c r="K10" s="55"/>
-      <c r="L10" s="55"/>
-      <c r="M10" s="55"/>
-      <c r="N10" s="55"/>
-      <c r="O10" s="55"/>
-      <c r="P10" s="55"/>
-      <c r="Q10" s="55"/>
-      <c r="S10" s="53" t="s">
+      <c r="J10" s="59"/>
+      <c r="K10" s="59"/>
+      <c r="L10" s="59"/>
+      <c r="M10" s="59"/>
+      <c r="N10" s="59"/>
+      <c r="O10" s="59"/>
+      <c r="P10" s="59"/>
+      <c r="Q10" s="59"/>
+      <c r="S10" s="57" t="s">
         <v>59</v>
       </c>
-      <c r="T10" s="52"/>
-      <c r="U10" s="52"/>
-      <c r="W10" s="56" t="s">
+      <c r="T10" s="56"/>
+      <c r="U10" s="56"/>
+      <c r="W10" s="55" t="s">
         <v>62</v>
       </c>
-      <c r="X10" s="56" t="s">
+      <c r="X10" s="55" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="11" spans="5:24" x14ac:dyDescent="0.25">
-      <c r="E11" s="52"/>
-      <c r="F11" s="55"/>
-      <c r="G11" s="55"/>
-      <c r="H11" s="55"/>
-      <c r="I11" s="55"/>
-      <c r="J11" s="55"/>
-      <c r="K11" s="55"/>
-      <c r="L11" s="55"/>
-      <c r="M11" s="55"/>
-      <c r="N11" s="55"/>
-      <c r="O11" s="55"/>
-      <c r="P11" s="55"/>
-      <c r="Q11" s="55"/>
-      <c r="S11" s="52"/>
-      <c r="T11" s="52"/>
-      <c r="U11" s="52"/>
-      <c r="W11" s="56"/>
-      <c r="X11" s="56"/>
+      <c r="E11" s="56"/>
+      <c r="F11" s="59"/>
+      <c r="G11" s="59"/>
+      <c r="H11" s="59"/>
+      <c r="I11" s="59"/>
+      <c r="J11" s="59"/>
+      <c r="K11" s="59"/>
+      <c r="L11" s="59"/>
+      <c r="M11" s="59"/>
+      <c r="N11" s="59"/>
+      <c r="O11" s="59"/>
+      <c r="P11" s="59"/>
+      <c r="Q11" s="59"/>
+      <c r="S11" s="56"/>
+      <c r="T11" s="56"/>
+      <c r="U11" s="56"/>
+      <c r="W11" s="55"/>
+      <c r="X11" s="55"/>
     </row>
     <row r="12" spans="5:24" x14ac:dyDescent="0.25">
-      <c r="E12" s="52"/>
-      <c r="F12" s="55"/>
-      <c r="G12" s="55"/>
-      <c r="H12" s="55"/>
-      <c r="I12" s="55"/>
-      <c r="J12" s="55"/>
-      <c r="K12" s="55"/>
-      <c r="L12" s="55"/>
-      <c r="M12" s="55"/>
-      <c r="N12" s="55"/>
-      <c r="O12" s="55"/>
-      <c r="P12" s="55"/>
-      <c r="Q12" s="55"/>
-      <c r="S12" s="52"/>
-      <c r="T12" s="52"/>
-      <c r="U12" s="52"/>
-      <c r="W12" s="56"/>
-      <c r="X12" s="56"/>
+      <c r="E12" s="56"/>
+      <c r="F12" s="59"/>
+      <c r="G12" s="59"/>
+      <c r="H12" s="59"/>
+      <c r="I12" s="59"/>
+      <c r="J12" s="59"/>
+      <c r="K12" s="59"/>
+      <c r="L12" s="59"/>
+      <c r="M12" s="59"/>
+      <c r="N12" s="59"/>
+      <c r="O12" s="59"/>
+      <c r="P12" s="59"/>
+      <c r="Q12" s="59"/>
+      <c r="S12" s="56"/>
+      <c r="T12" s="56"/>
+      <c r="U12" s="56"/>
+      <c r="W12" s="55"/>
+      <c r="X12" s="55"/>
     </row>
     <row r="13" spans="5:24" x14ac:dyDescent="0.25">
-      <c r="E13" s="52"/>
-      <c r="F13" s="55"/>
-      <c r="G13" s="55"/>
-      <c r="H13" s="55"/>
-      <c r="I13" s="55"/>
-      <c r="J13" s="55"/>
-      <c r="K13" s="55"/>
-      <c r="L13" s="55"/>
-      <c r="M13" s="55"/>
-      <c r="N13" s="55"/>
-      <c r="O13" s="55"/>
-      <c r="P13" s="55"/>
-      <c r="Q13" s="55"/>
-      <c r="S13" s="52"/>
-      <c r="T13" s="52"/>
-      <c r="U13" s="52"/>
-      <c r="W13" s="56"/>
-      <c r="X13" s="56"/>
+      <c r="E13" s="56"/>
+      <c r="F13" s="59"/>
+      <c r="G13" s="59"/>
+      <c r="H13" s="59"/>
+      <c r="I13" s="59"/>
+      <c r="J13" s="59"/>
+      <c r="K13" s="59"/>
+      <c r="L13" s="59"/>
+      <c r="M13" s="59"/>
+      <c r="N13" s="59"/>
+      <c r="O13" s="59"/>
+      <c r="P13" s="59"/>
+      <c r="Q13" s="59"/>
+      <c r="S13" s="56"/>
+      <c r="T13" s="56"/>
+      <c r="U13" s="56"/>
+      <c r="W13" s="55"/>
+      <c r="X13" s="55"/>
     </row>
     <row r="14" spans="5:24" x14ac:dyDescent="0.25">
-      <c r="E14" s="52"/>
-      <c r="F14" s="55"/>
-      <c r="G14" s="55"/>
-      <c r="H14" s="55"/>
-      <c r="I14" s="55"/>
-      <c r="J14" s="55"/>
-      <c r="K14" s="55"/>
-      <c r="L14" s="55"/>
-      <c r="M14" s="55"/>
-      <c r="N14" s="55"/>
-      <c r="O14" s="55"/>
-      <c r="P14" s="55"/>
-      <c r="Q14" s="55"/>
-      <c r="S14" s="52"/>
-      <c r="T14" s="52"/>
-      <c r="U14" s="52"/>
-      <c r="W14" s="56"/>
-      <c r="X14" s="56"/>
+      <c r="E14" s="56"/>
+      <c r="F14" s="59"/>
+      <c r="G14" s="59"/>
+      <c r="H14" s="59"/>
+      <c r="I14" s="59"/>
+      <c r="J14" s="59"/>
+      <c r="K14" s="59"/>
+      <c r="L14" s="59"/>
+      <c r="M14" s="59"/>
+      <c r="N14" s="59"/>
+      <c r="O14" s="59"/>
+      <c r="P14" s="59"/>
+      <c r="Q14" s="59"/>
+      <c r="S14" s="56"/>
+      <c r="T14" s="56"/>
+      <c r="U14" s="56"/>
+      <c r="W14" s="55"/>
+      <c r="X14" s="55"/>
     </row>
     <row r="15" spans="5:24" x14ac:dyDescent="0.25">
-      <c r="E15" s="52"/>
-      <c r="F15" s="55"/>
-      <c r="G15" s="55"/>
-      <c r="H15" s="55"/>
-      <c r="I15" s="55"/>
-      <c r="J15" s="55"/>
-      <c r="K15" s="55"/>
-      <c r="L15" s="55"/>
-      <c r="M15" s="55"/>
-      <c r="N15" s="55"/>
-      <c r="O15" s="55"/>
-      <c r="P15" s="55"/>
-      <c r="Q15" s="55"/>
-      <c r="S15" s="52"/>
-      <c r="T15" s="52"/>
-      <c r="U15" s="52"/>
-      <c r="W15" s="56"/>
-      <c r="X15" s="56"/>
+      <c r="E15" s="56"/>
+      <c r="F15" s="59"/>
+      <c r="G15" s="59"/>
+      <c r="H15" s="59"/>
+      <c r="I15" s="59"/>
+      <c r="J15" s="59"/>
+      <c r="K15" s="59"/>
+      <c r="L15" s="59"/>
+      <c r="M15" s="59"/>
+      <c r="N15" s="59"/>
+      <c r="O15" s="59"/>
+      <c r="P15" s="59"/>
+      <c r="Q15" s="59"/>
+      <c r="S15" s="56"/>
+      <c r="T15" s="56"/>
+      <c r="U15" s="56"/>
+      <c r="W15" s="55"/>
+      <c r="X15" s="55"/>
     </row>
     <row r="16" spans="5:24" x14ac:dyDescent="0.25">
-      <c r="E16" s="52"/>
-      <c r="F16" s="55"/>
-      <c r="G16" s="55"/>
-      <c r="H16" s="55"/>
-      <c r="I16" s="55"/>
-      <c r="J16" s="55"/>
-      <c r="K16" s="55"/>
-      <c r="L16" s="55"/>
-      <c r="M16" s="55"/>
-      <c r="N16" s="55"/>
-      <c r="O16" s="55"/>
-      <c r="P16" s="55"/>
-      <c r="Q16" s="55"/>
-      <c r="S16" s="52"/>
-      <c r="T16" s="52"/>
-      <c r="U16" s="52"/>
-      <c r="W16" s="56"/>
-      <c r="X16" s="56"/>
+      <c r="E16" s="56"/>
+      <c r="F16" s="59"/>
+      <c r="G16" s="59"/>
+      <c r="H16" s="59"/>
+      <c r="I16" s="59"/>
+      <c r="J16" s="59"/>
+      <c r="K16" s="59"/>
+      <c r="L16" s="59"/>
+      <c r="M16" s="59"/>
+      <c r="N16" s="59"/>
+      <c r="O16" s="59"/>
+      <c r="P16" s="59"/>
+      <c r="Q16" s="59"/>
+      <c r="S16" s="56"/>
+      <c r="T16" s="56"/>
+      <c r="U16" s="56"/>
+      <c r="W16" s="55"/>
+      <c r="X16" s="55"/>
     </row>
     <row r="17" spans="5:24" x14ac:dyDescent="0.25">
-      <c r="E17" s="52"/>
-      <c r="F17" s="55"/>
-      <c r="G17" s="55"/>
-      <c r="H17" s="55"/>
-      <c r="I17" s="55"/>
-      <c r="J17" s="55"/>
-      <c r="K17" s="55"/>
-      <c r="L17" s="55"/>
-      <c r="M17" s="55"/>
-      <c r="N17" s="55"/>
-      <c r="O17" s="55"/>
-      <c r="P17" s="55"/>
-      <c r="Q17" s="55"/>
-      <c r="S17" s="52"/>
-      <c r="T17" s="52"/>
-      <c r="U17" s="52"/>
-      <c r="W17" s="56"/>
-      <c r="X17" s="56"/>
+      <c r="E17" s="56"/>
+      <c r="F17" s="59"/>
+      <c r="G17" s="59"/>
+      <c r="H17" s="59"/>
+      <c r="I17" s="59"/>
+      <c r="J17" s="59"/>
+      <c r="K17" s="59"/>
+      <c r="L17" s="59"/>
+      <c r="M17" s="59"/>
+      <c r="N17" s="59"/>
+      <c r="O17" s="59"/>
+      <c r="P17" s="59"/>
+      <c r="Q17" s="59"/>
+      <c r="S17" s="56"/>
+      <c r="T17" s="56"/>
+      <c r="U17" s="56"/>
+      <c r="W17" s="55"/>
+      <c r="X17" s="55"/>
     </row>
     <row r="18" spans="5:24" x14ac:dyDescent="0.25">
-      <c r="E18" s="52"/>
-      <c r="F18" s="55"/>
-      <c r="G18" s="55"/>
-      <c r="H18" s="55"/>
-      <c r="I18" s="55"/>
-      <c r="J18" s="55"/>
-      <c r="K18" s="55"/>
-      <c r="L18" s="55"/>
-      <c r="M18" s="55"/>
-      <c r="N18" s="55"/>
-      <c r="O18" s="55"/>
-      <c r="P18" s="55"/>
-      <c r="Q18" s="55"/>
-      <c r="S18" s="52"/>
-      <c r="T18" s="52"/>
-      <c r="U18" s="52"/>
-      <c r="W18" s="56"/>
-      <c r="X18" s="56"/>
+      <c r="E18" s="56"/>
+      <c r="F18" s="59"/>
+      <c r="G18" s="59"/>
+      <c r="H18" s="59"/>
+      <c r="I18" s="59"/>
+      <c r="J18" s="59"/>
+      <c r="K18" s="59"/>
+      <c r="L18" s="59"/>
+      <c r="M18" s="59"/>
+      <c r="N18" s="59"/>
+      <c r="O18" s="59"/>
+      <c r="P18" s="59"/>
+      <c r="Q18" s="59"/>
+      <c r="S18" s="56"/>
+      <c r="T18" s="56"/>
+      <c r="U18" s="56"/>
+      <c r="W18" s="55"/>
+      <c r="X18" s="55"/>
     </row>
     <row r="19" spans="5:24" x14ac:dyDescent="0.25">
-      <c r="E19" s="52"/>
-      <c r="F19" s="55"/>
-      <c r="G19" s="55"/>
-      <c r="H19" s="55"/>
-      <c r="I19" s="55"/>
-      <c r="J19" s="55"/>
-      <c r="K19" s="55"/>
-      <c r="L19" s="55"/>
-      <c r="M19" s="55"/>
-      <c r="N19" s="55"/>
-      <c r="O19" s="55"/>
-      <c r="P19" s="55"/>
-      <c r="Q19" s="55"/>
-      <c r="S19" s="52"/>
-      <c r="T19" s="52"/>
-      <c r="U19" s="52"/>
-      <c r="W19" s="56"/>
-      <c r="X19" s="56"/>
+      <c r="E19" s="56"/>
+      <c r="F19" s="59"/>
+      <c r="G19" s="59"/>
+      <c r="H19" s="59"/>
+      <c r="I19" s="59"/>
+      <c r="J19" s="59"/>
+      <c r="K19" s="59"/>
+      <c r="L19" s="59"/>
+      <c r="M19" s="59"/>
+      <c r="N19" s="59"/>
+      <c r="O19" s="59"/>
+      <c r="P19" s="59"/>
+      <c r="Q19" s="59"/>
+      <c r="S19" s="56"/>
+      <c r="T19" s="56"/>
+      <c r="U19" s="56"/>
+      <c r="W19" s="55"/>
+      <c r="X19" s="55"/>
     </row>
     <row r="20" spans="5:24" x14ac:dyDescent="0.25">
-      <c r="E20" s="52"/>
-      <c r="F20" s="55"/>
-      <c r="G20" s="55"/>
-      <c r="H20" s="55"/>
-      <c r="I20" s="55"/>
-      <c r="J20" s="55"/>
-      <c r="K20" s="55"/>
-      <c r="L20" s="55"/>
-      <c r="M20" s="55"/>
-      <c r="N20" s="55"/>
-      <c r="O20" s="55"/>
-      <c r="P20" s="55"/>
-      <c r="Q20" s="55"/>
-      <c r="S20" s="52"/>
-      <c r="T20" s="52"/>
-      <c r="U20" s="52"/>
-      <c r="W20" s="56"/>
-      <c r="X20" s="56"/>
+      <c r="E20" s="56"/>
+      <c r="F20" s="59"/>
+      <c r="G20" s="59"/>
+      <c r="H20" s="59"/>
+      <c r="I20" s="59"/>
+      <c r="J20" s="59"/>
+      <c r="K20" s="59"/>
+      <c r="L20" s="59"/>
+      <c r="M20" s="59"/>
+      <c r="N20" s="59"/>
+      <c r="O20" s="59"/>
+      <c r="P20" s="59"/>
+      <c r="Q20" s="59"/>
+      <c r="S20" s="56"/>
+      <c r="T20" s="56"/>
+      <c r="U20" s="56"/>
+      <c r="W20" s="55"/>
+      <c r="X20" s="55"/>
     </row>
     <row r="21" spans="5:24" x14ac:dyDescent="0.25">
-      <c r="E21" s="52"/>
-      <c r="F21" s="55"/>
-      <c r="G21" s="55"/>
-      <c r="H21" s="55"/>
-      <c r="I21" s="55"/>
-      <c r="J21" s="55"/>
-      <c r="K21" s="55"/>
-      <c r="L21" s="55"/>
-      <c r="M21" s="55"/>
-      <c r="N21" s="55"/>
-      <c r="O21" s="55"/>
-      <c r="P21" s="55"/>
-      <c r="Q21" s="55"/>
-      <c r="S21" s="52"/>
-      <c r="T21" s="52"/>
-      <c r="U21" s="52"/>
-      <c r="W21" s="56"/>
-      <c r="X21" s="56"/>
+      <c r="E21" s="56"/>
+      <c r="F21" s="59"/>
+      <c r="G21" s="59"/>
+      <c r="H21" s="59"/>
+      <c r="I21" s="59"/>
+      <c r="J21" s="59"/>
+      <c r="K21" s="59"/>
+      <c r="L21" s="59"/>
+      <c r="M21" s="59"/>
+      <c r="N21" s="59"/>
+      <c r="O21" s="59"/>
+      <c r="P21" s="59"/>
+      <c r="Q21" s="59"/>
+      <c r="S21" s="56"/>
+      <c r="T21" s="56"/>
+      <c r="U21" s="56"/>
+      <c r="W21" s="55"/>
+      <c r="X21" s="55"/>
     </row>
     <row r="22" spans="5:24" x14ac:dyDescent="0.25">
-      <c r="E22" s="52"/>
-      <c r="F22" s="55"/>
-      <c r="G22" s="55"/>
-      <c r="H22" s="55"/>
-      <c r="I22" s="55"/>
-      <c r="J22" s="55"/>
-      <c r="K22" s="55"/>
-      <c r="L22" s="55"/>
-      <c r="M22" s="55"/>
-      <c r="N22" s="55"/>
-      <c r="O22" s="55"/>
-      <c r="P22" s="55"/>
-      <c r="Q22" s="55"/>
-      <c r="S22" s="52"/>
-      <c r="T22" s="52"/>
-      <c r="U22" s="52"/>
-      <c r="W22" s="56"/>
-      <c r="X22" s="56"/>
+      <c r="E22" s="56"/>
+      <c r="F22" s="59"/>
+      <c r="G22" s="59"/>
+      <c r="H22" s="59"/>
+      <c r="I22" s="59"/>
+      <c r="J22" s="59"/>
+      <c r="K22" s="59"/>
+      <c r="L22" s="59"/>
+      <c r="M22" s="59"/>
+      <c r="N22" s="59"/>
+      <c r="O22" s="59"/>
+      <c r="P22" s="59"/>
+      <c r="Q22" s="59"/>
+      <c r="S22" s="56"/>
+      <c r="T22" s="56"/>
+      <c r="U22" s="56"/>
+      <c r="W22" s="55"/>
+      <c r="X22" s="55"/>
     </row>
     <row r="23" spans="5:24" x14ac:dyDescent="0.25">
-      <c r="E23" s="52"/>
-      <c r="F23" s="55"/>
-      <c r="G23" s="55"/>
-      <c r="H23" s="55"/>
-      <c r="I23" s="55"/>
-      <c r="J23" s="55"/>
-      <c r="K23" s="55"/>
-      <c r="L23" s="55"/>
-      <c r="M23" s="55"/>
-      <c r="N23" s="55"/>
-      <c r="O23" s="55"/>
-      <c r="P23" s="55"/>
-      <c r="Q23" s="55"/>
-      <c r="S23" s="52"/>
-      <c r="T23" s="52"/>
-      <c r="U23" s="52"/>
-      <c r="W23" s="56"/>
-      <c r="X23" s="56"/>
+      <c r="E23" s="56"/>
+      <c r="F23" s="59"/>
+      <c r="G23" s="59"/>
+      <c r="H23" s="59"/>
+      <c r="I23" s="59"/>
+      <c r="J23" s="59"/>
+      <c r="K23" s="59"/>
+      <c r="L23" s="59"/>
+      <c r="M23" s="59"/>
+      <c r="N23" s="59"/>
+      <c r="O23" s="59"/>
+      <c r="P23" s="59"/>
+      <c r="Q23" s="59"/>
+      <c r="S23" s="56"/>
+      <c r="T23" s="56"/>
+      <c r="U23" s="56"/>
+      <c r="W23" s="55"/>
+      <c r="X23" s="55"/>
     </row>
     <row r="24" spans="5:24" x14ac:dyDescent="0.25">
-      <c r="E24" s="52"/>
-      <c r="F24" s="55"/>
-      <c r="G24" s="55"/>
-      <c r="H24" s="55"/>
-      <c r="I24" s="55"/>
-      <c r="J24" s="55"/>
-      <c r="K24" s="55"/>
-      <c r="L24" s="55"/>
-      <c r="M24" s="55"/>
-      <c r="N24" s="55"/>
-      <c r="O24" s="55"/>
-      <c r="P24" s="55"/>
-      <c r="Q24" s="55"/>
-      <c r="S24" s="52"/>
-      <c r="T24" s="52"/>
-      <c r="U24" s="52"/>
-      <c r="W24" s="56"/>
-      <c r="X24" s="56"/>
+      <c r="E24" s="56"/>
+      <c r="F24" s="59"/>
+      <c r="G24" s="59"/>
+      <c r="H24" s="59"/>
+      <c r="I24" s="59"/>
+      <c r="J24" s="59"/>
+      <c r="K24" s="59"/>
+      <c r="L24" s="59"/>
+      <c r="M24" s="59"/>
+      <c r="N24" s="59"/>
+      <c r="O24" s="59"/>
+      <c r="P24" s="59"/>
+      <c r="Q24" s="59"/>
+      <c r="S24" s="56"/>
+      <c r="T24" s="56"/>
+      <c r="U24" s="56"/>
+      <c r="W24" s="55"/>
+      <c r="X24" s="55"/>
     </row>
     <row r="25" spans="5:24" x14ac:dyDescent="0.25">
-      <c r="E25" s="52"/>
-      <c r="F25" s="55"/>
-      <c r="G25" s="55"/>
-      <c r="H25" s="55"/>
-      <c r="I25" s="55"/>
-      <c r="J25" s="55"/>
-      <c r="K25" s="55"/>
-      <c r="L25" s="55"/>
-      <c r="M25" s="55"/>
-      <c r="N25" s="55"/>
-      <c r="O25" s="55"/>
-      <c r="P25" s="55"/>
-      <c r="Q25" s="55"/>
-      <c r="S25" s="52"/>
-      <c r="T25" s="52"/>
-      <c r="U25" s="52"/>
-      <c r="W25" s="56"/>
-      <c r="X25" s="56"/>
+      <c r="E25" s="56"/>
+      <c r="F25" s="59"/>
+      <c r="G25" s="59"/>
+      <c r="H25" s="59"/>
+      <c r="I25" s="59"/>
+      <c r="J25" s="59"/>
+      <c r="K25" s="59"/>
+      <c r="L25" s="59"/>
+      <c r="M25" s="59"/>
+      <c r="N25" s="59"/>
+      <c r="O25" s="59"/>
+      <c r="P25" s="59"/>
+      <c r="Q25" s="59"/>
+      <c r="S25" s="56"/>
+      <c r="T25" s="56"/>
+      <c r="U25" s="56"/>
+      <c r="W25" s="55"/>
+      <c r="X25" s="55"/>
     </row>
     <row r="26" spans="5:24" x14ac:dyDescent="0.25">
-      <c r="E26" s="52"/>
-      <c r="F26" s="55"/>
-      <c r="G26" s="55"/>
-      <c r="H26" s="55"/>
-      <c r="I26" s="55"/>
-      <c r="J26" s="55"/>
-      <c r="K26" s="55"/>
-      <c r="L26" s="55"/>
-      <c r="M26" s="55"/>
-      <c r="N26" s="55"/>
-      <c r="O26" s="55"/>
-      <c r="P26" s="55"/>
-      <c r="Q26" s="55"/>
-      <c r="S26" s="52"/>
-      <c r="T26" s="52"/>
-      <c r="U26" s="52"/>
-      <c r="W26" s="56"/>
-      <c r="X26" s="56"/>
+      <c r="E26" s="56"/>
+      <c r="F26" s="59"/>
+      <c r="G26" s="59"/>
+      <c r="H26" s="59"/>
+      <c r="I26" s="59"/>
+      <c r="J26" s="59"/>
+      <c r="K26" s="59"/>
+      <c r="L26" s="59"/>
+      <c r="M26" s="59"/>
+      <c r="N26" s="59"/>
+      <c r="O26" s="59"/>
+      <c r="P26" s="59"/>
+      <c r="Q26" s="59"/>
+      <c r="S26" s="56"/>
+      <c r="T26" s="56"/>
+      <c r="U26" s="56"/>
+      <c r="W26" s="55"/>
+      <c r="X26" s="55"/>
     </row>
     <row r="27" spans="5:24" x14ac:dyDescent="0.25">
-      <c r="E27" s="52"/>
-      <c r="F27" s="55"/>
-      <c r="G27" s="55"/>
-      <c r="H27" s="55"/>
-      <c r="I27" s="55"/>
-      <c r="J27" s="55"/>
-      <c r="K27" s="55"/>
-      <c r="L27" s="55"/>
-      <c r="M27" s="55"/>
-      <c r="N27" s="55"/>
-      <c r="O27" s="55"/>
-      <c r="P27" s="55"/>
-      <c r="Q27" s="55"/>
-      <c r="S27" s="52"/>
-      <c r="T27" s="52"/>
-      <c r="U27" s="52"/>
-      <c r="W27" s="56"/>
-      <c r="X27" s="56"/>
+      <c r="E27" s="56"/>
+      <c r="F27" s="59"/>
+      <c r="G27" s="59"/>
+      <c r="H27" s="59"/>
+      <c r="I27" s="59"/>
+      <c r="J27" s="59"/>
+      <c r="K27" s="59"/>
+      <c r="L27" s="59"/>
+      <c r="M27" s="59"/>
+      <c r="N27" s="59"/>
+      <c r="O27" s="59"/>
+      <c r="P27" s="59"/>
+      <c r="Q27" s="59"/>
+      <c r="S27" s="56"/>
+      <c r="T27" s="56"/>
+      <c r="U27" s="56"/>
+      <c r="W27" s="55"/>
+      <c r="X27" s="55"/>
     </row>
     <row r="28" spans="5:24" x14ac:dyDescent="0.25">
-      <c r="E28" s="52"/>
-      <c r="F28" s="55"/>
-      <c r="G28" s="55"/>
-      <c r="H28" s="55"/>
-      <c r="I28" s="55"/>
-      <c r="J28" s="55"/>
-      <c r="K28" s="55"/>
-      <c r="L28" s="55"/>
-      <c r="M28" s="55"/>
-      <c r="N28" s="55"/>
-      <c r="O28" s="55"/>
-      <c r="P28" s="55"/>
-      <c r="Q28" s="55"/>
-      <c r="S28" s="52"/>
-      <c r="T28" s="52"/>
-      <c r="U28" s="52"/>
-      <c r="W28" s="56"/>
-      <c r="X28" s="56"/>
+      <c r="E28" s="56"/>
+      <c r="F28" s="59"/>
+      <c r="G28" s="59"/>
+      <c r="H28" s="59"/>
+      <c r="I28" s="59"/>
+      <c r="J28" s="59"/>
+      <c r="K28" s="59"/>
+      <c r="L28" s="59"/>
+      <c r="M28" s="59"/>
+      <c r="N28" s="59"/>
+      <c r="O28" s="59"/>
+      <c r="P28" s="59"/>
+      <c r="Q28" s="59"/>
+      <c r="S28" s="56"/>
+      <c r="T28" s="56"/>
+      <c r="U28" s="56"/>
+      <c r="W28" s="55"/>
+      <c r="X28" s="55"/>
     </row>
     <row r="29" spans="5:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E29" s="52">
+      <c r="E29" s="56">
         <v>4</v>
       </c>
-      <c r="F29" s="54" t="s">
+      <c r="F29" s="58" t="s">
         <v>54</v>
       </c>
-      <c r="G29" s="55"/>
-      <c r="H29" s="55"/>
-      <c r="I29" s="55"/>
-      <c r="J29" s="55"/>
-      <c r="K29" s="55"/>
-      <c r="L29" s="55"/>
-      <c r="M29" s="55"/>
-      <c r="N29" s="55"/>
-      <c r="O29" s="55"/>
-      <c r="P29" s="55"/>
-      <c r="Q29" s="55"/>
-      <c r="S29" s="52" t="s">
+      <c r="G29" s="59"/>
+      <c r="H29" s="59"/>
+      <c r="I29" s="59"/>
+      <c r="J29" s="59"/>
+      <c r="K29" s="59"/>
+      <c r="L29" s="59"/>
+      <c r="M29" s="59"/>
+      <c r="N29" s="59"/>
+      <c r="O29" s="59"/>
+      <c r="P29" s="59"/>
+      <c r="Q29" s="59"/>
+      <c r="S29" s="56" t="s">
         <v>58</v>
       </c>
-      <c r="T29" s="52"/>
-      <c r="U29" s="52"/>
-      <c r="W29" s="56" t="s">
+      <c r="T29" s="56"/>
+      <c r="U29" s="56"/>
+      <c r="W29" s="55" t="s">
         <v>65</v>
       </c>
-      <c r="X29" s="56"/>
+      <c r="X29" s="55"/>
     </row>
     <row r="30" spans="5:24" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E30" s="52"/>
-      <c r="F30" s="55"/>
-      <c r="G30" s="55"/>
-      <c r="H30" s="55"/>
-      <c r="I30" s="55"/>
-      <c r="J30" s="55"/>
-      <c r="K30" s="55"/>
-      <c r="L30" s="55"/>
-      <c r="M30" s="55"/>
-      <c r="N30" s="55"/>
-      <c r="O30" s="55"/>
-      <c r="P30" s="55"/>
-      <c r="Q30" s="55"/>
-      <c r="S30" s="52"/>
-      <c r="T30" s="52"/>
-      <c r="U30" s="52"/>
-      <c r="W30" s="56"/>
-      <c r="X30" s="56"/>
+      <c r="E30" s="56"/>
+      <c r="F30" s="59"/>
+      <c r="G30" s="59"/>
+      <c r="H30" s="59"/>
+      <c r="I30" s="59"/>
+      <c r="J30" s="59"/>
+      <c r="K30" s="59"/>
+      <c r="L30" s="59"/>
+      <c r="M30" s="59"/>
+      <c r="N30" s="59"/>
+      <c r="O30" s="59"/>
+      <c r="P30" s="59"/>
+      <c r="Q30" s="59"/>
+      <c r="S30" s="56"/>
+      <c r="T30" s="56"/>
+      <c r="U30" s="56"/>
+      <c r="W30" s="55"/>
+      <c r="X30" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="W3:X7"/>
-    <mergeCell ref="W8:X9"/>
-    <mergeCell ref="W29:X30"/>
-    <mergeCell ref="W10:W28"/>
-    <mergeCell ref="X10:X28"/>
     <mergeCell ref="S3:U7"/>
     <mergeCell ref="S8:U9"/>
     <mergeCell ref="S10:U28"/>
@@ -3792,6 +4149,11 @@
     <mergeCell ref="F10:H28"/>
     <mergeCell ref="I10:Q28"/>
     <mergeCell ref="F29:Q30"/>
+    <mergeCell ref="W3:X7"/>
+    <mergeCell ref="W8:X9"/>
+    <mergeCell ref="W29:X30"/>
+    <mergeCell ref="W10:W28"/>
+    <mergeCell ref="X10:X28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
format nilai kelas xii rpl3
</commit_message>
<xml_diff>
--- a/XIIRPL2(❁´◡`❁)(❁´◡`❁)(❁´◡`❁)(u‿ฺu✿ฺ)/DATA PRAKTIK XII RPl 2.xlsx
+++ b/XIIRPL2(❁´◡`❁)(❁´◡`❁)(❁´◡`❁)(u‿ฺu✿ฺ)/DATA PRAKTIK XII RPl 2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AdeSetiyawan)(✿◡‿◡)(✿◡‿◡)\XIIRPL2(❁´◡`❁)(❁´◡`❁)(❁´◡`❁)(u‿ฺu✿ฺ)\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\_01.AdeSetiyawan\01. Pembelajaran\pwpb2223\XIIRPL2(❁´◡`❁)(❁´◡`❁)(❁´◡`❁)(u‿ฺu✿ฺ)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B29C6C9-4862-4374-84FA-92A132247505}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF39EEC9-6FDE-4001-A8DE-7AF317D9C4EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7A470BEC-FF9B-4C58-B3A9-6A89F2B6EB46}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{7A470BEC-FF9B-4C58-B3A9-6A89F2B6EB46}"/>
   </bookViews>
   <sheets>
     <sheet name="Nilai All" sheetId="1" r:id="rId1"/>
@@ -26,6 +26,15 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -808,6 +817,12 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -874,26 +889,20 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1201,7 +1210,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1211,8 +1220,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E8966E4-2275-4E9F-82CA-974F40DBA593}">
   <dimension ref="B1:T1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T17" sqref="T17"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1232,51 +1241,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="39" t="s">
         <v>57</v>
       </c>
-      <c r="D1" s="38" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" s="41" t="s">
+      <c r="D1" s="40" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="43" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="51" t="s">
+      <c r="G1" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="53" t="s">
+      <c r="H1" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="53"/>
-      <c r="J1" s="53"/>
-      <c r="K1" s="49" t="s">
+      <c r="I1" s="55"/>
+      <c r="J1" s="55"/>
+      <c r="K1" s="51" t="s">
         <v>49</v>
       </c>
-      <c r="L1" s="50"/>
-      <c r="M1" s="50"/>
-      <c r="N1" s="50"/>
-      <c r="O1" s="50"/>
-      <c r="P1" s="50"/>
-      <c r="Q1" s="44" t="s">
+      <c r="L1" s="52"/>
+      <c r="M1" s="52"/>
+      <c r="N1" s="52"/>
+      <c r="O1" s="52"/>
+      <c r="P1" s="52"/>
+      <c r="Q1" s="46" t="s">
         <v>66</v>
       </c>
-      <c r="R1" s="44" t="s">
+      <c r="R1" s="46" t="s">
         <v>67</v>
       </c>
-      <c r="S1" s="35" t="s">
+      <c r="S1" s="37" t="s">
         <v>76</v>
       </c>
-      <c r="T1" s="36"/>
+      <c r="T1" s="38"/>
     </row>
     <row r="2" spans="2:20" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="37"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="52"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="54"/>
       <c r="H2" s="15" t="s">
         <v>10</v>
       </c>
@@ -1286,10 +1295,10 @@
       <c r="J2" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="60" t="s">
+      <c r="K2" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="L2" s="60" t="s">
+      <c r="L2" s="33" t="s">
         <v>5</v>
       </c>
       <c r="M2" s="9" t="s">
@@ -1304,34 +1313,34 @@
       <c r="P2" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="Q2" s="45"/>
-      <c r="R2" s="44"/>
-      <c r="S2" s="35"/>
-      <c r="T2" s="36"/>
+      <c r="Q2" s="47"/>
+      <c r="R2" s="46"/>
+      <c r="S2" s="37"/>
+      <c r="T2" s="38"/>
     </row>
     <row r="3" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="37"/>
-      <c r="D3" s="40"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="45"/>
       <c r="G3" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="H3" s="46" t="s">
+      <c r="H3" s="48" t="s">
         <v>47</v>
       </c>
-      <c r="I3" s="47"/>
-      <c r="J3" s="48"/>
-      <c r="K3" s="61" t="s">
+      <c r="I3" s="49"/>
+      <c r="J3" s="50"/>
+      <c r="K3" s="34" t="s">
         <v>89</v>
       </c>
-      <c r="L3" s="61"/>
+      <c r="L3" s="34"/>
       <c r="M3" s="8"/>
       <c r="N3" s="8"/>
       <c r="O3" s="8"/>
       <c r="P3" s="13"/>
-      <c r="Q3" s="45"/>
-      <c r="R3" s="44"/>
+      <c r="Q3" s="47"/>
+      <c r="R3" s="46"/>
       <c r="S3" s="26" t="s">
         <v>77</v>
       </c>
@@ -3023,7 +3032,7 @@
         <v>100</v>
       </c>
       <c r="H39" s="32">
-        <f t="shared" ref="H39:R39" si="2">(AVERAGE(H4:H38)*100)</f>
+        <f t="shared" ref="H39:P39" si="2">(AVERAGE(H4:H38)*100)</f>
         <v>100</v>
       </c>
       <c r="I39" s="32">
@@ -3068,13 +3077,13 @@
       </c>
     </row>
     <row r="40" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="G40" s="33">
+      <c r="G40" s="35">
         <f>AVERAGE(G39:J39)</f>
         <v>93.566176470588232</v>
       </c>
-      <c r="H40" s="34"/>
-      <c r="I40" s="34"/>
-      <c r="J40" s="34"/>
+      <c r="H40" s="36"/>
+      <c r="I40" s="36"/>
+      <c r="J40" s="36"/>
       <c r="K40" s="25"/>
       <c r="L40" s="25"/>
       <c r="M40" s="25"/>
@@ -3404,21 +3413,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.7">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="56" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
-      <c r="K1" s="54"/>
-      <c r="L1" s="54"/>
-      <c r="M1" s="54"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="56"/>
+      <c r="K1" s="56"/>
+      <c r="L1" s="56"/>
+      <c r="M1" s="56"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.7">
       <c r="A2" s="24">
@@ -3539,603 +3548,608 @@
       <c r="Q2" s="2"/>
     </row>
     <row r="3" spans="5:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E3" s="56">
-        <v>1</v>
-      </c>
-      <c r="F3" s="58" t="s">
+      <c r="E3" s="57">
+        <v>1</v>
+      </c>
+      <c r="F3" s="59" t="s">
         <v>51</v>
       </c>
-      <c r="G3" s="59"/>
-      <c r="H3" s="59"/>
-      <c r="I3" s="59"/>
-      <c r="J3" s="59"/>
-      <c r="K3" s="59"/>
-      <c r="L3" s="59"/>
-      <c r="M3" s="59"/>
-      <c r="N3" s="59"/>
-      <c r="O3" s="59"/>
-      <c r="P3" s="59"/>
-      <c r="Q3" s="59"/>
-      <c r="S3" s="56" t="s">
+      <c r="G3" s="60"/>
+      <c r="H3" s="60"/>
+      <c r="I3" s="60"/>
+      <c r="J3" s="60"/>
+      <c r="K3" s="60"/>
+      <c r="L3" s="60"/>
+      <c r="M3" s="60"/>
+      <c r="N3" s="60"/>
+      <c r="O3" s="60"/>
+      <c r="P3" s="60"/>
+      <c r="Q3" s="60"/>
+      <c r="S3" s="57" t="s">
         <v>58</v>
       </c>
-      <c r="T3" s="56"/>
-      <c r="U3" s="56"/>
-      <c r="W3" s="55" t="s">
+      <c r="T3" s="57"/>
+      <c r="U3" s="57"/>
+      <c r="W3" s="61" t="s">
         <v>60</v>
       </c>
-      <c r="X3" s="55"/>
+      <c r="X3" s="61"/>
     </row>
     <row r="4" spans="5:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E4" s="56"/>
-      <c r="F4" s="59"/>
-      <c r="G4" s="59"/>
-      <c r="H4" s="59"/>
-      <c r="I4" s="59"/>
-      <c r="J4" s="59"/>
-      <c r="K4" s="59"/>
-      <c r="L4" s="59"/>
-      <c r="M4" s="59"/>
-      <c r="N4" s="59"/>
-      <c r="O4" s="59"/>
-      <c r="P4" s="59"/>
-      <c r="Q4" s="59"/>
-      <c r="S4" s="56"/>
-      <c r="T4" s="56"/>
-      <c r="U4" s="56"/>
-      <c r="W4" s="55"/>
-      <c r="X4" s="55"/>
+      <c r="E4" s="57"/>
+      <c r="F4" s="60"/>
+      <c r="G4" s="60"/>
+      <c r="H4" s="60"/>
+      <c r="I4" s="60"/>
+      <c r="J4" s="60"/>
+      <c r="K4" s="60"/>
+      <c r="L4" s="60"/>
+      <c r="M4" s="60"/>
+      <c r="N4" s="60"/>
+      <c r="O4" s="60"/>
+      <c r="P4" s="60"/>
+      <c r="Q4" s="60"/>
+      <c r="S4" s="57"/>
+      <c r="T4" s="57"/>
+      <c r="U4" s="57"/>
+      <c r="W4" s="61"/>
+      <c r="X4" s="61"/>
     </row>
     <row r="5" spans="5:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E5" s="56"/>
-      <c r="F5" s="59"/>
-      <c r="G5" s="59"/>
-      <c r="H5" s="59"/>
-      <c r="I5" s="59"/>
-      <c r="J5" s="59"/>
-      <c r="K5" s="59"/>
-      <c r="L5" s="59"/>
-      <c r="M5" s="59"/>
-      <c r="N5" s="59"/>
-      <c r="O5" s="59"/>
-      <c r="P5" s="59"/>
-      <c r="Q5" s="59"/>
-      <c r="S5" s="56"/>
-      <c r="T5" s="56"/>
-      <c r="U5" s="56"/>
-      <c r="W5" s="55"/>
-      <c r="X5" s="55"/>
+      <c r="E5" s="57"/>
+      <c r="F5" s="60"/>
+      <c r="G5" s="60"/>
+      <c r="H5" s="60"/>
+      <c r="I5" s="60"/>
+      <c r="J5" s="60"/>
+      <c r="K5" s="60"/>
+      <c r="L5" s="60"/>
+      <c r="M5" s="60"/>
+      <c r="N5" s="60"/>
+      <c r="O5" s="60"/>
+      <c r="P5" s="60"/>
+      <c r="Q5" s="60"/>
+      <c r="S5" s="57"/>
+      <c r="T5" s="57"/>
+      <c r="U5" s="57"/>
+      <c r="W5" s="61"/>
+      <c r="X5" s="61"/>
     </row>
     <row r="6" spans="5:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E6" s="56"/>
-      <c r="F6" s="59"/>
-      <c r="G6" s="59"/>
-      <c r="H6" s="59"/>
-      <c r="I6" s="59"/>
-      <c r="J6" s="59"/>
-      <c r="K6" s="59"/>
-      <c r="L6" s="59"/>
-      <c r="M6" s="59"/>
-      <c r="N6" s="59"/>
-      <c r="O6" s="59"/>
-      <c r="P6" s="59"/>
-      <c r="Q6" s="59"/>
-      <c r="S6" s="56"/>
-      <c r="T6" s="56"/>
-      <c r="U6" s="56"/>
-      <c r="W6" s="55"/>
-      <c r="X6" s="55"/>
+      <c r="E6" s="57"/>
+      <c r="F6" s="60"/>
+      <c r="G6" s="60"/>
+      <c r="H6" s="60"/>
+      <c r="I6" s="60"/>
+      <c r="J6" s="60"/>
+      <c r="K6" s="60"/>
+      <c r="L6" s="60"/>
+      <c r="M6" s="60"/>
+      <c r="N6" s="60"/>
+      <c r="O6" s="60"/>
+      <c r="P6" s="60"/>
+      <c r="Q6" s="60"/>
+      <c r="S6" s="57"/>
+      <c r="T6" s="57"/>
+      <c r="U6" s="57"/>
+      <c r="W6" s="61"/>
+      <c r="X6" s="61"/>
     </row>
     <row r="7" spans="5:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E7" s="56"/>
-      <c r="F7" s="59"/>
-      <c r="G7" s="59"/>
-      <c r="H7" s="59"/>
-      <c r="I7" s="59"/>
-      <c r="J7" s="59"/>
-      <c r="K7" s="59"/>
-      <c r="L7" s="59"/>
-      <c r="M7" s="59"/>
-      <c r="N7" s="59"/>
-      <c r="O7" s="59"/>
-      <c r="P7" s="59"/>
-      <c r="Q7" s="59"/>
-      <c r="S7" s="56"/>
-      <c r="T7" s="56"/>
-      <c r="U7" s="56"/>
-      <c r="W7" s="55"/>
-      <c r="X7" s="55"/>
+      <c r="E7" s="57"/>
+      <c r="F7" s="60"/>
+      <c r="G7" s="60"/>
+      <c r="H7" s="60"/>
+      <c r="I7" s="60"/>
+      <c r="J7" s="60"/>
+      <c r="K7" s="60"/>
+      <c r="L7" s="60"/>
+      <c r="M7" s="60"/>
+      <c r="N7" s="60"/>
+      <c r="O7" s="60"/>
+      <c r="P7" s="60"/>
+      <c r="Q7" s="60"/>
+      <c r="S7" s="57"/>
+      <c r="T7" s="57"/>
+      <c r="U7" s="57"/>
+      <c r="W7" s="61"/>
+      <c r="X7" s="61"/>
     </row>
     <row r="8" spans="5:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E8" s="56">
+      <c r="E8" s="57">
         <v>2</v>
       </c>
-      <c r="F8" s="58" t="s">
+      <c r="F8" s="59" t="s">
         <v>52</v>
       </c>
-      <c r="G8" s="59"/>
-      <c r="H8" s="59"/>
-      <c r="I8" s="59"/>
-      <c r="J8" s="59"/>
-      <c r="K8" s="59"/>
-      <c r="L8" s="59"/>
-      <c r="M8" s="59"/>
-      <c r="N8" s="59"/>
-      <c r="O8" s="59"/>
-      <c r="P8" s="59"/>
-      <c r="Q8" s="59"/>
-      <c r="S8" s="56" t="s">
+      <c r="G8" s="60"/>
+      <c r="H8" s="60"/>
+      <c r="I8" s="60"/>
+      <c r="J8" s="60"/>
+      <c r="K8" s="60"/>
+      <c r="L8" s="60"/>
+      <c r="M8" s="60"/>
+      <c r="N8" s="60"/>
+      <c r="O8" s="60"/>
+      <c r="P8" s="60"/>
+      <c r="Q8" s="60"/>
+      <c r="S8" s="57" t="s">
         <v>58</v>
       </c>
-      <c r="T8" s="56"/>
-      <c r="U8" s="56"/>
-      <c r="W8" s="55" t="s">
+      <c r="T8" s="57"/>
+      <c r="U8" s="57"/>
+      <c r="W8" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="X8" s="55"/>
+      <c r="X8" s="61"/>
     </row>
     <row r="9" spans="5:24" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E9" s="56"/>
-      <c r="F9" s="59"/>
-      <c r="G9" s="59"/>
-      <c r="H9" s="59"/>
-      <c r="I9" s="59"/>
-      <c r="J9" s="59"/>
-      <c r="K9" s="59"/>
-      <c r="L9" s="59"/>
-      <c r="M9" s="59"/>
-      <c r="N9" s="59"/>
-      <c r="O9" s="59"/>
-      <c r="P9" s="59"/>
-      <c r="Q9" s="59"/>
-      <c r="S9" s="56"/>
-      <c r="T9" s="56"/>
-      <c r="U9" s="56"/>
-      <c r="W9" s="55"/>
-      <c r="X9" s="55"/>
+      <c r="E9" s="57"/>
+      <c r="F9" s="60"/>
+      <c r="G9" s="60"/>
+      <c r="H9" s="60"/>
+      <c r="I9" s="60"/>
+      <c r="J9" s="60"/>
+      <c r="K9" s="60"/>
+      <c r="L9" s="60"/>
+      <c r="M9" s="60"/>
+      <c r="N9" s="60"/>
+      <c r="O9" s="60"/>
+      <c r="P9" s="60"/>
+      <c r="Q9" s="60"/>
+      <c r="S9" s="57"/>
+      <c r="T9" s="57"/>
+      <c r="U9" s="57"/>
+      <c r="W9" s="61"/>
+      <c r="X9" s="61"/>
     </row>
     <row r="10" spans="5:24" x14ac:dyDescent="0.25">
-      <c r="E10" s="56">
+      <c r="E10" s="57">
         <v>3</v>
       </c>
-      <c r="F10" s="58" t="s">
+      <c r="F10" s="59" t="s">
         <v>53</v>
       </c>
-      <c r="G10" s="59"/>
-      <c r="H10" s="59"/>
-      <c r="I10" s="58" t="s">
+      <c r="G10" s="60"/>
+      <c r="H10" s="60"/>
+      <c r="I10" s="59" t="s">
         <v>64</v>
       </c>
-      <c r="J10" s="59"/>
-      <c r="K10" s="59"/>
-      <c r="L10" s="59"/>
-      <c r="M10" s="59"/>
-      <c r="N10" s="59"/>
-      <c r="O10" s="59"/>
-      <c r="P10" s="59"/>
-      <c r="Q10" s="59"/>
-      <c r="S10" s="57" t="s">
+      <c r="J10" s="60"/>
+      <c r="K10" s="60"/>
+      <c r="L10" s="60"/>
+      <c r="M10" s="60"/>
+      <c r="N10" s="60"/>
+      <c r="O10" s="60"/>
+      <c r="P10" s="60"/>
+      <c r="Q10" s="60"/>
+      <c r="S10" s="58" t="s">
         <v>59</v>
       </c>
-      <c r="T10" s="56"/>
-      <c r="U10" s="56"/>
-      <c r="W10" s="55" t="s">
+      <c r="T10" s="57"/>
+      <c r="U10" s="57"/>
+      <c r="W10" s="61" t="s">
         <v>62</v>
       </c>
-      <c r="X10" s="55" t="s">
+      <c r="X10" s="61" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="11" spans="5:24" x14ac:dyDescent="0.25">
-      <c r="E11" s="56"/>
-      <c r="F11" s="59"/>
-      <c r="G11" s="59"/>
-      <c r="H11" s="59"/>
-      <c r="I11" s="59"/>
-      <c r="J11" s="59"/>
-      <c r="K11" s="59"/>
-      <c r="L11" s="59"/>
-      <c r="M11" s="59"/>
-      <c r="N11" s="59"/>
-      <c r="O11" s="59"/>
-      <c r="P11" s="59"/>
-      <c r="Q11" s="59"/>
-      <c r="S11" s="56"/>
-      <c r="T11" s="56"/>
-      <c r="U11" s="56"/>
-      <c r="W11" s="55"/>
-      <c r="X11" s="55"/>
+      <c r="E11" s="57"/>
+      <c r="F11" s="60"/>
+      <c r="G11" s="60"/>
+      <c r="H11" s="60"/>
+      <c r="I11" s="60"/>
+      <c r="J11" s="60"/>
+      <c r="K11" s="60"/>
+      <c r="L11" s="60"/>
+      <c r="M11" s="60"/>
+      <c r="N11" s="60"/>
+      <c r="O11" s="60"/>
+      <c r="P11" s="60"/>
+      <c r="Q11" s="60"/>
+      <c r="S11" s="57"/>
+      <c r="T11" s="57"/>
+      <c r="U11" s="57"/>
+      <c r="W11" s="61"/>
+      <c r="X11" s="61"/>
     </row>
     <row r="12" spans="5:24" x14ac:dyDescent="0.25">
-      <c r="E12" s="56"/>
-      <c r="F12" s="59"/>
-      <c r="G12" s="59"/>
-      <c r="H12" s="59"/>
-      <c r="I12" s="59"/>
-      <c r="J12" s="59"/>
-      <c r="K12" s="59"/>
-      <c r="L12" s="59"/>
-      <c r="M12" s="59"/>
-      <c r="N12" s="59"/>
-      <c r="O12" s="59"/>
-      <c r="P12" s="59"/>
-      <c r="Q12" s="59"/>
-      <c r="S12" s="56"/>
-      <c r="T12" s="56"/>
-      <c r="U12" s="56"/>
-      <c r="W12" s="55"/>
-      <c r="X12" s="55"/>
+      <c r="E12" s="57"/>
+      <c r="F12" s="60"/>
+      <c r="G12" s="60"/>
+      <c r="H12" s="60"/>
+      <c r="I12" s="60"/>
+      <c r="J12" s="60"/>
+      <c r="K12" s="60"/>
+      <c r="L12" s="60"/>
+      <c r="M12" s="60"/>
+      <c r="N12" s="60"/>
+      <c r="O12" s="60"/>
+      <c r="P12" s="60"/>
+      <c r="Q12" s="60"/>
+      <c r="S12" s="57"/>
+      <c r="T12" s="57"/>
+      <c r="U12" s="57"/>
+      <c r="W12" s="61"/>
+      <c r="X12" s="61"/>
     </row>
     <row r="13" spans="5:24" x14ac:dyDescent="0.25">
-      <c r="E13" s="56"/>
-      <c r="F13" s="59"/>
-      <c r="G13" s="59"/>
-      <c r="H13" s="59"/>
-      <c r="I13" s="59"/>
-      <c r="J13" s="59"/>
-      <c r="K13" s="59"/>
-      <c r="L13" s="59"/>
-      <c r="M13" s="59"/>
-      <c r="N13" s="59"/>
-      <c r="O13" s="59"/>
-      <c r="P13" s="59"/>
-      <c r="Q13" s="59"/>
-      <c r="S13" s="56"/>
-      <c r="T13" s="56"/>
-      <c r="U13" s="56"/>
-      <c r="W13" s="55"/>
-      <c r="X13" s="55"/>
+      <c r="E13" s="57"/>
+      <c r="F13" s="60"/>
+      <c r="G13" s="60"/>
+      <c r="H13" s="60"/>
+      <c r="I13" s="60"/>
+      <c r="J13" s="60"/>
+      <c r="K13" s="60"/>
+      <c r="L13" s="60"/>
+      <c r="M13" s="60"/>
+      <c r="N13" s="60"/>
+      <c r="O13" s="60"/>
+      <c r="P13" s="60"/>
+      <c r="Q13" s="60"/>
+      <c r="S13" s="57"/>
+      <c r="T13" s="57"/>
+      <c r="U13" s="57"/>
+      <c r="W13" s="61"/>
+      <c r="X13" s="61"/>
     </row>
     <row r="14" spans="5:24" x14ac:dyDescent="0.25">
-      <c r="E14" s="56"/>
-      <c r="F14" s="59"/>
-      <c r="G14" s="59"/>
-      <c r="H14" s="59"/>
-      <c r="I14" s="59"/>
-      <c r="J14" s="59"/>
-      <c r="K14" s="59"/>
-      <c r="L14" s="59"/>
-      <c r="M14" s="59"/>
-      <c r="N14" s="59"/>
-      <c r="O14" s="59"/>
-      <c r="P14" s="59"/>
-      <c r="Q14" s="59"/>
-      <c r="S14" s="56"/>
-      <c r="T14" s="56"/>
-      <c r="U14" s="56"/>
-      <c r="W14" s="55"/>
-      <c r="X14" s="55"/>
+      <c r="E14" s="57"/>
+      <c r="F14" s="60"/>
+      <c r="G14" s="60"/>
+      <c r="H14" s="60"/>
+      <c r="I14" s="60"/>
+      <c r="J14" s="60"/>
+      <c r="K14" s="60"/>
+      <c r="L14" s="60"/>
+      <c r="M14" s="60"/>
+      <c r="N14" s="60"/>
+      <c r="O14" s="60"/>
+      <c r="P14" s="60"/>
+      <c r="Q14" s="60"/>
+      <c r="S14" s="57"/>
+      <c r="T14" s="57"/>
+      <c r="U14" s="57"/>
+      <c r="W14" s="61"/>
+      <c r="X14" s="61"/>
     </row>
     <row r="15" spans="5:24" x14ac:dyDescent="0.25">
-      <c r="E15" s="56"/>
-      <c r="F15" s="59"/>
-      <c r="G15" s="59"/>
-      <c r="H15" s="59"/>
-      <c r="I15" s="59"/>
-      <c r="J15" s="59"/>
-      <c r="K15" s="59"/>
-      <c r="L15" s="59"/>
-      <c r="M15" s="59"/>
-      <c r="N15" s="59"/>
-      <c r="O15" s="59"/>
-      <c r="P15" s="59"/>
-      <c r="Q15" s="59"/>
-      <c r="S15" s="56"/>
-      <c r="T15" s="56"/>
-      <c r="U15" s="56"/>
-      <c r="W15" s="55"/>
-      <c r="X15" s="55"/>
+      <c r="E15" s="57"/>
+      <c r="F15" s="60"/>
+      <c r="G15" s="60"/>
+      <c r="H15" s="60"/>
+      <c r="I15" s="60"/>
+      <c r="J15" s="60"/>
+      <c r="K15" s="60"/>
+      <c r="L15" s="60"/>
+      <c r="M15" s="60"/>
+      <c r="N15" s="60"/>
+      <c r="O15" s="60"/>
+      <c r="P15" s="60"/>
+      <c r="Q15" s="60"/>
+      <c r="S15" s="57"/>
+      <c r="T15" s="57"/>
+      <c r="U15" s="57"/>
+      <c r="W15" s="61"/>
+      <c r="X15" s="61"/>
     </row>
     <row r="16" spans="5:24" x14ac:dyDescent="0.25">
-      <c r="E16" s="56"/>
-      <c r="F16" s="59"/>
-      <c r="G16" s="59"/>
-      <c r="H16" s="59"/>
-      <c r="I16" s="59"/>
-      <c r="J16" s="59"/>
-      <c r="K16" s="59"/>
-      <c r="L16" s="59"/>
-      <c r="M16" s="59"/>
-      <c r="N16" s="59"/>
-      <c r="O16" s="59"/>
-      <c r="P16" s="59"/>
-      <c r="Q16" s="59"/>
-      <c r="S16" s="56"/>
-      <c r="T16" s="56"/>
-      <c r="U16" s="56"/>
-      <c r="W16" s="55"/>
-      <c r="X16" s="55"/>
+      <c r="E16" s="57"/>
+      <c r="F16" s="60"/>
+      <c r="G16" s="60"/>
+      <c r="H16" s="60"/>
+      <c r="I16" s="60"/>
+      <c r="J16" s="60"/>
+      <c r="K16" s="60"/>
+      <c r="L16" s="60"/>
+      <c r="M16" s="60"/>
+      <c r="N16" s="60"/>
+      <c r="O16" s="60"/>
+      <c r="P16" s="60"/>
+      <c r="Q16" s="60"/>
+      <c r="S16" s="57"/>
+      <c r="T16" s="57"/>
+      <c r="U16" s="57"/>
+      <c r="W16" s="61"/>
+      <c r="X16" s="61"/>
     </row>
     <row r="17" spans="5:24" x14ac:dyDescent="0.25">
-      <c r="E17" s="56"/>
-      <c r="F17" s="59"/>
-      <c r="G17" s="59"/>
-      <c r="H17" s="59"/>
-      <c r="I17" s="59"/>
-      <c r="J17" s="59"/>
-      <c r="K17" s="59"/>
-      <c r="L17" s="59"/>
-      <c r="M17" s="59"/>
-      <c r="N17" s="59"/>
-      <c r="O17" s="59"/>
-      <c r="P17" s="59"/>
-      <c r="Q17" s="59"/>
-      <c r="S17" s="56"/>
-      <c r="T17" s="56"/>
-      <c r="U17" s="56"/>
-      <c r="W17" s="55"/>
-      <c r="X17" s="55"/>
+      <c r="E17" s="57"/>
+      <c r="F17" s="60"/>
+      <c r="G17" s="60"/>
+      <c r="H17" s="60"/>
+      <c r="I17" s="60"/>
+      <c r="J17" s="60"/>
+      <c r="K17" s="60"/>
+      <c r="L17" s="60"/>
+      <c r="M17" s="60"/>
+      <c r="N17" s="60"/>
+      <c r="O17" s="60"/>
+      <c r="P17" s="60"/>
+      <c r="Q17" s="60"/>
+      <c r="S17" s="57"/>
+      <c r="T17" s="57"/>
+      <c r="U17" s="57"/>
+      <c r="W17" s="61"/>
+      <c r="X17" s="61"/>
     </row>
     <row r="18" spans="5:24" x14ac:dyDescent="0.25">
-      <c r="E18" s="56"/>
-      <c r="F18" s="59"/>
-      <c r="G18" s="59"/>
-      <c r="H18" s="59"/>
-      <c r="I18" s="59"/>
-      <c r="J18" s="59"/>
-      <c r="K18" s="59"/>
-      <c r="L18" s="59"/>
-      <c r="M18" s="59"/>
-      <c r="N18" s="59"/>
-      <c r="O18" s="59"/>
-      <c r="P18" s="59"/>
-      <c r="Q18" s="59"/>
-      <c r="S18" s="56"/>
-      <c r="T18" s="56"/>
-      <c r="U18" s="56"/>
-      <c r="W18" s="55"/>
-      <c r="X18" s="55"/>
+      <c r="E18" s="57"/>
+      <c r="F18" s="60"/>
+      <c r="G18" s="60"/>
+      <c r="H18" s="60"/>
+      <c r="I18" s="60"/>
+      <c r="J18" s="60"/>
+      <c r="K18" s="60"/>
+      <c r="L18" s="60"/>
+      <c r="M18" s="60"/>
+      <c r="N18" s="60"/>
+      <c r="O18" s="60"/>
+      <c r="P18" s="60"/>
+      <c r="Q18" s="60"/>
+      <c r="S18" s="57"/>
+      <c r="T18" s="57"/>
+      <c r="U18" s="57"/>
+      <c r="W18" s="61"/>
+      <c r="X18" s="61"/>
     </row>
     <row r="19" spans="5:24" x14ac:dyDescent="0.25">
-      <c r="E19" s="56"/>
-      <c r="F19" s="59"/>
-      <c r="G19" s="59"/>
-      <c r="H19" s="59"/>
-      <c r="I19" s="59"/>
-      <c r="J19" s="59"/>
-      <c r="K19" s="59"/>
-      <c r="L19" s="59"/>
-      <c r="M19" s="59"/>
-      <c r="N19" s="59"/>
-      <c r="O19" s="59"/>
-      <c r="P19" s="59"/>
-      <c r="Q19" s="59"/>
-      <c r="S19" s="56"/>
-      <c r="T19" s="56"/>
-      <c r="U19" s="56"/>
-      <c r="W19" s="55"/>
-      <c r="X19" s="55"/>
+      <c r="E19" s="57"/>
+      <c r="F19" s="60"/>
+      <c r="G19" s="60"/>
+      <c r="H19" s="60"/>
+      <c r="I19" s="60"/>
+      <c r="J19" s="60"/>
+      <c r="K19" s="60"/>
+      <c r="L19" s="60"/>
+      <c r="M19" s="60"/>
+      <c r="N19" s="60"/>
+      <c r="O19" s="60"/>
+      <c r="P19" s="60"/>
+      <c r="Q19" s="60"/>
+      <c r="S19" s="57"/>
+      <c r="T19" s="57"/>
+      <c r="U19" s="57"/>
+      <c r="W19" s="61"/>
+      <c r="X19" s="61"/>
     </row>
     <row r="20" spans="5:24" x14ac:dyDescent="0.25">
-      <c r="E20" s="56"/>
-      <c r="F20" s="59"/>
-      <c r="G20" s="59"/>
-      <c r="H20" s="59"/>
-      <c r="I20" s="59"/>
-      <c r="J20" s="59"/>
-      <c r="K20" s="59"/>
-      <c r="L20" s="59"/>
-      <c r="M20" s="59"/>
-      <c r="N20" s="59"/>
-      <c r="O20" s="59"/>
-      <c r="P20" s="59"/>
-      <c r="Q20" s="59"/>
-      <c r="S20" s="56"/>
-      <c r="T20" s="56"/>
-      <c r="U20" s="56"/>
-      <c r="W20" s="55"/>
-      <c r="X20" s="55"/>
+      <c r="E20" s="57"/>
+      <c r="F20" s="60"/>
+      <c r="G20" s="60"/>
+      <c r="H20" s="60"/>
+      <c r="I20" s="60"/>
+      <c r="J20" s="60"/>
+      <c r="K20" s="60"/>
+      <c r="L20" s="60"/>
+      <c r="M20" s="60"/>
+      <c r="N20" s="60"/>
+      <c r="O20" s="60"/>
+      <c r="P20" s="60"/>
+      <c r="Q20" s="60"/>
+      <c r="S20" s="57"/>
+      <c r="T20" s="57"/>
+      <c r="U20" s="57"/>
+      <c r="W20" s="61"/>
+      <c r="X20" s="61"/>
     </row>
     <row r="21" spans="5:24" x14ac:dyDescent="0.25">
-      <c r="E21" s="56"/>
-      <c r="F21" s="59"/>
-      <c r="G21" s="59"/>
-      <c r="H21" s="59"/>
-      <c r="I21" s="59"/>
-      <c r="J21" s="59"/>
-      <c r="K21" s="59"/>
-      <c r="L21" s="59"/>
-      <c r="M21" s="59"/>
-      <c r="N21" s="59"/>
-      <c r="O21" s="59"/>
-      <c r="P21" s="59"/>
-      <c r="Q21" s="59"/>
-      <c r="S21" s="56"/>
-      <c r="T21" s="56"/>
-      <c r="U21" s="56"/>
-      <c r="W21" s="55"/>
-      <c r="X21" s="55"/>
+      <c r="E21" s="57"/>
+      <c r="F21" s="60"/>
+      <c r="G21" s="60"/>
+      <c r="H21" s="60"/>
+      <c r="I21" s="60"/>
+      <c r="J21" s="60"/>
+      <c r="K21" s="60"/>
+      <c r="L21" s="60"/>
+      <c r="M21" s="60"/>
+      <c r="N21" s="60"/>
+      <c r="O21" s="60"/>
+      <c r="P21" s="60"/>
+      <c r="Q21" s="60"/>
+      <c r="S21" s="57"/>
+      <c r="T21" s="57"/>
+      <c r="U21" s="57"/>
+      <c r="W21" s="61"/>
+      <c r="X21" s="61"/>
     </row>
     <row r="22" spans="5:24" x14ac:dyDescent="0.25">
-      <c r="E22" s="56"/>
-      <c r="F22" s="59"/>
-      <c r="G22" s="59"/>
-      <c r="H22" s="59"/>
-      <c r="I22" s="59"/>
-      <c r="J22" s="59"/>
-      <c r="K22" s="59"/>
-      <c r="L22" s="59"/>
-      <c r="M22" s="59"/>
-      <c r="N22" s="59"/>
-      <c r="O22" s="59"/>
-      <c r="P22" s="59"/>
-      <c r="Q22" s="59"/>
-      <c r="S22" s="56"/>
-      <c r="T22" s="56"/>
-      <c r="U22" s="56"/>
-      <c r="W22" s="55"/>
-      <c r="X22" s="55"/>
+      <c r="E22" s="57"/>
+      <c r="F22" s="60"/>
+      <c r="G22" s="60"/>
+      <c r="H22" s="60"/>
+      <c r="I22" s="60"/>
+      <c r="J22" s="60"/>
+      <c r="K22" s="60"/>
+      <c r="L22" s="60"/>
+      <c r="M22" s="60"/>
+      <c r="N22" s="60"/>
+      <c r="O22" s="60"/>
+      <c r="P22" s="60"/>
+      <c r="Q22" s="60"/>
+      <c r="S22" s="57"/>
+      <c r="T22" s="57"/>
+      <c r="U22" s="57"/>
+      <c r="W22" s="61"/>
+      <c r="X22" s="61"/>
     </row>
     <row r="23" spans="5:24" x14ac:dyDescent="0.25">
-      <c r="E23" s="56"/>
-      <c r="F23" s="59"/>
-      <c r="G23" s="59"/>
-      <c r="H23" s="59"/>
-      <c r="I23" s="59"/>
-      <c r="J23" s="59"/>
-      <c r="K23" s="59"/>
-      <c r="L23" s="59"/>
-      <c r="M23" s="59"/>
-      <c r="N23" s="59"/>
-      <c r="O23" s="59"/>
-      <c r="P23" s="59"/>
-      <c r="Q23" s="59"/>
-      <c r="S23" s="56"/>
-      <c r="T23" s="56"/>
-      <c r="U23" s="56"/>
-      <c r="W23" s="55"/>
-      <c r="X23" s="55"/>
+      <c r="E23" s="57"/>
+      <c r="F23" s="60"/>
+      <c r="G23" s="60"/>
+      <c r="H23" s="60"/>
+      <c r="I23" s="60"/>
+      <c r="J23" s="60"/>
+      <c r="K23" s="60"/>
+      <c r="L23" s="60"/>
+      <c r="M23" s="60"/>
+      <c r="N23" s="60"/>
+      <c r="O23" s="60"/>
+      <c r="P23" s="60"/>
+      <c r="Q23" s="60"/>
+      <c r="S23" s="57"/>
+      <c r="T23" s="57"/>
+      <c r="U23" s="57"/>
+      <c r="W23" s="61"/>
+      <c r="X23" s="61"/>
     </row>
     <row r="24" spans="5:24" x14ac:dyDescent="0.25">
-      <c r="E24" s="56"/>
-      <c r="F24" s="59"/>
-      <c r="G24" s="59"/>
-      <c r="H24" s="59"/>
-      <c r="I24" s="59"/>
-      <c r="J24" s="59"/>
-      <c r="K24" s="59"/>
-      <c r="L24" s="59"/>
-      <c r="M24" s="59"/>
-      <c r="N24" s="59"/>
-      <c r="O24" s="59"/>
-      <c r="P24" s="59"/>
-      <c r="Q24" s="59"/>
-      <c r="S24" s="56"/>
-      <c r="T24" s="56"/>
-      <c r="U24" s="56"/>
-      <c r="W24" s="55"/>
-      <c r="X24" s="55"/>
+      <c r="E24" s="57"/>
+      <c r="F24" s="60"/>
+      <c r="G24" s="60"/>
+      <c r="H24" s="60"/>
+      <c r="I24" s="60"/>
+      <c r="J24" s="60"/>
+      <c r="K24" s="60"/>
+      <c r="L24" s="60"/>
+      <c r="M24" s="60"/>
+      <c r="N24" s="60"/>
+      <c r="O24" s="60"/>
+      <c r="P24" s="60"/>
+      <c r="Q24" s="60"/>
+      <c r="S24" s="57"/>
+      <c r="T24" s="57"/>
+      <c r="U24" s="57"/>
+      <c r="W24" s="61"/>
+      <c r="X24" s="61"/>
     </row>
     <row r="25" spans="5:24" x14ac:dyDescent="0.25">
-      <c r="E25" s="56"/>
-      <c r="F25" s="59"/>
-      <c r="G25" s="59"/>
-      <c r="H25" s="59"/>
-      <c r="I25" s="59"/>
-      <c r="J25" s="59"/>
-      <c r="K25" s="59"/>
-      <c r="L25" s="59"/>
-      <c r="M25" s="59"/>
-      <c r="N25" s="59"/>
-      <c r="O25" s="59"/>
-      <c r="P25" s="59"/>
-      <c r="Q25" s="59"/>
-      <c r="S25" s="56"/>
-      <c r="T25" s="56"/>
-      <c r="U25" s="56"/>
-      <c r="W25" s="55"/>
-      <c r="X25" s="55"/>
+      <c r="E25" s="57"/>
+      <c r="F25" s="60"/>
+      <c r="G25" s="60"/>
+      <c r="H25" s="60"/>
+      <c r="I25" s="60"/>
+      <c r="J25" s="60"/>
+      <c r="K25" s="60"/>
+      <c r="L25" s="60"/>
+      <c r="M25" s="60"/>
+      <c r="N25" s="60"/>
+      <c r="O25" s="60"/>
+      <c r="P25" s="60"/>
+      <c r="Q25" s="60"/>
+      <c r="S25" s="57"/>
+      <c r="T25" s="57"/>
+      <c r="U25" s="57"/>
+      <c r="W25" s="61"/>
+      <c r="X25" s="61"/>
     </row>
     <row r="26" spans="5:24" x14ac:dyDescent="0.25">
-      <c r="E26" s="56"/>
-      <c r="F26" s="59"/>
-      <c r="G26" s="59"/>
-      <c r="H26" s="59"/>
-      <c r="I26" s="59"/>
-      <c r="J26" s="59"/>
-      <c r="K26" s="59"/>
-      <c r="L26" s="59"/>
-      <c r="M26" s="59"/>
-      <c r="N26" s="59"/>
-      <c r="O26" s="59"/>
-      <c r="P26" s="59"/>
-      <c r="Q26" s="59"/>
-      <c r="S26" s="56"/>
-      <c r="T26" s="56"/>
-      <c r="U26" s="56"/>
-      <c r="W26" s="55"/>
-      <c r="X26" s="55"/>
+      <c r="E26" s="57"/>
+      <c r="F26" s="60"/>
+      <c r="G26" s="60"/>
+      <c r="H26" s="60"/>
+      <c r="I26" s="60"/>
+      <c r="J26" s="60"/>
+      <c r="K26" s="60"/>
+      <c r="L26" s="60"/>
+      <c r="M26" s="60"/>
+      <c r="N26" s="60"/>
+      <c r="O26" s="60"/>
+      <c r="P26" s="60"/>
+      <c r="Q26" s="60"/>
+      <c r="S26" s="57"/>
+      <c r="T26" s="57"/>
+      <c r="U26" s="57"/>
+      <c r="W26" s="61"/>
+      <c r="X26" s="61"/>
     </row>
     <row r="27" spans="5:24" x14ac:dyDescent="0.25">
-      <c r="E27" s="56"/>
-      <c r="F27" s="59"/>
-      <c r="G27" s="59"/>
-      <c r="H27" s="59"/>
-      <c r="I27" s="59"/>
-      <c r="J27" s="59"/>
-      <c r="K27" s="59"/>
-      <c r="L27" s="59"/>
-      <c r="M27" s="59"/>
-      <c r="N27" s="59"/>
-      <c r="O27" s="59"/>
-      <c r="P27" s="59"/>
-      <c r="Q27" s="59"/>
-      <c r="S27" s="56"/>
-      <c r="T27" s="56"/>
-      <c r="U27" s="56"/>
-      <c r="W27" s="55"/>
-      <c r="X27" s="55"/>
+      <c r="E27" s="57"/>
+      <c r="F27" s="60"/>
+      <c r="G27" s="60"/>
+      <c r="H27" s="60"/>
+      <c r="I27" s="60"/>
+      <c r="J27" s="60"/>
+      <c r="K27" s="60"/>
+      <c r="L27" s="60"/>
+      <c r="M27" s="60"/>
+      <c r="N27" s="60"/>
+      <c r="O27" s="60"/>
+      <c r="P27" s="60"/>
+      <c r="Q27" s="60"/>
+      <c r="S27" s="57"/>
+      <c r="T27" s="57"/>
+      <c r="U27" s="57"/>
+      <c r="W27" s="61"/>
+      <c r="X27" s="61"/>
     </row>
     <row r="28" spans="5:24" x14ac:dyDescent="0.25">
-      <c r="E28" s="56"/>
-      <c r="F28" s="59"/>
-      <c r="G28" s="59"/>
-      <c r="H28" s="59"/>
-      <c r="I28" s="59"/>
-      <c r="J28" s="59"/>
-      <c r="K28" s="59"/>
-      <c r="L28" s="59"/>
-      <c r="M28" s="59"/>
-      <c r="N28" s="59"/>
-      <c r="O28" s="59"/>
-      <c r="P28" s="59"/>
-      <c r="Q28" s="59"/>
-      <c r="S28" s="56"/>
-      <c r="T28" s="56"/>
-      <c r="U28" s="56"/>
-      <c r="W28" s="55"/>
-      <c r="X28" s="55"/>
+      <c r="E28" s="57"/>
+      <c r="F28" s="60"/>
+      <c r="G28" s="60"/>
+      <c r="H28" s="60"/>
+      <c r="I28" s="60"/>
+      <c r="J28" s="60"/>
+      <c r="K28" s="60"/>
+      <c r="L28" s="60"/>
+      <c r="M28" s="60"/>
+      <c r="N28" s="60"/>
+      <c r="O28" s="60"/>
+      <c r="P28" s="60"/>
+      <c r="Q28" s="60"/>
+      <c r="S28" s="57"/>
+      <c r="T28" s="57"/>
+      <c r="U28" s="57"/>
+      <c r="W28" s="61"/>
+      <c r="X28" s="61"/>
     </row>
     <row r="29" spans="5:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E29" s="56">
+      <c r="E29" s="57">
         <v>4</v>
       </c>
-      <c r="F29" s="58" t="s">
+      <c r="F29" s="59" t="s">
         <v>54</v>
       </c>
-      <c r="G29" s="59"/>
-      <c r="H29" s="59"/>
-      <c r="I29" s="59"/>
-      <c r="J29" s="59"/>
-      <c r="K29" s="59"/>
-      <c r="L29" s="59"/>
-      <c r="M29" s="59"/>
-      <c r="N29" s="59"/>
-      <c r="O29" s="59"/>
-      <c r="P29" s="59"/>
-      <c r="Q29" s="59"/>
-      <c r="S29" s="56" t="s">
+      <c r="G29" s="60"/>
+      <c r="H29" s="60"/>
+      <c r="I29" s="60"/>
+      <c r="J29" s="60"/>
+      <c r="K29" s="60"/>
+      <c r="L29" s="60"/>
+      <c r="M29" s="60"/>
+      <c r="N29" s="60"/>
+      <c r="O29" s="60"/>
+      <c r="P29" s="60"/>
+      <c r="Q29" s="60"/>
+      <c r="S29" s="57" t="s">
         <v>58</v>
       </c>
-      <c r="T29" s="56"/>
-      <c r="U29" s="56"/>
-      <c r="W29" s="55" t="s">
+      <c r="T29" s="57"/>
+      <c r="U29" s="57"/>
+      <c r="W29" s="61" t="s">
         <v>65</v>
       </c>
-      <c r="X29" s="55"/>
+      <c r="X29" s="61"/>
     </row>
     <row r="30" spans="5:24" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E30" s="56"/>
-      <c r="F30" s="59"/>
-      <c r="G30" s="59"/>
-      <c r="H30" s="59"/>
-      <c r="I30" s="59"/>
-      <c r="J30" s="59"/>
-      <c r="K30" s="59"/>
-      <c r="L30" s="59"/>
-      <c r="M30" s="59"/>
-      <c r="N30" s="59"/>
-      <c r="O30" s="59"/>
-      <c r="P30" s="59"/>
-      <c r="Q30" s="59"/>
-      <c r="S30" s="56"/>
-      <c r="T30" s="56"/>
-      <c r="U30" s="56"/>
-      <c r="W30" s="55"/>
-      <c r="X30" s="55"/>
+      <c r="E30" s="57"/>
+      <c r="F30" s="60"/>
+      <c r="G30" s="60"/>
+      <c r="H30" s="60"/>
+      <c r="I30" s="60"/>
+      <c r="J30" s="60"/>
+      <c r="K30" s="60"/>
+      <c r="L30" s="60"/>
+      <c r="M30" s="60"/>
+      <c r="N30" s="60"/>
+      <c r="O30" s="60"/>
+      <c r="P30" s="60"/>
+      <c r="Q30" s="60"/>
+      <c r="S30" s="57"/>
+      <c r="T30" s="57"/>
+      <c r="U30" s="57"/>
+      <c r="W30" s="61"/>
+      <c r="X30" s="61"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="W3:X7"/>
+    <mergeCell ref="W8:X9"/>
+    <mergeCell ref="W29:X30"/>
+    <mergeCell ref="W10:W28"/>
+    <mergeCell ref="X10:X28"/>
     <mergeCell ref="S3:U7"/>
     <mergeCell ref="S8:U9"/>
     <mergeCell ref="S10:U28"/>
@@ -4149,11 +4163,6 @@
     <mergeCell ref="F10:H28"/>
     <mergeCell ref="I10:Q28"/>
     <mergeCell ref="F29:Q30"/>
-    <mergeCell ref="W3:X7"/>
-    <mergeCell ref="W8:X9"/>
-    <mergeCell ref="W29:X30"/>
-    <mergeCell ref="W10:W28"/>
-    <mergeCell ref="X10:X28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
nilai model dan migration xii rpl 2
</commit_message>
<xml_diff>
--- a/XIIRPL2(❁´◡`❁)(❁´◡`❁)(❁´◡`❁)(u‿ฺu✿ฺ)/DATA PRAKTIK XII RPl 2.xlsx
+++ b/XIIRPL2(❁´◡`❁)(❁´◡`❁)(❁´◡`❁)(u‿ฺu✿ฺ)/DATA PRAKTIK XII RPl 2.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\_01.AdeSetiyawan\01. Pembelajaran\pwpb2223\XIIRPL2(❁´◡`❁)(❁´◡`❁)(❁´◡`❁)(u‿ฺu✿ฺ)\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AdeSetiyawan)(✿◡‿◡)(✿◡‿◡)\XIIRPL2(❁´◡`❁)(❁´◡`❁)(❁´◡`❁)(u‿ฺu✿ฺ)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF39EEC9-6FDE-4001-A8DE-7AF317D9C4EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27A2450D-6900-4893-908B-BA1013A223E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{7A470BEC-FF9B-4C58-B3A9-6A89F2B6EB46}"/>
+    <workbookView xWindow="0" yWindow="9240" windowWidth="28800" windowHeight="6240" xr2:uid="{7A470BEC-FF9B-4C58-B3A9-6A89F2B6EB46}"/>
   </bookViews>
   <sheets>
     <sheet name="Nilai All" sheetId="1" r:id="rId1"/>
-    <sheet name="Soal Migration" sheetId="5" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="4" r:id="rId3"/>
-    <sheet name="Sesi 1" sheetId="3" r:id="rId4"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId5"/>
+    <sheet name="Sheet3" sheetId="6" r:id="rId2"/>
+    <sheet name="Soal Migration" sheetId="5" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
+    <sheet name="Sesi 1" sheetId="3" r:id="rId5"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Nilai All'!$E$1:$G$38</definedName>
@@ -27,21 +28,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="135">
   <si>
     <t xml:space="preserve">Nama </t>
   </si>
@@ -364,6 +356,93 @@
   </si>
   <si>
     <t>=  tbjual_kaos_bola  =</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DB </t>
+  </si>
+  <si>
+    <t xml:space="preserve">TABLE </t>
+  </si>
+  <si>
+    <t xml:space="preserve">soal </t>
+  </si>
+  <si>
+    <t>laravel</t>
+  </si>
+  <si>
+    <t>php artisan make:model aku -m (--migration)</t>
+  </si>
+  <si>
+    <t>akus</t>
+  </si>
+  <si>
+    <t>FIELD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nama field </t>
+  </si>
+  <si>
+    <t xml:space="preserve">primary key </t>
+  </si>
+  <si>
+    <t>type data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">id </t>
+  </si>
+  <si>
+    <t>PK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">int </t>
+  </si>
+  <si>
+    <t>$table-&gt;id();</t>
+  </si>
+  <si>
+    <t>bigInt</t>
+  </si>
+  <si>
+    <t>varchar</t>
+  </si>
+  <si>
+    <t>$table-&gt;string('tempatVaksin');</t>
+  </si>
+  <si>
+    <t>$table-&gt;string('jenisVaksin');</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>$table-&gt;date('tanggalVaksin);</t>
+  </si>
+  <si>
+    <t>create_at</t>
+  </si>
+  <si>
+    <t>update_at</t>
+  </si>
+  <si>
+    <t>nama db terserah kalian</t>
+  </si>
+  <si>
+    <t>tbberita</t>
+  </si>
+  <si>
+    <t>judulberita</t>
+  </si>
+  <si>
+    <t>tagberita</t>
+  </si>
+  <si>
+    <t>isiBerita</t>
+  </si>
+  <si>
+    <t>tanggalPublish</t>
+  </si>
+  <si>
+    <t>01.02.2023</t>
   </si>
 </sst>
 </file>
@@ -373,7 +452,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0&quot;%&quot;"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -421,6 +500,13 @@
     </font>
     <font>
       <sz val="36"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="48"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -733,7 +819,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -889,6 +975,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -901,8 +990,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1210,7 +1304,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1220,8 +1314,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E8966E4-2275-4E9F-82CA-974F40DBA593}">
   <dimension ref="B1:T1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1334,7 +1428,9 @@
       <c r="K3" s="34" t="s">
         <v>89</v>
       </c>
-      <c r="L3" s="34"/>
+      <c r="L3" s="34" t="s">
+        <v>134</v>
+      </c>
       <c r="M3" s="8"/>
       <c r="N3" s="8"/>
       <c r="O3" s="8"/>
@@ -1360,7 +1456,7 @@
       </c>
       <c r="F4" s="6">
         <f t="shared" ref="F4:F38" si="0">((SUM(G4:P4)*10)*70%)+(AVERAGE(Q4:R4)*30%)</f>
-        <v>38</v>
+        <v>43.949999999999996</v>
       </c>
       <c r="G4" s="10">
         <v>1</v>
@@ -1377,7 +1473,9 @@
       <c r="K4" s="10">
         <v>1</v>
       </c>
-      <c r="L4" s="10"/>
+      <c r="L4" s="10">
+        <v>0.85</v>
+      </c>
       <c r="M4" s="10"/>
       <c r="N4" s="10"/>
       <c r="O4" s="10"/>
@@ -1408,7 +1506,7 @@
       </c>
       <c r="F5" s="6">
         <f t="shared" si="0"/>
-        <v>48.25</v>
+        <v>54.55</v>
       </c>
       <c r="G5" s="10">
         <v>1</v>
@@ -1425,7 +1523,9 @@
       <c r="K5" s="10">
         <v>1</v>
       </c>
-      <c r="L5" s="10"/>
+      <c r="L5" s="10">
+        <v>0.9</v>
+      </c>
       <c r="M5" s="10"/>
       <c r="N5" s="10"/>
       <c r="O5" s="10"/>
@@ -1459,7 +1559,7 @@
       </c>
       <c r="F6" s="6">
         <f t="shared" si="0"/>
-        <v>24.5</v>
+        <v>30.799999999999997</v>
       </c>
       <c r="G6" s="10">
         <v>1</v>
@@ -1476,7 +1576,9 @@
       <c r="K6" s="10">
         <v>0</v>
       </c>
-      <c r="L6" s="10"/>
+      <c r="L6" s="10">
+        <v>0.9</v>
+      </c>
       <c r="M6" s="10"/>
       <c r="N6" s="10"/>
       <c r="O6" s="10"/>
@@ -1504,7 +1606,7 @@
       </c>
       <c r="F7" s="6">
         <f t="shared" si="0"/>
-        <v>48.25</v>
+        <v>55.25</v>
       </c>
       <c r="G7" s="10">
         <v>1</v>
@@ -1521,7 +1623,9 @@
       <c r="K7" s="10">
         <v>1</v>
       </c>
-      <c r="L7" s="10"/>
+      <c r="L7" s="10">
+        <v>1</v>
+      </c>
       <c r="M7" s="10"/>
       <c r="N7" s="10"/>
       <c r="O7" s="10"/>
@@ -1552,7 +1656,7 @@
       </c>
       <c r="F8" s="6">
         <f>((SUM(G8:P8)*10)*70%)+(AVERAGE(Q8:R8)*30%)</f>
-        <v>46.25</v>
+        <v>53.25</v>
       </c>
       <c r="G8" s="10">
         <v>1</v>
@@ -1569,7 +1673,9 @@
       <c r="K8" s="10">
         <v>1</v>
       </c>
-      <c r="L8" s="10"/>
+      <c r="L8" s="10">
+        <v>1</v>
+      </c>
       <c r="M8" s="10"/>
       <c r="N8" s="10"/>
       <c r="O8" s="10"/>
@@ -1634,7 +1740,7 @@
       </c>
       <c r="F10" s="6">
         <f t="shared" si="0"/>
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="G10" s="10">
         <v>1</v>
@@ -1651,7 +1757,9 @@
       <c r="K10" s="10">
         <v>1</v>
       </c>
-      <c r="L10" s="10"/>
+      <c r="L10" s="10">
+        <v>1</v>
+      </c>
       <c r="M10" s="10"/>
       <c r="N10" s="10"/>
       <c r="O10" s="10"/>
@@ -1682,7 +1790,7 @@
       </c>
       <c r="F11" s="6">
         <f t="shared" si="0"/>
-        <v>40.75</v>
+        <v>47.05</v>
       </c>
       <c r="G11" s="10">
         <v>1</v>
@@ -1699,7 +1807,9 @@
       <c r="K11" s="10">
         <v>1</v>
       </c>
-      <c r="L11" s="10"/>
+      <c r="L11" s="10">
+        <v>0.9</v>
+      </c>
       <c r="M11" s="10"/>
       <c r="N11" s="10"/>
       <c r="O11" s="10"/>
@@ -1733,7 +1843,7 @@
       </c>
       <c r="F12" s="6">
         <f t="shared" si="0"/>
-        <v>36.5</v>
+        <v>42.8</v>
       </c>
       <c r="G12" s="10">
         <v>1</v>
@@ -1750,7 +1860,9 @@
       <c r="K12" s="10">
         <v>0</v>
       </c>
-      <c r="L12" s="10"/>
+      <c r="L12" s="10">
+        <v>0.9</v>
+      </c>
       <c r="M12" s="10"/>
       <c r="N12" s="10"/>
       <c r="O12" s="10"/>
@@ -1829,7 +1941,7 @@
       </c>
       <c r="F14" s="6">
         <f t="shared" si="0"/>
-        <v>43.75</v>
+        <v>50.75</v>
       </c>
       <c r="G14" s="10">
         <v>1</v>
@@ -1846,7 +1958,9 @@
       <c r="K14" s="10">
         <v>1</v>
       </c>
-      <c r="L14" s="10"/>
+      <c r="L14" s="10">
+        <v>1</v>
+      </c>
       <c r="M14" s="10"/>
       <c r="N14" s="10"/>
       <c r="O14" s="10"/>
@@ -1877,7 +1991,7 @@
       </c>
       <c r="F15" s="6">
         <f t="shared" si="0"/>
-        <v>45.25</v>
+        <v>52.25</v>
       </c>
       <c r="G15" s="10">
         <v>1</v>
@@ -1894,7 +2008,9 @@
       <c r="K15" s="10">
         <v>1</v>
       </c>
-      <c r="L15" s="10"/>
+      <c r="L15" s="10">
+        <v>1</v>
+      </c>
       <c r="M15" s="10"/>
       <c r="N15" s="10"/>
       <c r="O15" s="10"/>
@@ -1945,7 +2061,9 @@
       <c r="K16" s="10">
         <v>0</v>
       </c>
-      <c r="L16" s="10"/>
+      <c r="L16" s="10">
+        <v>0</v>
+      </c>
       <c r="M16" s="10"/>
       <c r="N16" s="10"/>
       <c r="O16" s="10"/>
@@ -1976,7 +2094,7 @@
       </c>
       <c r="F17" s="6">
         <f t="shared" si="0"/>
-        <v>47.95</v>
+        <v>54.95</v>
       </c>
       <c r="G17" s="10">
         <v>1</v>
@@ -1993,7 +2111,9 @@
       <c r="K17" s="10">
         <v>1</v>
       </c>
-      <c r="L17" s="10"/>
+      <c r="L17" s="10">
+        <v>1</v>
+      </c>
       <c r="M17" s="10"/>
       <c r="N17" s="10"/>
       <c r="O17" s="10"/>
@@ -2075,7 +2195,7 @@
       </c>
       <c r="F19" s="6">
         <f t="shared" si="0"/>
-        <v>47.75</v>
+        <v>54.75</v>
       </c>
       <c r="G19" s="10">
         <v>1</v>
@@ -2092,7 +2212,9 @@
       <c r="K19" s="10">
         <v>1</v>
       </c>
-      <c r="L19" s="10"/>
+      <c r="L19" s="10">
+        <v>1</v>
+      </c>
       <c r="M19" s="10"/>
       <c r="N19" s="10"/>
       <c r="O19" s="10"/>
@@ -2126,7 +2248,7 @@
       </c>
       <c r="F20" s="6">
         <f t="shared" si="0"/>
-        <v>24.5</v>
+        <v>31.499999999999996</v>
       </c>
       <c r="G20" s="11">
         <v>1</v>
@@ -2143,7 +2265,9 @@
       <c r="K20" s="10">
         <v>0</v>
       </c>
-      <c r="L20" s="10"/>
+      <c r="L20" s="10">
+        <v>1</v>
+      </c>
       <c r="M20" s="10"/>
       <c r="N20" s="10"/>
       <c r="O20" s="10"/>
@@ -2171,7 +2295,7 @@
       </c>
       <c r="F21" s="6">
         <f t="shared" si="0"/>
-        <v>43.75</v>
+        <v>50.75</v>
       </c>
       <c r="G21" s="10">
         <v>1</v>
@@ -2188,7 +2312,9 @@
       <c r="K21" s="10">
         <v>1</v>
       </c>
-      <c r="L21" s="10"/>
+      <c r="L21" s="10">
+        <v>1</v>
+      </c>
       <c r="M21" s="10"/>
       <c r="N21" s="10"/>
       <c r="O21" s="10"/>
@@ -2219,7 +2345,7 @@
       </c>
       <c r="F22" s="6">
         <f t="shared" si="0"/>
-        <v>38</v>
+        <v>44.3</v>
       </c>
       <c r="G22" s="10">
         <v>1</v>
@@ -2236,7 +2362,9 @@
       <c r="K22" s="10">
         <v>0.5</v>
       </c>
-      <c r="L22" s="10"/>
+      <c r="L22" s="10">
+        <v>0.9</v>
+      </c>
       <c r="M22" s="10"/>
       <c r="N22" s="10"/>
       <c r="O22" s="10"/>
@@ -2318,7 +2446,7 @@
       </c>
       <c r="F24" s="6">
         <f t="shared" si="0"/>
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="G24" s="10">
         <v>1</v>
@@ -2335,7 +2463,9 @@
       <c r="K24" s="10">
         <v>0.75</v>
       </c>
-      <c r="L24" s="10"/>
+      <c r="L24" s="10">
+        <v>1</v>
+      </c>
       <c r="M24" s="10"/>
       <c r="N24" s="10"/>
       <c r="O24" s="10"/>
@@ -2366,7 +2496,7 @@
       </c>
       <c r="F25" s="6">
         <f t="shared" si="0"/>
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="G25" s="10">
         <v>1</v>
@@ -2383,7 +2513,9 @@
       <c r="K25" s="10">
         <v>1</v>
       </c>
-      <c r="L25" s="10"/>
+      <c r="L25" s="10">
+        <v>1</v>
+      </c>
       <c r="M25" s="10"/>
       <c r="N25" s="10"/>
       <c r="O25" s="10"/>
@@ -2462,7 +2594,7 @@
       </c>
       <c r="F27" s="6">
         <f t="shared" si="0"/>
-        <v>43.75</v>
+        <v>50.75</v>
       </c>
       <c r="G27" s="10">
         <v>1</v>
@@ -2479,7 +2611,9 @@
       <c r="K27" s="10">
         <v>1</v>
       </c>
-      <c r="L27" s="10"/>
+      <c r="L27" s="10">
+        <v>1</v>
+      </c>
       <c r="M27" s="10"/>
       <c r="N27" s="10"/>
       <c r="O27" s="10"/>
@@ -2510,7 +2644,7 @@
       </c>
       <c r="F28" s="6">
         <f t="shared" si="0"/>
-        <v>43.75</v>
+        <v>50.75</v>
       </c>
       <c r="G28" s="10">
         <v>1</v>
@@ -2527,7 +2661,9 @@
       <c r="K28" s="10">
         <v>1</v>
       </c>
-      <c r="L28" s="10"/>
+      <c r="L28" s="10">
+        <v>1</v>
+      </c>
       <c r="M28" s="10"/>
       <c r="N28" s="10"/>
       <c r="O28" s="10"/>
@@ -2558,7 +2694,7 @@
       </c>
       <c r="F29" s="6">
         <f t="shared" si="0"/>
-        <v>39.75</v>
+        <v>46.05</v>
       </c>
       <c r="G29" s="11">
         <v>1</v>
@@ -2575,7 +2711,9 @@
       <c r="K29" s="10">
         <v>0.75</v>
       </c>
-      <c r="L29" s="10"/>
+      <c r="L29" s="10">
+        <v>0.9</v>
+      </c>
       <c r="M29" s="10"/>
       <c r="N29" s="10"/>
       <c r="O29" s="10"/>
@@ -2606,7 +2744,7 @@
       </c>
       <c r="F30" s="6">
         <f t="shared" si="0"/>
-        <v>47.75</v>
+        <v>54.75</v>
       </c>
       <c r="G30" s="10">
         <v>1</v>
@@ -2623,7 +2761,9 @@
       <c r="K30" s="10">
         <v>1</v>
       </c>
-      <c r="L30" s="10"/>
+      <c r="L30" s="10">
+        <v>1</v>
+      </c>
       <c r="M30" s="10"/>
       <c r="N30" s="10"/>
       <c r="O30" s="10"/>
@@ -2654,7 +2794,7 @@
       </c>
       <c r="F31" s="6">
         <f t="shared" si="0"/>
-        <v>48.5</v>
+        <v>55.5</v>
       </c>
       <c r="G31" s="10">
         <v>1</v>
@@ -2671,7 +2811,9 @@
       <c r="K31" s="10">
         <v>1</v>
       </c>
-      <c r="L31" s="10"/>
+      <c r="L31" s="10">
+        <v>1</v>
+      </c>
       <c r="M31" s="10"/>
       <c r="N31" s="10"/>
       <c r="O31" s="10"/>
@@ -2702,7 +2844,7 @@
       </c>
       <c r="F32" s="6">
         <f t="shared" si="0"/>
-        <v>45.5</v>
+        <v>52.5</v>
       </c>
       <c r="G32" s="10">
         <v>1</v>
@@ -2719,7 +2861,9 @@
       <c r="K32" s="10">
         <v>1</v>
       </c>
-      <c r="L32" s="10"/>
+      <c r="L32" s="10">
+        <v>1</v>
+      </c>
       <c r="M32" s="10"/>
       <c r="N32" s="10"/>
       <c r="O32" s="10"/>
@@ -2750,7 +2894,7 @@
       </c>
       <c r="F33" s="6">
         <f t="shared" si="0"/>
-        <v>49.25</v>
+        <v>55.55</v>
       </c>
       <c r="G33" s="10">
         <v>1</v>
@@ -2767,7 +2911,9 @@
       <c r="K33" s="10">
         <v>1</v>
       </c>
-      <c r="L33" s="10"/>
+      <c r="L33" s="10">
+        <v>0.9</v>
+      </c>
       <c r="M33" s="10"/>
       <c r="N33" s="10"/>
       <c r="O33" s="10"/>
@@ -2798,7 +2944,7 @@
       </c>
       <c r="F34" s="6">
         <f t="shared" si="0"/>
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="G34" s="10">
         <v>1</v>
@@ -2815,7 +2961,9 @@
       <c r="K34" s="10">
         <v>1</v>
       </c>
-      <c r="L34" s="10"/>
+      <c r="L34" s="10">
+        <v>1</v>
+      </c>
       <c r="M34" s="10"/>
       <c r="N34" s="10"/>
       <c r="O34" s="10"/>
@@ -2846,7 +2994,7 @@
       </c>
       <c r="F35" s="6">
         <f t="shared" si="0"/>
-        <v>39.75</v>
+        <v>46.05</v>
       </c>
       <c r="G35" s="10">
         <v>1</v>
@@ -2863,7 +3011,9 @@
       <c r="K35" s="10">
         <v>0.75</v>
       </c>
-      <c r="L35" s="10"/>
+      <c r="L35" s="10">
+        <v>0.9</v>
+      </c>
       <c r="M35" s="10"/>
       <c r="N35" s="10"/>
       <c r="O35" s="10"/>
@@ -2894,7 +3044,7 @@
       </c>
       <c r="F36" s="6">
         <f t="shared" si="0"/>
-        <v>33.25</v>
+        <v>39.549999999999997</v>
       </c>
       <c r="G36" s="10">
         <v>1</v>
@@ -2911,7 +3061,9 @@
       <c r="K36" s="10">
         <v>1</v>
       </c>
-      <c r="L36" s="10"/>
+      <c r="L36" s="10">
+        <v>0.9</v>
+      </c>
       <c r="M36" s="10"/>
       <c r="N36" s="10"/>
       <c r="O36" s="10"/>
@@ -2939,7 +3091,7 @@
       </c>
       <c r="F37" s="6">
         <f t="shared" si="0"/>
-        <v>43.75</v>
+        <v>50.75</v>
       </c>
       <c r="G37" s="10">
         <v>1</v>
@@ -2956,7 +3108,9 @@
       <c r="K37" s="10">
         <v>0.75</v>
       </c>
-      <c r="L37" s="10"/>
+      <c r="L37" s="10">
+        <v>1</v>
+      </c>
       <c r="M37" s="10"/>
       <c r="N37" s="10"/>
       <c r="O37" s="10"/>
@@ -2990,7 +3144,7 @@
       </c>
       <c r="F38" s="6">
         <f t="shared" si="0"/>
-        <v>39.5</v>
+        <v>46.5</v>
       </c>
       <c r="G38" s="10">
         <v>1</v>
@@ -3007,7 +3161,9 @@
       <c r="K38" s="10">
         <v>0</v>
       </c>
-      <c r="L38" s="10"/>
+      <c r="L38" s="10">
+        <v>1</v>
+      </c>
       <c r="M38" s="10"/>
       <c r="N38" s="10"/>
       <c r="O38" s="10"/>
@@ -3047,9 +3203,9 @@
         <f t="shared" si="2"/>
         <v>73.529411764705884</v>
       </c>
-      <c r="L39" s="32" t="e">
+      <c r="L39" s="32">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>93.166666666666657</v>
       </c>
       <c r="M39" s="32" t="e">
         <f t="shared" si="2"/>
@@ -3199,6 +3355,152 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{272B4357-72D9-4FFA-86DA-5A8470DFA243}">
+  <dimension ref="B1:G12"/>
+  <sheetViews>
+    <sheetView topLeftCell="B5" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="40.7109375" defaultRowHeight="60" customHeight="1" x14ac:dyDescent="0.9"/>
+  <cols>
+    <col min="1" max="2" width="40.7109375" style="62"/>
+    <col min="3" max="3" width="55.5703125" style="62" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="50" style="62" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="38.85546875" style="62" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="48" style="62" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="0" style="62" hidden="1" customWidth="1"/>
+    <col min="8" max="16384" width="40.7109375" style="62"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:7" ht="60" hidden="1" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="B1" s="63" t="s">
+        <v>110</v>
+      </c>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="62" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="2:7" ht="60" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="B2" s="64" t="s">
+        <v>106</v>
+      </c>
+      <c r="C2" s="65" t="s">
+        <v>128</v>
+      </c>
+      <c r="D2" s="65"/>
+      <c r="E2" s="65"/>
+      <c r="F2" s="63"/>
+    </row>
+    <row r="3" spans="2:7" ht="60" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="C3" s="62" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" ht="60" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="B4" s="62" t="s">
+        <v>107</v>
+      </c>
+      <c r="C4" s="62" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" ht="60" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="B5" s="62" t="s">
+        <v>112</v>
+      </c>
+      <c r="C5" s="62" t="s">
+        <v>113</v>
+      </c>
+      <c r="D5" s="62" t="s">
+        <v>114</v>
+      </c>
+      <c r="E5" s="62" t="s">
+        <v>115</v>
+      </c>
+      <c r="F5" s="62" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" ht="60" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="C6" s="62" t="s">
+        <v>116</v>
+      </c>
+      <c r="D6" s="62" t="s">
+        <v>117</v>
+      </c>
+      <c r="E6" s="62" t="s">
+        <v>118</v>
+      </c>
+      <c r="F6" s="62" t="s">
+        <v>119</v>
+      </c>
+      <c r="G6" s="62" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" ht="60" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="C7" s="62" t="s">
+        <v>130</v>
+      </c>
+      <c r="E7" s="62" t="s">
+        <v>121</v>
+      </c>
+      <c r="F7" s="62" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" ht="60" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="C8" s="62" t="s">
+        <v>131</v>
+      </c>
+      <c r="E8" s="62" t="s">
+        <v>121</v>
+      </c>
+      <c r="F8" s="62" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" ht="60" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="C9" s="62" t="s">
+        <v>132</v>
+      </c>
+      <c r="E9" s="62" t="s">
+        <v>121</v>
+      </c>
+      <c r="F9" s="62" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" ht="60" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="C10" s="62" t="s">
+        <v>133</v>
+      </c>
+      <c r="E10" s="62" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" ht="60" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="C11" s="62" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" ht="60" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="C12" s="62" t="s">
+        <v>127</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F32B9B9-AE73-473C-AE26-D53E54D53E5A}">
   <dimension ref="A1:B38"/>
   <sheetViews>
@@ -3374,7 +3676,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{715B0C13-179F-4FD8-B66D-ED38FCC03D1C}">
   <dimension ref="B5:B6"/>
   <sheetViews>
@@ -3399,7 +3701,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{153E42C8-D1FE-4E64-96D9-EED2206D80DB}">
   <dimension ref="A1:M10"/>
   <sheetViews>
@@ -3519,7 +3821,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD728A97-A86D-4319-B892-289BC7014D66}">
   <dimension ref="E2:X30"/>
   <sheetViews>
@@ -3548,608 +3850,603 @@
       <c r="Q2" s="2"/>
     </row>
     <row r="3" spans="5:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E3" s="57">
-        <v>1</v>
-      </c>
-      <c r="F3" s="59" t="s">
+      <c r="E3" s="58">
+        <v>1</v>
+      </c>
+      <c r="F3" s="60" t="s">
         <v>51</v>
       </c>
-      <c r="G3" s="60"/>
-      <c r="H3" s="60"/>
-      <c r="I3" s="60"/>
-      <c r="J3" s="60"/>
-      <c r="K3" s="60"/>
-      <c r="L3" s="60"/>
-      <c r="M3" s="60"/>
-      <c r="N3" s="60"/>
-      <c r="O3" s="60"/>
-      <c r="P3" s="60"/>
-      <c r="Q3" s="60"/>
-      <c r="S3" s="57" t="s">
+      <c r="G3" s="61"/>
+      <c r="H3" s="61"/>
+      <c r="I3" s="61"/>
+      <c r="J3" s="61"/>
+      <c r="K3" s="61"/>
+      <c r="L3" s="61"/>
+      <c r="M3" s="61"/>
+      <c r="N3" s="61"/>
+      <c r="O3" s="61"/>
+      <c r="P3" s="61"/>
+      <c r="Q3" s="61"/>
+      <c r="S3" s="58" t="s">
         <v>58</v>
       </c>
-      <c r="T3" s="57"/>
-      <c r="U3" s="57"/>
-      <c r="W3" s="61" t="s">
+      <c r="T3" s="58"/>
+      <c r="U3" s="58"/>
+      <c r="W3" s="57" t="s">
         <v>60</v>
       </c>
-      <c r="X3" s="61"/>
+      <c r="X3" s="57"/>
     </row>
     <row r="4" spans="5:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E4" s="57"/>
-      <c r="F4" s="60"/>
-      <c r="G4" s="60"/>
-      <c r="H4" s="60"/>
-      <c r="I4" s="60"/>
-      <c r="J4" s="60"/>
-      <c r="K4" s="60"/>
-      <c r="L4" s="60"/>
-      <c r="M4" s="60"/>
-      <c r="N4" s="60"/>
-      <c r="O4" s="60"/>
-      <c r="P4" s="60"/>
-      <c r="Q4" s="60"/>
-      <c r="S4" s="57"/>
-      <c r="T4" s="57"/>
-      <c r="U4" s="57"/>
-      <c r="W4" s="61"/>
-      <c r="X4" s="61"/>
+      <c r="E4" s="58"/>
+      <c r="F4" s="61"/>
+      <c r="G4" s="61"/>
+      <c r="H4" s="61"/>
+      <c r="I4" s="61"/>
+      <c r="J4" s="61"/>
+      <c r="K4" s="61"/>
+      <c r="L4" s="61"/>
+      <c r="M4" s="61"/>
+      <c r="N4" s="61"/>
+      <c r="O4" s="61"/>
+      <c r="P4" s="61"/>
+      <c r="Q4" s="61"/>
+      <c r="S4" s="58"/>
+      <c r="T4" s="58"/>
+      <c r="U4" s="58"/>
+      <c r="W4" s="57"/>
+      <c r="X4" s="57"/>
     </row>
     <row r="5" spans="5:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E5" s="57"/>
-      <c r="F5" s="60"/>
-      <c r="G5" s="60"/>
-      <c r="H5" s="60"/>
-      <c r="I5" s="60"/>
-      <c r="J5" s="60"/>
-      <c r="K5" s="60"/>
-      <c r="L5" s="60"/>
-      <c r="M5" s="60"/>
-      <c r="N5" s="60"/>
-      <c r="O5" s="60"/>
-      <c r="P5" s="60"/>
-      <c r="Q5" s="60"/>
-      <c r="S5" s="57"/>
-      <c r="T5" s="57"/>
-      <c r="U5" s="57"/>
-      <c r="W5" s="61"/>
-      <c r="X5" s="61"/>
+      <c r="E5" s="58"/>
+      <c r="F5" s="61"/>
+      <c r="G5" s="61"/>
+      <c r="H5" s="61"/>
+      <c r="I5" s="61"/>
+      <c r="J5" s="61"/>
+      <c r="K5" s="61"/>
+      <c r="L5" s="61"/>
+      <c r="M5" s="61"/>
+      <c r="N5" s="61"/>
+      <c r="O5" s="61"/>
+      <c r="P5" s="61"/>
+      <c r="Q5" s="61"/>
+      <c r="S5" s="58"/>
+      <c r="T5" s="58"/>
+      <c r="U5" s="58"/>
+      <c r="W5" s="57"/>
+      <c r="X5" s="57"/>
     </row>
     <row r="6" spans="5:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E6" s="57"/>
-      <c r="F6" s="60"/>
-      <c r="G6" s="60"/>
-      <c r="H6" s="60"/>
-      <c r="I6" s="60"/>
-      <c r="J6" s="60"/>
-      <c r="K6" s="60"/>
-      <c r="L6" s="60"/>
-      <c r="M6" s="60"/>
-      <c r="N6" s="60"/>
-      <c r="O6" s="60"/>
-      <c r="P6" s="60"/>
-      <c r="Q6" s="60"/>
-      <c r="S6" s="57"/>
-      <c r="T6" s="57"/>
-      <c r="U6" s="57"/>
-      <c r="W6" s="61"/>
-      <c r="X6" s="61"/>
+      <c r="E6" s="58"/>
+      <c r="F6" s="61"/>
+      <c r="G6" s="61"/>
+      <c r="H6" s="61"/>
+      <c r="I6" s="61"/>
+      <c r="J6" s="61"/>
+      <c r="K6" s="61"/>
+      <c r="L6" s="61"/>
+      <c r="M6" s="61"/>
+      <c r="N6" s="61"/>
+      <c r="O6" s="61"/>
+      <c r="P6" s="61"/>
+      <c r="Q6" s="61"/>
+      <c r="S6" s="58"/>
+      <c r="T6" s="58"/>
+      <c r="U6" s="58"/>
+      <c r="W6" s="57"/>
+      <c r="X6" s="57"/>
     </row>
     <row r="7" spans="5:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E7" s="57"/>
-      <c r="F7" s="60"/>
-      <c r="G7" s="60"/>
-      <c r="H7" s="60"/>
-      <c r="I7" s="60"/>
-      <c r="J7" s="60"/>
-      <c r="K7" s="60"/>
-      <c r="L7" s="60"/>
-      <c r="M7" s="60"/>
-      <c r="N7" s="60"/>
-      <c r="O7" s="60"/>
-      <c r="P7" s="60"/>
-      <c r="Q7" s="60"/>
-      <c r="S7" s="57"/>
-      <c r="T7" s="57"/>
-      <c r="U7" s="57"/>
-      <c r="W7" s="61"/>
-      <c r="X7" s="61"/>
+      <c r="E7" s="58"/>
+      <c r="F7" s="61"/>
+      <c r="G7" s="61"/>
+      <c r="H7" s="61"/>
+      <c r="I7" s="61"/>
+      <c r="J7" s="61"/>
+      <c r="K7" s="61"/>
+      <c r="L7" s="61"/>
+      <c r="M7" s="61"/>
+      <c r="N7" s="61"/>
+      <c r="O7" s="61"/>
+      <c r="P7" s="61"/>
+      <c r="Q7" s="61"/>
+      <c r="S7" s="58"/>
+      <c r="T7" s="58"/>
+      <c r="U7" s="58"/>
+      <c r="W7" s="57"/>
+      <c r="X7" s="57"/>
     </row>
     <row r="8" spans="5:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E8" s="57">
+      <c r="E8" s="58">
         <v>2</v>
       </c>
-      <c r="F8" s="59" t="s">
+      <c r="F8" s="60" t="s">
         <v>52</v>
       </c>
-      <c r="G8" s="60"/>
-      <c r="H8" s="60"/>
-      <c r="I8" s="60"/>
-      <c r="J8" s="60"/>
-      <c r="K8" s="60"/>
-      <c r="L8" s="60"/>
-      <c r="M8" s="60"/>
-      <c r="N8" s="60"/>
-      <c r="O8" s="60"/>
-      <c r="P8" s="60"/>
-      <c r="Q8" s="60"/>
-      <c r="S8" s="57" t="s">
+      <c r="G8" s="61"/>
+      <c r="H8" s="61"/>
+      <c r="I8" s="61"/>
+      <c r="J8" s="61"/>
+      <c r="K8" s="61"/>
+      <c r="L8" s="61"/>
+      <c r="M8" s="61"/>
+      <c r="N8" s="61"/>
+      <c r="O8" s="61"/>
+      <c r="P8" s="61"/>
+      <c r="Q8" s="61"/>
+      <c r="S8" s="58" t="s">
         <v>58</v>
       </c>
-      <c r="T8" s="57"/>
-      <c r="U8" s="57"/>
-      <c r="W8" s="61" t="s">
+      <c r="T8" s="58"/>
+      <c r="U8" s="58"/>
+      <c r="W8" s="57" t="s">
         <v>61</v>
       </c>
-      <c r="X8" s="61"/>
+      <c r="X8" s="57"/>
     </row>
     <row r="9" spans="5:24" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E9" s="57"/>
-      <c r="F9" s="60"/>
-      <c r="G9" s="60"/>
-      <c r="H9" s="60"/>
-      <c r="I9" s="60"/>
-      <c r="J9" s="60"/>
-      <c r="K9" s="60"/>
-      <c r="L9" s="60"/>
-      <c r="M9" s="60"/>
-      <c r="N9" s="60"/>
-      <c r="O9" s="60"/>
-      <c r="P9" s="60"/>
-      <c r="Q9" s="60"/>
-      <c r="S9" s="57"/>
-      <c r="T9" s="57"/>
-      <c r="U9" s="57"/>
-      <c r="W9" s="61"/>
-      <c r="X9" s="61"/>
+      <c r="E9" s="58"/>
+      <c r="F9" s="61"/>
+      <c r="G9" s="61"/>
+      <c r="H9" s="61"/>
+      <c r="I9" s="61"/>
+      <c r="J9" s="61"/>
+      <c r="K9" s="61"/>
+      <c r="L9" s="61"/>
+      <c r="M9" s="61"/>
+      <c r="N9" s="61"/>
+      <c r="O9" s="61"/>
+      <c r="P9" s="61"/>
+      <c r="Q9" s="61"/>
+      <c r="S9" s="58"/>
+      <c r="T9" s="58"/>
+      <c r="U9" s="58"/>
+      <c r="W9" s="57"/>
+      <c r="X9" s="57"/>
     </row>
     <row r="10" spans="5:24" x14ac:dyDescent="0.25">
-      <c r="E10" s="57">
+      <c r="E10" s="58">
         <v>3</v>
       </c>
-      <c r="F10" s="59" t="s">
+      <c r="F10" s="60" t="s">
         <v>53</v>
       </c>
-      <c r="G10" s="60"/>
-      <c r="H10" s="60"/>
-      <c r="I10" s="59" t="s">
+      <c r="G10" s="61"/>
+      <c r="H10" s="61"/>
+      <c r="I10" s="60" t="s">
         <v>64</v>
       </c>
-      <c r="J10" s="60"/>
-      <c r="K10" s="60"/>
-      <c r="L10" s="60"/>
-      <c r="M10" s="60"/>
-      <c r="N10" s="60"/>
-      <c r="O10" s="60"/>
-      <c r="P10" s="60"/>
-      <c r="Q10" s="60"/>
-      <c r="S10" s="58" t="s">
+      <c r="J10" s="61"/>
+      <c r="K10" s="61"/>
+      <c r="L10" s="61"/>
+      <c r="M10" s="61"/>
+      <c r="N10" s="61"/>
+      <c r="O10" s="61"/>
+      <c r="P10" s="61"/>
+      <c r="Q10" s="61"/>
+      <c r="S10" s="59" t="s">
         <v>59</v>
       </c>
-      <c r="T10" s="57"/>
-      <c r="U10" s="57"/>
-      <c r="W10" s="61" t="s">
+      <c r="T10" s="58"/>
+      <c r="U10" s="58"/>
+      <c r="W10" s="57" t="s">
         <v>62</v>
       </c>
-      <c r="X10" s="61" t="s">
+      <c r="X10" s="57" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="11" spans="5:24" x14ac:dyDescent="0.25">
-      <c r="E11" s="57"/>
-      <c r="F11" s="60"/>
-      <c r="G11" s="60"/>
-      <c r="H11" s="60"/>
-      <c r="I11" s="60"/>
-      <c r="J11" s="60"/>
-      <c r="K11" s="60"/>
-      <c r="L11" s="60"/>
-      <c r="M11" s="60"/>
-      <c r="N11" s="60"/>
-      <c r="O11" s="60"/>
-      <c r="P11" s="60"/>
-      <c r="Q11" s="60"/>
-      <c r="S11" s="57"/>
-      <c r="T11" s="57"/>
-      <c r="U11" s="57"/>
-      <c r="W11" s="61"/>
-      <c r="X11" s="61"/>
+      <c r="E11" s="58"/>
+      <c r="F11" s="61"/>
+      <c r="G11" s="61"/>
+      <c r="H11" s="61"/>
+      <c r="I11" s="61"/>
+      <c r="J11" s="61"/>
+      <c r="K11" s="61"/>
+      <c r="L11" s="61"/>
+      <c r="M11" s="61"/>
+      <c r="N11" s="61"/>
+      <c r="O11" s="61"/>
+      <c r="P11" s="61"/>
+      <c r="Q11" s="61"/>
+      <c r="S11" s="58"/>
+      <c r="T11" s="58"/>
+      <c r="U11" s="58"/>
+      <c r="W11" s="57"/>
+      <c r="X11" s="57"/>
     </row>
     <row r="12" spans="5:24" x14ac:dyDescent="0.25">
-      <c r="E12" s="57"/>
-      <c r="F12" s="60"/>
-      <c r="G12" s="60"/>
-      <c r="H12" s="60"/>
-      <c r="I12" s="60"/>
-      <c r="J12" s="60"/>
-      <c r="K12" s="60"/>
-      <c r="L12" s="60"/>
-      <c r="M12" s="60"/>
-      <c r="N12" s="60"/>
-      <c r="O12" s="60"/>
-      <c r="P12" s="60"/>
-      <c r="Q12" s="60"/>
-      <c r="S12" s="57"/>
-      <c r="T12" s="57"/>
-      <c r="U12" s="57"/>
-      <c r="W12" s="61"/>
-      <c r="X12" s="61"/>
+      <c r="E12" s="58"/>
+      <c r="F12" s="61"/>
+      <c r="G12" s="61"/>
+      <c r="H12" s="61"/>
+      <c r="I12" s="61"/>
+      <c r="J12" s="61"/>
+      <c r="K12" s="61"/>
+      <c r="L12" s="61"/>
+      <c r="M12" s="61"/>
+      <c r="N12" s="61"/>
+      <c r="O12" s="61"/>
+      <c r="P12" s="61"/>
+      <c r="Q12" s="61"/>
+      <c r="S12" s="58"/>
+      <c r="T12" s="58"/>
+      <c r="U12" s="58"/>
+      <c r="W12" s="57"/>
+      <c r="X12" s="57"/>
     </row>
     <row r="13" spans="5:24" x14ac:dyDescent="0.25">
-      <c r="E13" s="57"/>
-      <c r="F13" s="60"/>
-      <c r="G13" s="60"/>
-      <c r="H13" s="60"/>
-      <c r="I13" s="60"/>
-      <c r="J13" s="60"/>
-      <c r="K13" s="60"/>
-      <c r="L13" s="60"/>
-      <c r="M13" s="60"/>
-      <c r="N13" s="60"/>
-      <c r="O13" s="60"/>
-      <c r="P13" s="60"/>
-      <c r="Q13" s="60"/>
-      <c r="S13" s="57"/>
-      <c r="T13" s="57"/>
-      <c r="U13" s="57"/>
-      <c r="W13" s="61"/>
-      <c r="X13" s="61"/>
+      <c r="E13" s="58"/>
+      <c r="F13" s="61"/>
+      <c r="G13" s="61"/>
+      <c r="H13" s="61"/>
+      <c r="I13" s="61"/>
+      <c r="J13" s="61"/>
+      <c r="K13" s="61"/>
+      <c r="L13" s="61"/>
+      <c r="M13" s="61"/>
+      <c r="N13" s="61"/>
+      <c r="O13" s="61"/>
+      <c r="P13" s="61"/>
+      <c r="Q13" s="61"/>
+      <c r="S13" s="58"/>
+      <c r="T13" s="58"/>
+      <c r="U13" s="58"/>
+      <c r="W13" s="57"/>
+      <c r="X13" s="57"/>
     </row>
     <row r="14" spans="5:24" x14ac:dyDescent="0.25">
-      <c r="E14" s="57"/>
-      <c r="F14" s="60"/>
-      <c r="G14" s="60"/>
-      <c r="H14" s="60"/>
-      <c r="I14" s="60"/>
-      <c r="J14" s="60"/>
-      <c r="K14" s="60"/>
-      <c r="L14" s="60"/>
-      <c r="M14" s="60"/>
-      <c r="N14" s="60"/>
-      <c r="O14" s="60"/>
-      <c r="P14" s="60"/>
-      <c r="Q14" s="60"/>
-      <c r="S14" s="57"/>
-      <c r="T14" s="57"/>
-      <c r="U14" s="57"/>
-      <c r="W14" s="61"/>
-      <c r="X14" s="61"/>
+      <c r="E14" s="58"/>
+      <c r="F14" s="61"/>
+      <c r="G14" s="61"/>
+      <c r="H14" s="61"/>
+      <c r="I14" s="61"/>
+      <c r="J14" s="61"/>
+      <c r="K14" s="61"/>
+      <c r="L14" s="61"/>
+      <c r="M14" s="61"/>
+      <c r="N14" s="61"/>
+      <c r="O14" s="61"/>
+      <c r="P14" s="61"/>
+      <c r="Q14" s="61"/>
+      <c r="S14" s="58"/>
+      <c r="T14" s="58"/>
+      <c r="U14" s="58"/>
+      <c r="W14" s="57"/>
+      <c r="X14" s="57"/>
     </row>
     <row r="15" spans="5:24" x14ac:dyDescent="0.25">
-      <c r="E15" s="57"/>
-      <c r="F15" s="60"/>
-      <c r="G15" s="60"/>
-      <c r="H15" s="60"/>
-      <c r="I15" s="60"/>
-      <c r="J15" s="60"/>
-      <c r="K15" s="60"/>
-      <c r="L15" s="60"/>
-      <c r="M15" s="60"/>
-      <c r="N15" s="60"/>
-      <c r="O15" s="60"/>
-      <c r="P15" s="60"/>
-      <c r="Q15" s="60"/>
-      <c r="S15" s="57"/>
-      <c r="T15" s="57"/>
-      <c r="U15" s="57"/>
-      <c r="W15" s="61"/>
-      <c r="X15" s="61"/>
+      <c r="E15" s="58"/>
+      <c r="F15" s="61"/>
+      <c r="G15" s="61"/>
+      <c r="H15" s="61"/>
+      <c r="I15" s="61"/>
+      <c r="J15" s="61"/>
+      <c r="K15" s="61"/>
+      <c r="L15" s="61"/>
+      <c r="M15" s="61"/>
+      <c r="N15" s="61"/>
+      <c r="O15" s="61"/>
+      <c r="P15" s="61"/>
+      <c r="Q15" s="61"/>
+      <c r="S15" s="58"/>
+      <c r="T15" s="58"/>
+      <c r="U15" s="58"/>
+      <c r="W15" s="57"/>
+      <c r="X15" s="57"/>
     </row>
     <row r="16" spans="5:24" x14ac:dyDescent="0.25">
-      <c r="E16" s="57"/>
-      <c r="F16" s="60"/>
-      <c r="G16" s="60"/>
-      <c r="H16" s="60"/>
-      <c r="I16" s="60"/>
-      <c r="J16" s="60"/>
-      <c r="K16" s="60"/>
-      <c r="L16" s="60"/>
-      <c r="M16" s="60"/>
-      <c r="N16" s="60"/>
-      <c r="O16" s="60"/>
-      <c r="P16" s="60"/>
-      <c r="Q16" s="60"/>
-      <c r="S16" s="57"/>
-      <c r="T16" s="57"/>
-      <c r="U16" s="57"/>
-      <c r="W16" s="61"/>
-      <c r="X16" s="61"/>
+      <c r="E16" s="58"/>
+      <c r="F16" s="61"/>
+      <c r="G16" s="61"/>
+      <c r="H16" s="61"/>
+      <c r="I16" s="61"/>
+      <c r="J16" s="61"/>
+      <c r="K16" s="61"/>
+      <c r="L16" s="61"/>
+      <c r="M16" s="61"/>
+      <c r="N16" s="61"/>
+      <c r="O16" s="61"/>
+      <c r="P16" s="61"/>
+      <c r="Q16" s="61"/>
+      <c r="S16" s="58"/>
+      <c r="T16" s="58"/>
+      <c r="U16" s="58"/>
+      <c r="W16" s="57"/>
+      <c r="X16" s="57"/>
     </row>
     <row r="17" spans="5:24" x14ac:dyDescent="0.25">
-      <c r="E17" s="57"/>
-      <c r="F17" s="60"/>
-      <c r="G17" s="60"/>
-      <c r="H17" s="60"/>
-      <c r="I17" s="60"/>
-      <c r="J17" s="60"/>
-      <c r="K17" s="60"/>
-      <c r="L17" s="60"/>
-      <c r="M17" s="60"/>
-      <c r="N17" s="60"/>
-      <c r="O17" s="60"/>
-      <c r="P17" s="60"/>
-      <c r="Q17" s="60"/>
-      <c r="S17" s="57"/>
-      <c r="T17" s="57"/>
-      <c r="U17" s="57"/>
-      <c r="W17" s="61"/>
-      <c r="X17" s="61"/>
+      <c r="E17" s="58"/>
+      <c r="F17" s="61"/>
+      <c r="G17" s="61"/>
+      <c r="H17" s="61"/>
+      <c r="I17" s="61"/>
+      <c r="J17" s="61"/>
+      <c r="K17" s="61"/>
+      <c r="L17" s="61"/>
+      <c r="M17" s="61"/>
+      <c r="N17" s="61"/>
+      <c r="O17" s="61"/>
+      <c r="P17" s="61"/>
+      <c r="Q17" s="61"/>
+      <c r="S17" s="58"/>
+      <c r="T17" s="58"/>
+      <c r="U17" s="58"/>
+      <c r="W17" s="57"/>
+      <c r="X17" s="57"/>
     </row>
     <row r="18" spans="5:24" x14ac:dyDescent="0.25">
-      <c r="E18" s="57"/>
-      <c r="F18" s="60"/>
-      <c r="G18" s="60"/>
-      <c r="H18" s="60"/>
-      <c r="I18" s="60"/>
-      <c r="J18" s="60"/>
-      <c r="K18" s="60"/>
-      <c r="L18" s="60"/>
-      <c r="M18" s="60"/>
-      <c r="N18" s="60"/>
-      <c r="O18" s="60"/>
-      <c r="P18" s="60"/>
-      <c r="Q18" s="60"/>
-      <c r="S18" s="57"/>
-      <c r="T18" s="57"/>
-      <c r="U18" s="57"/>
-      <c r="W18" s="61"/>
-      <c r="X18" s="61"/>
+      <c r="E18" s="58"/>
+      <c r="F18" s="61"/>
+      <c r="G18" s="61"/>
+      <c r="H18" s="61"/>
+      <c r="I18" s="61"/>
+      <c r="J18" s="61"/>
+      <c r="K18" s="61"/>
+      <c r="L18" s="61"/>
+      <c r="M18" s="61"/>
+      <c r="N18" s="61"/>
+      <c r="O18" s="61"/>
+      <c r="P18" s="61"/>
+      <c r="Q18" s="61"/>
+      <c r="S18" s="58"/>
+      <c r="T18" s="58"/>
+      <c r="U18" s="58"/>
+      <c r="W18" s="57"/>
+      <c r="X18" s="57"/>
     </row>
     <row r="19" spans="5:24" x14ac:dyDescent="0.25">
-      <c r="E19" s="57"/>
-      <c r="F19" s="60"/>
-      <c r="G19" s="60"/>
-      <c r="H19" s="60"/>
-      <c r="I19" s="60"/>
-      <c r="J19" s="60"/>
-      <c r="K19" s="60"/>
-      <c r="L19" s="60"/>
-      <c r="M19" s="60"/>
-      <c r="N19" s="60"/>
-      <c r="O19" s="60"/>
-      <c r="P19" s="60"/>
-      <c r="Q19" s="60"/>
-      <c r="S19" s="57"/>
-      <c r="T19" s="57"/>
-      <c r="U19" s="57"/>
-      <c r="W19" s="61"/>
-      <c r="X19" s="61"/>
+      <c r="E19" s="58"/>
+      <c r="F19" s="61"/>
+      <c r="G19" s="61"/>
+      <c r="H19" s="61"/>
+      <c r="I19" s="61"/>
+      <c r="J19" s="61"/>
+      <c r="K19" s="61"/>
+      <c r="L19" s="61"/>
+      <c r="M19" s="61"/>
+      <c r="N19" s="61"/>
+      <c r="O19" s="61"/>
+      <c r="P19" s="61"/>
+      <c r="Q19" s="61"/>
+      <c r="S19" s="58"/>
+      <c r="T19" s="58"/>
+      <c r="U19" s="58"/>
+      <c r="W19" s="57"/>
+      <c r="X19" s="57"/>
     </row>
     <row r="20" spans="5:24" x14ac:dyDescent="0.25">
-      <c r="E20" s="57"/>
-      <c r="F20" s="60"/>
-      <c r="G20" s="60"/>
-      <c r="H20" s="60"/>
-      <c r="I20" s="60"/>
-      <c r="J20" s="60"/>
-      <c r="K20" s="60"/>
-      <c r="L20" s="60"/>
-      <c r="M20" s="60"/>
-      <c r="N20" s="60"/>
-      <c r="O20" s="60"/>
-      <c r="P20" s="60"/>
-      <c r="Q20" s="60"/>
-      <c r="S20" s="57"/>
-      <c r="T20" s="57"/>
-      <c r="U20" s="57"/>
-      <c r="W20" s="61"/>
-      <c r="X20" s="61"/>
+      <c r="E20" s="58"/>
+      <c r="F20" s="61"/>
+      <c r="G20" s="61"/>
+      <c r="H20" s="61"/>
+      <c r="I20" s="61"/>
+      <c r="J20" s="61"/>
+      <c r="K20" s="61"/>
+      <c r="L20" s="61"/>
+      <c r="M20" s="61"/>
+      <c r="N20" s="61"/>
+      <c r="O20" s="61"/>
+      <c r="P20" s="61"/>
+      <c r="Q20" s="61"/>
+      <c r="S20" s="58"/>
+      <c r="T20" s="58"/>
+      <c r="U20" s="58"/>
+      <c r="W20" s="57"/>
+      <c r="X20" s="57"/>
     </row>
     <row r="21" spans="5:24" x14ac:dyDescent="0.25">
-      <c r="E21" s="57"/>
-      <c r="F21" s="60"/>
-      <c r="G21" s="60"/>
-      <c r="H21" s="60"/>
-      <c r="I21" s="60"/>
-      <c r="J21" s="60"/>
-      <c r="K21" s="60"/>
-      <c r="L21" s="60"/>
-      <c r="M21" s="60"/>
-      <c r="N21" s="60"/>
-      <c r="O21" s="60"/>
-      <c r="P21" s="60"/>
-      <c r="Q21" s="60"/>
-      <c r="S21" s="57"/>
-      <c r="T21" s="57"/>
-      <c r="U21" s="57"/>
-      <c r="W21" s="61"/>
-      <c r="X21" s="61"/>
+      <c r="E21" s="58"/>
+      <c r="F21" s="61"/>
+      <c r="G21" s="61"/>
+      <c r="H21" s="61"/>
+      <c r="I21" s="61"/>
+      <c r="J21" s="61"/>
+      <c r="K21" s="61"/>
+      <c r="L21" s="61"/>
+      <c r="M21" s="61"/>
+      <c r="N21" s="61"/>
+      <c r="O21" s="61"/>
+      <c r="P21" s="61"/>
+      <c r="Q21" s="61"/>
+      <c r="S21" s="58"/>
+      <c r="T21" s="58"/>
+      <c r="U21" s="58"/>
+      <c r="W21" s="57"/>
+      <c r="X21" s="57"/>
     </row>
     <row r="22" spans="5:24" x14ac:dyDescent="0.25">
-      <c r="E22" s="57"/>
-      <c r="F22" s="60"/>
-      <c r="G22" s="60"/>
-      <c r="H22" s="60"/>
-      <c r="I22" s="60"/>
-      <c r="J22" s="60"/>
-      <c r="K22" s="60"/>
-      <c r="L22" s="60"/>
-      <c r="M22" s="60"/>
-      <c r="N22" s="60"/>
-      <c r="O22" s="60"/>
-      <c r="P22" s="60"/>
-      <c r="Q22" s="60"/>
-      <c r="S22" s="57"/>
-      <c r="T22" s="57"/>
-      <c r="U22" s="57"/>
-      <c r="W22" s="61"/>
-      <c r="X22" s="61"/>
+      <c r="E22" s="58"/>
+      <c r="F22" s="61"/>
+      <c r="G22" s="61"/>
+      <c r="H22" s="61"/>
+      <c r="I22" s="61"/>
+      <c r="J22" s="61"/>
+      <c r="K22" s="61"/>
+      <c r="L22" s="61"/>
+      <c r="M22" s="61"/>
+      <c r="N22" s="61"/>
+      <c r="O22" s="61"/>
+      <c r="P22" s="61"/>
+      <c r="Q22" s="61"/>
+      <c r="S22" s="58"/>
+      <c r="T22" s="58"/>
+      <c r="U22" s="58"/>
+      <c r="W22" s="57"/>
+      <c r="X22" s="57"/>
     </row>
     <row r="23" spans="5:24" x14ac:dyDescent="0.25">
-      <c r="E23" s="57"/>
-      <c r="F23" s="60"/>
-      <c r="G23" s="60"/>
-      <c r="H23" s="60"/>
-      <c r="I23" s="60"/>
-      <c r="J23" s="60"/>
-      <c r="K23" s="60"/>
-      <c r="L23" s="60"/>
-      <c r="M23" s="60"/>
-      <c r="N23" s="60"/>
-      <c r="O23" s="60"/>
-      <c r="P23" s="60"/>
-      <c r="Q23" s="60"/>
-      <c r="S23" s="57"/>
-      <c r="T23" s="57"/>
-      <c r="U23" s="57"/>
-      <c r="W23" s="61"/>
-      <c r="X23" s="61"/>
+      <c r="E23" s="58"/>
+      <c r="F23" s="61"/>
+      <c r="G23" s="61"/>
+      <c r="H23" s="61"/>
+      <c r="I23" s="61"/>
+      <c r="J23" s="61"/>
+      <c r="K23" s="61"/>
+      <c r="L23" s="61"/>
+      <c r="M23" s="61"/>
+      <c r="N23" s="61"/>
+      <c r="O23" s="61"/>
+      <c r="P23" s="61"/>
+      <c r="Q23" s="61"/>
+      <c r="S23" s="58"/>
+      <c r="T23" s="58"/>
+      <c r="U23" s="58"/>
+      <c r="W23" s="57"/>
+      <c r="X23" s="57"/>
     </row>
     <row r="24" spans="5:24" x14ac:dyDescent="0.25">
-      <c r="E24" s="57"/>
-      <c r="F24" s="60"/>
-      <c r="G24" s="60"/>
-      <c r="H24" s="60"/>
-      <c r="I24" s="60"/>
-      <c r="J24" s="60"/>
-      <c r="K24" s="60"/>
-      <c r="L24" s="60"/>
-      <c r="M24" s="60"/>
-      <c r="N24" s="60"/>
-      <c r="O24" s="60"/>
-      <c r="P24" s="60"/>
-      <c r="Q24" s="60"/>
-      <c r="S24" s="57"/>
-      <c r="T24" s="57"/>
-      <c r="U24" s="57"/>
-      <c r="W24" s="61"/>
-      <c r="X24" s="61"/>
+      <c r="E24" s="58"/>
+      <c r="F24" s="61"/>
+      <c r="G24" s="61"/>
+      <c r="H24" s="61"/>
+      <c r="I24" s="61"/>
+      <c r="J24" s="61"/>
+      <c r="K24" s="61"/>
+      <c r="L24" s="61"/>
+      <c r="M24" s="61"/>
+      <c r="N24" s="61"/>
+      <c r="O24" s="61"/>
+      <c r="P24" s="61"/>
+      <c r="Q24" s="61"/>
+      <c r="S24" s="58"/>
+      <c r="T24" s="58"/>
+      <c r="U24" s="58"/>
+      <c r="W24" s="57"/>
+      <c r="X24" s="57"/>
     </row>
     <row r="25" spans="5:24" x14ac:dyDescent="0.25">
-      <c r="E25" s="57"/>
-      <c r="F25" s="60"/>
-      <c r="G25" s="60"/>
-      <c r="H25" s="60"/>
-      <c r="I25" s="60"/>
-      <c r="J25" s="60"/>
-      <c r="K25" s="60"/>
-      <c r="L25" s="60"/>
-      <c r="M25" s="60"/>
-      <c r="N25" s="60"/>
-      <c r="O25" s="60"/>
-      <c r="P25" s="60"/>
-      <c r="Q25" s="60"/>
-      <c r="S25" s="57"/>
-      <c r="T25" s="57"/>
-      <c r="U25" s="57"/>
-      <c r="W25" s="61"/>
-      <c r="X25" s="61"/>
+      <c r="E25" s="58"/>
+      <c r="F25" s="61"/>
+      <c r="G25" s="61"/>
+      <c r="H25" s="61"/>
+      <c r="I25" s="61"/>
+      <c r="J25" s="61"/>
+      <c r="K25" s="61"/>
+      <c r="L25" s="61"/>
+      <c r="M25" s="61"/>
+      <c r="N25" s="61"/>
+      <c r="O25" s="61"/>
+      <c r="P25" s="61"/>
+      <c r="Q25" s="61"/>
+      <c r="S25" s="58"/>
+      <c r="T25" s="58"/>
+      <c r="U25" s="58"/>
+      <c r="W25" s="57"/>
+      <c r="X25" s="57"/>
     </row>
     <row r="26" spans="5:24" x14ac:dyDescent="0.25">
-      <c r="E26" s="57"/>
-      <c r="F26" s="60"/>
-      <c r="G26" s="60"/>
-      <c r="H26" s="60"/>
-      <c r="I26" s="60"/>
-      <c r="J26" s="60"/>
-      <c r="K26" s="60"/>
-      <c r="L26" s="60"/>
-      <c r="M26" s="60"/>
-      <c r="N26" s="60"/>
-      <c r="O26" s="60"/>
-      <c r="P26" s="60"/>
-      <c r="Q26" s="60"/>
-      <c r="S26" s="57"/>
-      <c r="T26" s="57"/>
-      <c r="U26" s="57"/>
-      <c r="W26" s="61"/>
-      <c r="X26" s="61"/>
+      <c r="E26" s="58"/>
+      <c r="F26" s="61"/>
+      <c r="G26" s="61"/>
+      <c r="H26" s="61"/>
+      <c r="I26" s="61"/>
+      <c r="J26" s="61"/>
+      <c r="K26" s="61"/>
+      <c r="L26" s="61"/>
+      <c r="M26" s="61"/>
+      <c r="N26" s="61"/>
+      <c r="O26" s="61"/>
+      <c r="P26" s="61"/>
+      <c r="Q26" s="61"/>
+      <c r="S26" s="58"/>
+      <c r="T26" s="58"/>
+      <c r="U26" s="58"/>
+      <c r="W26" s="57"/>
+      <c r="X26" s="57"/>
     </row>
     <row r="27" spans="5:24" x14ac:dyDescent="0.25">
-      <c r="E27" s="57"/>
-      <c r="F27" s="60"/>
-      <c r="G27" s="60"/>
-      <c r="H27" s="60"/>
-      <c r="I27" s="60"/>
-      <c r="J27" s="60"/>
-      <c r="K27" s="60"/>
-      <c r="L27" s="60"/>
-      <c r="M27" s="60"/>
-      <c r="N27" s="60"/>
-      <c r="O27" s="60"/>
-      <c r="P27" s="60"/>
-      <c r="Q27" s="60"/>
-      <c r="S27" s="57"/>
-      <c r="T27" s="57"/>
-      <c r="U27" s="57"/>
-      <c r="W27" s="61"/>
-      <c r="X27" s="61"/>
+      <c r="E27" s="58"/>
+      <c r="F27" s="61"/>
+      <c r="G27" s="61"/>
+      <c r="H27" s="61"/>
+      <c r="I27" s="61"/>
+      <c r="J27" s="61"/>
+      <c r="K27" s="61"/>
+      <c r="L27" s="61"/>
+      <c r="M27" s="61"/>
+      <c r="N27" s="61"/>
+      <c r="O27" s="61"/>
+      <c r="P27" s="61"/>
+      <c r="Q27" s="61"/>
+      <c r="S27" s="58"/>
+      <c r="T27" s="58"/>
+      <c r="U27" s="58"/>
+      <c r="W27" s="57"/>
+      <c r="X27" s="57"/>
     </row>
     <row r="28" spans="5:24" x14ac:dyDescent="0.25">
-      <c r="E28" s="57"/>
-      <c r="F28" s="60"/>
-      <c r="G28" s="60"/>
-      <c r="H28" s="60"/>
-      <c r="I28" s="60"/>
-      <c r="J28" s="60"/>
-      <c r="K28" s="60"/>
-      <c r="L28" s="60"/>
-      <c r="M28" s="60"/>
-      <c r="N28" s="60"/>
-      <c r="O28" s="60"/>
-      <c r="P28" s="60"/>
-      <c r="Q28" s="60"/>
-      <c r="S28" s="57"/>
-      <c r="T28" s="57"/>
-      <c r="U28" s="57"/>
-      <c r="W28" s="61"/>
-      <c r="X28" s="61"/>
+      <c r="E28" s="58"/>
+      <c r="F28" s="61"/>
+      <c r="G28" s="61"/>
+      <c r="H28" s="61"/>
+      <c r="I28" s="61"/>
+      <c r="J28" s="61"/>
+      <c r="K28" s="61"/>
+      <c r="L28" s="61"/>
+      <c r="M28" s="61"/>
+      <c r="N28" s="61"/>
+      <c r="O28" s="61"/>
+      <c r="P28" s="61"/>
+      <c r="Q28" s="61"/>
+      <c r="S28" s="58"/>
+      <c r="T28" s="58"/>
+      <c r="U28" s="58"/>
+      <c r="W28" s="57"/>
+      <c r="X28" s="57"/>
     </row>
     <row r="29" spans="5:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E29" s="57">
+      <c r="E29" s="58">
         <v>4</v>
       </c>
-      <c r="F29" s="59" t="s">
+      <c r="F29" s="60" t="s">
         <v>54</v>
       </c>
-      <c r="G29" s="60"/>
-      <c r="H29" s="60"/>
-      <c r="I29" s="60"/>
-      <c r="J29" s="60"/>
-      <c r="K29" s="60"/>
-      <c r="L29" s="60"/>
-      <c r="M29" s="60"/>
-      <c r="N29" s="60"/>
-      <c r="O29" s="60"/>
-      <c r="P29" s="60"/>
-      <c r="Q29" s="60"/>
-      <c r="S29" s="57" t="s">
+      <c r="G29" s="61"/>
+      <c r="H29" s="61"/>
+      <c r="I29" s="61"/>
+      <c r="J29" s="61"/>
+      <c r="K29" s="61"/>
+      <c r="L29" s="61"/>
+      <c r="M29" s="61"/>
+      <c r="N29" s="61"/>
+      <c r="O29" s="61"/>
+      <c r="P29" s="61"/>
+      <c r="Q29" s="61"/>
+      <c r="S29" s="58" t="s">
         <v>58</v>
       </c>
-      <c r="T29" s="57"/>
-      <c r="U29" s="57"/>
-      <c r="W29" s="61" t="s">
+      <c r="T29" s="58"/>
+      <c r="U29" s="58"/>
+      <c r="W29" s="57" t="s">
         <v>65</v>
       </c>
-      <c r="X29" s="61"/>
+      <c r="X29" s="57"/>
     </row>
     <row r="30" spans="5:24" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E30" s="57"/>
-      <c r="F30" s="60"/>
-      <c r="G30" s="60"/>
-      <c r="H30" s="60"/>
-      <c r="I30" s="60"/>
-      <c r="J30" s="60"/>
-      <c r="K30" s="60"/>
-      <c r="L30" s="60"/>
-      <c r="M30" s="60"/>
-      <c r="N30" s="60"/>
-      <c r="O30" s="60"/>
-      <c r="P30" s="60"/>
-      <c r="Q30" s="60"/>
-      <c r="S30" s="57"/>
-      <c r="T30" s="57"/>
-      <c r="U30" s="57"/>
-      <c r="W30" s="61"/>
-      <c r="X30" s="61"/>
+      <c r="E30" s="58"/>
+      <c r="F30" s="61"/>
+      <c r="G30" s="61"/>
+      <c r="H30" s="61"/>
+      <c r="I30" s="61"/>
+      <c r="J30" s="61"/>
+      <c r="K30" s="61"/>
+      <c r="L30" s="61"/>
+      <c r="M30" s="61"/>
+      <c r="N30" s="61"/>
+      <c r="O30" s="61"/>
+      <c r="P30" s="61"/>
+      <c r="Q30" s="61"/>
+      <c r="S30" s="58"/>
+      <c r="T30" s="58"/>
+      <c r="U30" s="58"/>
+      <c r="W30" s="57"/>
+      <c r="X30" s="57"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="W3:X7"/>
-    <mergeCell ref="W8:X9"/>
-    <mergeCell ref="W29:X30"/>
-    <mergeCell ref="W10:W28"/>
-    <mergeCell ref="X10:X28"/>
     <mergeCell ref="S3:U7"/>
     <mergeCell ref="S8:U9"/>
     <mergeCell ref="S10:U28"/>
@@ -4163,6 +4460,11 @@
     <mergeCell ref="F10:H28"/>
     <mergeCell ref="I10:Q28"/>
     <mergeCell ref="F29:Q30"/>
+    <mergeCell ref="W3:X7"/>
+    <mergeCell ref="W8:X9"/>
+    <mergeCell ref="W29:X30"/>
+    <mergeCell ref="W10:W28"/>
+    <mergeCell ref="X10:X28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update nilai xii rpl 2
</commit_message>
<xml_diff>
--- a/XIIRPL2(❁´◡`❁)(❁´◡`❁)(❁´◡`❁)(u‿ฺu✿ฺ)/DATA PRAKTIK XII RPl 2.xlsx
+++ b/XIIRPL2(❁´◡`❁)(❁´◡`❁)(❁´◡`❁)(u‿ฺu✿ฺ)/DATA PRAKTIK XII RPl 2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AdeSetiyawan)(✿◡‿◡)(✿◡‿◡)\XIIRPL2(❁´◡`❁)(❁´◡`❁)(❁´◡`❁)(u‿ฺu✿ฺ)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27A2450D-6900-4893-908B-BA1013A223E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A3AB07F-4CCE-4221-B8D0-28FDFD19503E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="9240" windowWidth="28800" windowHeight="6240" xr2:uid="{7A470BEC-FF9B-4C58-B3A9-6A89F2B6EB46}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{7A470BEC-FF9B-4C58-B3A9-6A89F2B6EB46}"/>
   </bookViews>
   <sheets>
     <sheet name="Nilai All" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="140">
   <si>
     <t xml:space="preserve">Nama </t>
   </si>
@@ -310,9 +310,6 @@
     <t>25.01.2023</t>
   </si>
   <si>
-    <t>25,01,23 (sakit)</t>
-  </si>
-  <si>
     <t>25,01,23 Ijin Kelas Karir</t>
   </si>
   <si>
@@ -427,22 +424,41 @@
     <t>nama db terserah kalian</t>
   </si>
   <si>
-    <t>tbberita</t>
-  </si>
-  <si>
-    <t>judulberita</t>
-  </si>
-  <si>
-    <t>tagberita</t>
-  </si>
-  <si>
-    <t>isiBerita</t>
-  </si>
-  <si>
-    <t>tanggalPublish</t>
-  </si>
-  <si>
     <t>01.02.2023</t>
+  </si>
+  <si>
+    <t>tbalbum</t>
+  </si>
+  <si>
+    <t>namaFoto</t>
+  </si>
+  <si>
+    <t>lokasiFoto</t>
+  </si>
+  <si>
+    <t>tanggalFoto</t>
+  </si>
+  <si>
+    <t>jenisFileFoto</t>
+  </si>
+  <si>
+    <t>25,01,23 (sakit)
+1.2.2023 (sakit)</t>
+  </si>
+  <si>
+    <t>nama_lengkap</t>
+  </si>
+  <si>
+    <t>tanggal_lahir</t>
+  </si>
+  <si>
+    <t>tempat_lahir</t>
+  </si>
+  <si>
+    <t>jenisKelamin</t>
+  </si>
+  <si>
+    <t>tbbiodata</t>
   </si>
 </sst>
 </file>
@@ -819,7 +835,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -909,87 +925,6 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
@@ -998,6 +933,91 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1304,7 +1324,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1314,8 +1334,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E8966E4-2275-4E9F-82CA-974F40DBA593}">
   <dimension ref="B1:T1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1335,51 +1355,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="C1" s="39" t="s">
+      <c r="C1" s="43" t="s">
         <v>57</v>
       </c>
-      <c r="D1" s="40" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="43" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" s="43" t="s">
+      <c r="D1" s="44" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="47" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="53" t="s">
+      <c r="G1" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="55" t="s">
+      <c r="H1" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="55"/>
-      <c r="J1" s="55"/>
-      <c r="K1" s="51" t="s">
+      <c r="I1" s="59"/>
+      <c r="J1" s="59"/>
+      <c r="K1" s="55" t="s">
         <v>49</v>
       </c>
-      <c r="L1" s="52"/>
-      <c r="M1" s="52"/>
-      <c r="N1" s="52"/>
-      <c r="O1" s="52"/>
-      <c r="P1" s="52"/>
-      <c r="Q1" s="46" t="s">
+      <c r="L1" s="56"/>
+      <c r="M1" s="56"/>
+      <c r="N1" s="56"/>
+      <c r="O1" s="56"/>
+      <c r="P1" s="56"/>
+      <c r="Q1" s="50" t="s">
         <v>66</v>
       </c>
-      <c r="R1" s="46" t="s">
+      <c r="R1" s="50" t="s">
         <v>67</v>
       </c>
-      <c r="S1" s="37" t="s">
+      <c r="S1" s="41" t="s">
         <v>76</v>
       </c>
-      <c r="T1" s="38"/>
+      <c r="T1" s="42"/>
     </row>
     <row r="2" spans="2:20" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="39"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="54"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="58"/>
       <c r="H2" s="15" t="s">
         <v>10</v>
       </c>
@@ -1407,36 +1427,36 @@
       <c r="P2" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="Q2" s="47"/>
-      <c r="R2" s="46"/>
-      <c r="S2" s="37"/>
-      <c r="T2" s="38"/>
+      <c r="Q2" s="51"/>
+      <c r="R2" s="50"/>
+      <c r="S2" s="41"/>
+      <c r="T2" s="42"/>
     </row>
     <row r="3" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="39"/>
-      <c r="D3" s="42"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="45"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
       <c r="G3" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="H3" s="48" t="s">
+      <c r="H3" s="52" t="s">
         <v>47</v>
       </c>
-      <c r="I3" s="49"/>
-      <c r="J3" s="50"/>
+      <c r="I3" s="53"/>
+      <c r="J3" s="54"/>
       <c r="K3" s="34" t="s">
         <v>89</v>
       </c>
       <c r="L3" s="34" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="M3" s="8"/>
       <c r="N3" s="8"/>
       <c r="O3" s="8"/>
       <c r="P3" s="13"/>
-      <c r="Q3" s="47"/>
-      <c r="R3" s="46"/>
+      <c r="Q3" s="51"/>
+      <c r="R3" s="50"/>
       <c r="S3" s="26" t="s">
         <v>77</v>
       </c>
@@ -1546,7 +1566,7 @@
     </row>
     <row r="6" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C6" s="22">
         <v>1</v>
@@ -1559,7 +1579,7 @@
       </c>
       <c r="F6" s="6">
         <f t="shared" si="0"/>
-        <v>30.799999999999997</v>
+        <v>37.1</v>
       </c>
       <c r="G6" s="10">
         <v>1</v>
@@ -1574,7 +1594,7 @@
         <v>0.75</v>
       </c>
       <c r="K6" s="10">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="L6" s="10">
         <v>0.9</v>
@@ -1830,7 +1850,7 @@
     </row>
     <row r="12" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C12" s="22">
         <v>1</v>
@@ -1843,7 +1863,7 @@
       </c>
       <c r="F12" s="6">
         <f t="shared" si="0"/>
-        <v>42.8</v>
+        <v>49.1</v>
       </c>
       <c r="G12" s="10">
         <v>1</v>
@@ -1858,7 +1878,7 @@
         <v>0.75</v>
       </c>
       <c r="K12" s="10">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="L12" s="10">
         <v>0.9</v>
@@ -1893,7 +1913,7 @@
       </c>
       <c r="F13" s="6">
         <f t="shared" si="0"/>
-        <v>47.5</v>
+        <v>52.75</v>
       </c>
       <c r="G13" s="10">
         <v>1</v>
@@ -1910,7 +1930,9 @@
       <c r="K13" s="10">
         <v>1</v>
       </c>
-      <c r="L13" s="10"/>
+      <c r="L13" s="10">
+        <v>0.75</v>
+      </c>
       <c r="M13" s="10"/>
       <c r="N13" s="10"/>
       <c r="O13" s="10"/>
@@ -2029,9 +2051,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B16" s="2" t="s">
-        <v>90</v>
+    <row r="16" spans="2:20" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="66" t="s">
+        <v>134</v>
       </c>
       <c r="C16" s="3">
         <v>1</v>
@@ -2134,7 +2156,7 @@
     </row>
     <row r="18" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C18" s="22">
         <v>1</v>
@@ -2147,7 +2169,7 @@
       </c>
       <c r="F18" s="6">
         <f t="shared" si="0"/>
-        <v>35.75</v>
+        <v>46.25</v>
       </c>
       <c r="G18" s="10">
         <v>1</v>
@@ -2162,9 +2184,11 @@
         <v>0.75</v>
       </c>
       <c r="K18" s="10">
-        <v>0</v>
-      </c>
-      <c r="L18" s="10"/>
+        <v>0.75</v>
+      </c>
+      <c r="L18" s="10">
+        <v>0.75</v>
+      </c>
       <c r="M18" s="10"/>
       <c r="N18" s="10"/>
       <c r="O18" s="10"/>
@@ -2235,7 +2259,7 @@
     </row>
     <row r="20" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C20" s="22">
         <v>1</v>
@@ -2385,7 +2409,7 @@
     </row>
     <row r="23" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C23" s="22">
         <v>2</v>
@@ -2398,7 +2422,7 @@
       </c>
       <c r="F23" s="6">
         <f t="shared" si="0"/>
-        <v>34.25</v>
+        <v>44.75</v>
       </c>
       <c r="G23" s="11">
         <v>1</v>
@@ -2413,9 +2437,11 @@
         <v>0.75</v>
       </c>
       <c r="K23" s="10">
-        <v>0</v>
-      </c>
-      <c r="L23" s="10"/>
+        <v>0.75</v>
+      </c>
+      <c r="L23" s="10">
+        <v>0.75</v>
+      </c>
       <c r="M23" s="10"/>
       <c r="N23" s="10"/>
       <c r="O23" s="10"/>
@@ -3131,7 +3157,7 @@
     </row>
     <row r="38" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B38" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C38" s="22">
         <v>1</v>
@@ -3144,7 +3170,7 @@
       </c>
       <c r="F38" s="6">
         <f t="shared" si="0"/>
-        <v>46.5</v>
+        <v>53.5</v>
       </c>
       <c r="G38" s="10">
         <v>1</v>
@@ -3159,7 +3185,7 @@
         <v>0.75</v>
       </c>
       <c r="K38" s="10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L38" s="10">
         <v>1</v>
@@ -3201,11 +3227,11 @@
       </c>
       <c r="K39" s="32">
         <f t="shared" si="2"/>
-        <v>73.529411764705884</v>
+        <v>86.176470588235304</v>
       </c>
       <c r="L39" s="32">
         <f t="shared" si="2"/>
-        <v>93.166666666666657</v>
+        <v>91.515151515151501</v>
       </c>
       <c r="M39" s="32" t="e">
         <f t="shared" si="2"/>
@@ -3233,13 +3259,13 @@
       </c>
     </row>
     <row r="40" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="G40" s="35">
+      <c r="G40" s="39">
         <f>AVERAGE(G39:J39)</f>
         <v>93.566176470588232</v>
       </c>
-      <c r="H40" s="36"/>
-      <c r="I40" s="36"/>
-      <c r="J40" s="36"/>
+      <c r="H40" s="40"/>
+      <c r="I40" s="40"/>
+      <c r="J40" s="40"/>
       <c r="K40" s="25"/>
       <c r="L40" s="25"/>
       <c r="M40" s="25"/>
@@ -3356,143 +3382,178 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{272B4357-72D9-4FFA-86DA-5A8470DFA243}">
-  <dimension ref="B1:G12"/>
+  <dimension ref="B1:H12"/>
   <sheetViews>
-    <sheetView topLeftCell="B5" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="40.7109375" defaultRowHeight="60" customHeight="1" x14ac:dyDescent="0.9"/>
   <cols>
-    <col min="1" max="2" width="40.7109375" style="62"/>
-    <col min="3" max="3" width="55.5703125" style="62" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="50" style="62" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="38.85546875" style="62" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="48" style="62" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="0" style="62" hidden="1" customWidth="1"/>
-    <col min="8" max="16384" width="40.7109375" style="62"/>
+    <col min="1" max="1" width="40.7109375" style="35"/>
+    <col min="2" max="2" width="60.28515625" style="35" customWidth="1"/>
+    <col min="3" max="3" width="38.5703125" style="35" customWidth="1"/>
+    <col min="4" max="4" width="54.5703125" style="35" customWidth="1"/>
+    <col min="5" max="5" width="23.7109375" style="35" customWidth="1"/>
+    <col min="6" max="6" width="38.85546875" style="35" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="48" style="35" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="0" style="35" hidden="1" customWidth="1"/>
+    <col min="9" max="16384" width="40.7109375" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="60" hidden="1" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="B1" s="63" t="s">
+    <row r="1" spans="2:8" ht="60" hidden="1" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="B1" s="36" t="s">
+        <v>109</v>
+      </c>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="35" t="s">
         <v>110</v>
       </c>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="62" t="s">
+    </row>
+    <row r="2" spans="2:8" ht="60" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="B2" s="37" t="s">
+        <v>105</v>
+      </c>
+      <c r="C2" s="37"/>
+      <c r="D2" s="38" t="s">
+        <v>127</v>
+      </c>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="36"/>
+    </row>
+    <row r="3" spans="2:8" ht="60" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="D3" s="35" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" ht="60" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="B4" s="35" t="s">
+        <v>106</v>
+      </c>
+      <c r="C4" s="35" t="s">
+        <v>139</v>
+      </c>
+      <c r="D4" s="35" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" ht="60" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="B5" s="35" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="2" spans="2:7" ht="60" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="B2" s="64" t="s">
-        <v>106</v>
-      </c>
-      <c r="C2" s="65" t="s">
-        <v>128</v>
-      </c>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="63"/>
-    </row>
-    <row r="3" spans="2:7" ht="60" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="C3" s="62" t="s">
+      <c r="D5" s="35" t="s">
+        <v>112</v>
+      </c>
+      <c r="E5" s="35" t="s">
+        <v>113</v>
+      </c>
+      <c r="F5" s="35" t="s">
+        <v>114</v>
+      </c>
+      <c r="G5" s="35" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="4" spans="2:7" ht="60" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="B4" s="62" t="s">
-        <v>107</v>
-      </c>
-      <c r="C4" s="62" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" ht="60" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="B5" s="62" t="s">
-        <v>112</v>
-      </c>
-      <c r="C5" s="62" t="s">
-        <v>113</v>
-      </c>
-      <c r="D5" s="62" t="s">
-        <v>114</v>
-      </c>
-      <c r="E5" s="62" t="s">
+    <row r="6" spans="2:8" ht="60" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="D6" s="67" t="s">
         <v>115</v>
       </c>
-      <c r="F5" s="62" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" ht="60" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="C6" s="62" t="s">
+      <c r="E6" s="67" t="s">
         <v>116</v>
       </c>
-      <c r="D6" s="62" t="s">
+      <c r="F6" s="67" t="s">
         <v>117</v>
       </c>
-      <c r="E6" s="62" t="s">
+      <c r="G6" s="35" t="s">
         <v>118</v>
       </c>
-      <c r="F6" s="62" t="s">
+      <c r="H6" s="35" t="s">
         <v>119</v>
       </c>
-      <c r="G6" s="62" t="s">
+    </row>
+    <row r="7" spans="2:8" ht="60" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="B7" s="35" t="s">
+        <v>135</v>
+      </c>
+      <c r="C7" s="35" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="7" spans="2:7" ht="60" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="C7" s="62" t="s">
+      <c r="D7" s="35" t="s">
         <v>130</v>
       </c>
-      <c r="E7" s="62" t="s">
+      <c r="F7" s="35" t="s">
+        <v>120</v>
+      </c>
+      <c r="G7" s="35" t="s">
         <v>121</v>
       </c>
-      <c r="F7" s="62" t="s">
+    </row>
+    <row r="8" spans="2:8" ht="60" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="B8" s="35" t="s">
+        <v>136</v>
+      </c>
+      <c r="C8" s="35" t="s">
+        <v>123</v>
+      </c>
+      <c r="D8" s="35" t="s">
+        <v>131</v>
+      </c>
+      <c r="F8" s="35" t="s">
+        <v>120</v>
+      </c>
+      <c r="G8" s="35" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="8" spans="2:7" ht="60" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="C8" s="62" t="s">
-        <v>131</v>
-      </c>
-      <c r="E8" s="62" t="s">
-        <v>121</v>
-      </c>
-      <c r="F8" s="62" t="s">
+    <row r="9" spans="2:8" ht="60" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="B9" s="35" t="s">
+        <v>137</v>
+      </c>
+      <c r="C9" s="35" t="s">
+        <v>120</v>
+      </c>
+      <c r="D9" s="35" t="s">
+        <v>132</v>
+      </c>
+      <c r="F9" s="35" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="9" spans="2:7" ht="60" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="C9" s="62" t="s">
-        <v>132</v>
-      </c>
-      <c r="E9" s="62" t="s">
-        <v>121</v>
-      </c>
-      <c r="F9" s="62" t="s">
+      <c r="G9" s="35" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" ht="60" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="B10" s="35" t="s">
+        <v>138</v>
+      </c>
+      <c r="C10" s="35" t="s">
+        <v>120</v>
+      </c>
+      <c r="D10" s="35" t="s">
+        <v>133</v>
+      </c>
+      <c r="F10" s="35" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" ht="60" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="D11" s="67" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="10" spans="2:7" ht="60" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="C10" s="62" t="s">
-        <v>133</v>
-      </c>
-      <c r="E10" s="62" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7" ht="60" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="C11" s="62" t="s">
+      <c r="E11" s="67"/>
+      <c r="F11" s="67"/>
+    </row>
+    <row r="12" spans="2:8" ht="60" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="D12" s="67" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="12" spans="2:7" ht="60" customHeight="1" x14ac:dyDescent="0.9">
-      <c r="C12" s="62" t="s">
-        <v>127</v>
-      </c>
+      <c r="E12" s="67"/>
+      <c r="F12" s="67"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3512,27 +3573,27 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
@@ -3543,7 +3604,7 @@
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
@@ -3554,32 +3615,32 @@
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -3608,30 +3669,30 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>102</v>
+      </c>
+      <c r="B25" t="s">
         <v>103</v>
-      </c>
-      <c r="B25" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -3660,15 +3721,15 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>102</v>
+      </c>
+      <c r="B36" t="s">
         <v>103</v>
-      </c>
-      <c r="B36" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -3715,21 +3776,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.7">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="60" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
-      <c r="J1" s="56"/>
-      <c r="K1" s="56"/>
-      <c r="L1" s="56"/>
-      <c r="M1" s="56"/>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
+      <c r="H1" s="60"/>
+      <c r="I1" s="60"/>
+      <c r="J1" s="60"/>
+      <c r="K1" s="60"/>
+      <c r="L1" s="60"/>
+      <c r="M1" s="60"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.7">
       <c r="A2" s="24">
@@ -3850,603 +3911,608 @@
       <c r="Q2" s="2"/>
     </row>
     <row r="3" spans="5:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E3" s="58">
-        <v>1</v>
-      </c>
-      <c r="F3" s="60" t="s">
+      <c r="E3" s="61">
+        <v>1</v>
+      </c>
+      <c r="F3" s="63" t="s">
         <v>51</v>
       </c>
-      <c r="G3" s="61"/>
-      <c r="H3" s="61"/>
-      <c r="I3" s="61"/>
-      <c r="J3" s="61"/>
-      <c r="K3" s="61"/>
-      <c r="L3" s="61"/>
-      <c r="M3" s="61"/>
-      <c r="N3" s="61"/>
-      <c r="O3" s="61"/>
-      <c r="P3" s="61"/>
-      <c r="Q3" s="61"/>
-      <c r="S3" s="58" t="s">
+      <c r="G3" s="64"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="64"/>
+      <c r="J3" s="64"/>
+      <c r="K3" s="64"/>
+      <c r="L3" s="64"/>
+      <c r="M3" s="64"/>
+      <c r="N3" s="64"/>
+      <c r="O3" s="64"/>
+      <c r="P3" s="64"/>
+      <c r="Q3" s="64"/>
+      <c r="S3" s="61" t="s">
         <v>58</v>
       </c>
-      <c r="T3" s="58"/>
-      <c r="U3" s="58"/>
-      <c r="W3" s="57" t="s">
+      <c r="T3" s="61"/>
+      <c r="U3" s="61"/>
+      <c r="W3" s="65" t="s">
         <v>60</v>
       </c>
-      <c r="X3" s="57"/>
+      <c r="X3" s="65"/>
     </row>
     <row r="4" spans="5:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E4" s="58"/>
-      <c r="F4" s="61"/>
-      <c r="G4" s="61"/>
-      <c r="H4" s="61"/>
-      <c r="I4" s="61"/>
-      <c r="J4" s="61"/>
-      <c r="K4" s="61"/>
-      <c r="L4" s="61"/>
-      <c r="M4" s="61"/>
-      <c r="N4" s="61"/>
-      <c r="O4" s="61"/>
-      <c r="P4" s="61"/>
-      <c r="Q4" s="61"/>
-      <c r="S4" s="58"/>
-      <c r="T4" s="58"/>
-      <c r="U4" s="58"/>
-      <c r="W4" s="57"/>
-      <c r="X4" s="57"/>
+      <c r="E4" s="61"/>
+      <c r="F4" s="64"/>
+      <c r="G4" s="64"/>
+      <c r="H4" s="64"/>
+      <c r="I4" s="64"/>
+      <c r="J4" s="64"/>
+      <c r="K4" s="64"/>
+      <c r="L4" s="64"/>
+      <c r="M4" s="64"/>
+      <c r="N4" s="64"/>
+      <c r="O4" s="64"/>
+      <c r="P4" s="64"/>
+      <c r="Q4" s="64"/>
+      <c r="S4" s="61"/>
+      <c r="T4" s="61"/>
+      <c r="U4" s="61"/>
+      <c r="W4" s="65"/>
+      <c r="X4" s="65"/>
     </row>
     <row r="5" spans="5:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E5" s="58"/>
-      <c r="F5" s="61"/>
-      <c r="G5" s="61"/>
-      <c r="H5" s="61"/>
-      <c r="I5" s="61"/>
-      <c r="J5" s="61"/>
-      <c r="K5" s="61"/>
-      <c r="L5" s="61"/>
-      <c r="M5" s="61"/>
-      <c r="N5" s="61"/>
-      <c r="O5" s="61"/>
-      <c r="P5" s="61"/>
-      <c r="Q5" s="61"/>
-      <c r="S5" s="58"/>
-      <c r="T5" s="58"/>
-      <c r="U5" s="58"/>
-      <c r="W5" s="57"/>
-      <c r="X5" s="57"/>
+      <c r="E5" s="61"/>
+      <c r="F5" s="64"/>
+      <c r="G5" s="64"/>
+      <c r="H5" s="64"/>
+      <c r="I5" s="64"/>
+      <c r="J5" s="64"/>
+      <c r="K5" s="64"/>
+      <c r="L5" s="64"/>
+      <c r="M5" s="64"/>
+      <c r="N5" s="64"/>
+      <c r="O5" s="64"/>
+      <c r="P5" s="64"/>
+      <c r="Q5" s="64"/>
+      <c r="S5" s="61"/>
+      <c r="T5" s="61"/>
+      <c r="U5" s="61"/>
+      <c r="W5" s="65"/>
+      <c r="X5" s="65"/>
     </row>
     <row r="6" spans="5:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E6" s="58"/>
-      <c r="F6" s="61"/>
-      <c r="G6" s="61"/>
-      <c r="H6" s="61"/>
-      <c r="I6" s="61"/>
-      <c r="J6" s="61"/>
-      <c r="K6" s="61"/>
-      <c r="L6" s="61"/>
-      <c r="M6" s="61"/>
-      <c r="N6" s="61"/>
-      <c r="O6" s="61"/>
-      <c r="P6" s="61"/>
-      <c r="Q6" s="61"/>
-      <c r="S6" s="58"/>
-      <c r="T6" s="58"/>
-      <c r="U6" s="58"/>
-      <c r="W6" s="57"/>
-      <c r="X6" s="57"/>
+      <c r="E6" s="61"/>
+      <c r="F6" s="64"/>
+      <c r="G6" s="64"/>
+      <c r="H6" s="64"/>
+      <c r="I6" s="64"/>
+      <c r="J6" s="64"/>
+      <c r="K6" s="64"/>
+      <c r="L6" s="64"/>
+      <c r="M6" s="64"/>
+      <c r="N6" s="64"/>
+      <c r="O6" s="64"/>
+      <c r="P6" s="64"/>
+      <c r="Q6" s="64"/>
+      <c r="S6" s="61"/>
+      <c r="T6" s="61"/>
+      <c r="U6" s="61"/>
+      <c r="W6" s="65"/>
+      <c r="X6" s="65"/>
     </row>
     <row r="7" spans="5:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E7" s="58"/>
-      <c r="F7" s="61"/>
-      <c r="G7" s="61"/>
-      <c r="H7" s="61"/>
-      <c r="I7" s="61"/>
-      <c r="J7" s="61"/>
-      <c r="K7" s="61"/>
-      <c r="L7" s="61"/>
-      <c r="M7" s="61"/>
-      <c r="N7" s="61"/>
-      <c r="O7" s="61"/>
-      <c r="P7" s="61"/>
-      <c r="Q7" s="61"/>
-      <c r="S7" s="58"/>
-      <c r="T7" s="58"/>
-      <c r="U7" s="58"/>
-      <c r="W7" s="57"/>
-      <c r="X7" s="57"/>
+      <c r="E7" s="61"/>
+      <c r="F7" s="64"/>
+      <c r="G7" s="64"/>
+      <c r="H7" s="64"/>
+      <c r="I7" s="64"/>
+      <c r="J7" s="64"/>
+      <c r="K7" s="64"/>
+      <c r="L7" s="64"/>
+      <c r="M7" s="64"/>
+      <c r="N7" s="64"/>
+      <c r="O7" s="64"/>
+      <c r="P7" s="64"/>
+      <c r="Q7" s="64"/>
+      <c r="S7" s="61"/>
+      <c r="T7" s="61"/>
+      <c r="U7" s="61"/>
+      <c r="W7" s="65"/>
+      <c r="X7" s="65"/>
     </row>
     <row r="8" spans="5:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E8" s="58">
+      <c r="E8" s="61">
         <v>2</v>
       </c>
-      <c r="F8" s="60" t="s">
+      <c r="F8" s="63" t="s">
         <v>52</v>
       </c>
-      <c r="G8" s="61"/>
-      <c r="H8" s="61"/>
-      <c r="I8" s="61"/>
-      <c r="J8" s="61"/>
-      <c r="K8" s="61"/>
-      <c r="L8" s="61"/>
-      <c r="M8" s="61"/>
-      <c r="N8" s="61"/>
-      <c r="O8" s="61"/>
-      <c r="P8" s="61"/>
-      <c r="Q8" s="61"/>
-      <c r="S8" s="58" t="s">
+      <c r="G8" s="64"/>
+      <c r="H8" s="64"/>
+      <c r="I8" s="64"/>
+      <c r="J8" s="64"/>
+      <c r="K8" s="64"/>
+      <c r="L8" s="64"/>
+      <c r="M8" s="64"/>
+      <c r="N8" s="64"/>
+      <c r="O8" s="64"/>
+      <c r="P8" s="64"/>
+      <c r="Q8" s="64"/>
+      <c r="S8" s="61" t="s">
         <v>58</v>
       </c>
-      <c r="T8" s="58"/>
-      <c r="U8" s="58"/>
-      <c r="W8" s="57" t="s">
+      <c r="T8" s="61"/>
+      <c r="U8" s="61"/>
+      <c r="W8" s="65" t="s">
         <v>61</v>
       </c>
-      <c r="X8" s="57"/>
+      <c r="X8" s="65"/>
     </row>
     <row r="9" spans="5:24" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E9" s="58"/>
-      <c r="F9" s="61"/>
-      <c r="G9" s="61"/>
-      <c r="H9" s="61"/>
-      <c r="I9" s="61"/>
-      <c r="J9" s="61"/>
-      <c r="K9" s="61"/>
-      <c r="L9" s="61"/>
-      <c r="M9" s="61"/>
-      <c r="N9" s="61"/>
-      <c r="O9" s="61"/>
-      <c r="P9" s="61"/>
-      <c r="Q9" s="61"/>
-      <c r="S9" s="58"/>
-      <c r="T9" s="58"/>
-      <c r="U9" s="58"/>
-      <c r="W9" s="57"/>
-      <c r="X9" s="57"/>
+      <c r="E9" s="61"/>
+      <c r="F9" s="64"/>
+      <c r="G9" s="64"/>
+      <c r="H9" s="64"/>
+      <c r="I9" s="64"/>
+      <c r="J9" s="64"/>
+      <c r="K9" s="64"/>
+      <c r="L9" s="64"/>
+      <c r="M9" s="64"/>
+      <c r="N9" s="64"/>
+      <c r="O9" s="64"/>
+      <c r="P9" s="64"/>
+      <c r="Q9" s="64"/>
+      <c r="S9" s="61"/>
+      <c r="T9" s="61"/>
+      <c r="U9" s="61"/>
+      <c r="W9" s="65"/>
+      <c r="X9" s="65"/>
     </row>
     <row r="10" spans="5:24" x14ac:dyDescent="0.25">
-      <c r="E10" s="58">
+      <c r="E10" s="61">
         <v>3</v>
       </c>
-      <c r="F10" s="60" t="s">
+      <c r="F10" s="63" t="s">
         <v>53</v>
       </c>
-      <c r="G10" s="61"/>
-      <c r="H10" s="61"/>
-      <c r="I10" s="60" t="s">
+      <c r="G10" s="64"/>
+      <c r="H10" s="64"/>
+      <c r="I10" s="63" t="s">
         <v>64</v>
       </c>
-      <c r="J10" s="61"/>
-      <c r="K10" s="61"/>
-      <c r="L10" s="61"/>
-      <c r="M10" s="61"/>
-      <c r="N10" s="61"/>
-      <c r="O10" s="61"/>
-      <c r="P10" s="61"/>
-      <c r="Q10" s="61"/>
-      <c r="S10" s="59" t="s">
+      <c r="J10" s="64"/>
+      <c r="K10" s="64"/>
+      <c r="L10" s="64"/>
+      <c r="M10" s="64"/>
+      <c r="N10" s="64"/>
+      <c r="O10" s="64"/>
+      <c r="P10" s="64"/>
+      <c r="Q10" s="64"/>
+      <c r="S10" s="62" t="s">
         <v>59</v>
       </c>
-      <c r="T10" s="58"/>
-      <c r="U10" s="58"/>
-      <c r="W10" s="57" t="s">
+      <c r="T10" s="61"/>
+      <c r="U10" s="61"/>
+      <c r="W10" s="65" t="s">
         <v>62</v>
       </c>
-      <c r="X10" s="57" t="s">
+      <c r="X10" s="65" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="11" spans="5:24" x14ac:dyDescent="0.25">
-      <c r="E11" s="58"/>
-      <c r="F11" s="61"/>
-      <c r="G11" s="61"/>
-      <c r="H11" s="61"/>
-      <c r="I11" s="61"/>
-      <c r="J11" s="61"/>
-      <c r="K11" s="61"/>
-      <c r="L11" s="61"/>
-      <c r="M11" s="61"/>
-      <c r="N11" s="61"/>
-      <c r="O11" s="61"/>
-      <c r="P11" s="61"/>
-      <c r="Q11" s="61"/>
-      <c r="S11" s="58"/>
-      <c r="T11" s="58"/>
-      <c r="U11" s="58"/>
-      <c r="W11" s="57"/>
-      <c r="X11" s="57"/>
+      <c r="E11" s="61"/>
+      <c r="F11" s="64"/>
+      <c r="G11" s="64"/>
+      <c r="H11" s="64"/>
+      <c r="I11" s="64"/>
+      <c r="J11" s="64"/>
+      <c r="K11" s="64"/>
+      <c r="L11" s="64"/>
+      <c r="M11" s="64"/>
+      <c r="N11" s="64"/>
+      <c r="O11" s="64"/>
+      <c r="P11" s="64"/>
+      <c r="Q11" s="64"/>
+      <c r="S11" s="61"/>
+      <c r="T11" s="61"/>
+      <c r="U11" s="61"/>
+      <c r="W11" s="65"/>
+      <c r="X11" s="65"/>
     </row>
     <row r="12" spans="5:24" x14ac:dyDescent="0.25">
-      <c r="E12" s="58"/>
-      <c r="F12" s="61"/>
-      <c r="G12" s="61"/>
-      <c r="H12" s="61"/>
-      <c r="I12" s="61"/>
-      <c r="J12" s="61"/>
-      <c r="K12" s="61"/>
-      <c r="L12" s="61"/>
-      <c r="M12" s="61"/>
-      <c r="N12" s="61"/>
-      <c r="O12" s="61"/>
-      <c r="P12" s="61"/>
-      <c r="Q12" s="61"/>
-      <c r="S12" s="58"/>
-      <c r="T12" s="58"/>
-      <c r="U12" s="58"/>
-      <c r="W12" s="57"/>
-      <c r="X12" s="57"/>
+      <c r="E12" s="61"/>
+      <c r="F12" s="64"/>
+      <c r="G12" s="64"/>
+      <c r="H12" s="64"/>
+      <c r="I12" s="64"/>
+      <c r="J12" s="64"/>
+      <c r="K12" s="64"/>
+      <c r="L12" s="64"/>
+      <c r="M12" s="64"/>
+      <c r="N12" s="64"/>
+      <c r="O12" s="64"/>
+      <c r="P12" s="64"/>
+      <c r="Q12" s="64"/>
+      <c r="S12" s="61"/>
+      <c r="T12" s="61"/>
+      <c r="U12" s="61"/>
+      <c r="W12" s="65"/>
+      <c r="X12" s="65"/>
     </row>
     <row r="13" spans="5:24" x14ac:dyDescent="0.25">
-      <c r="E13" s="58"/>
-      <c r="F13" s="61"/>
-      <c r="G13" s="61"/>
-      <c r="H13" s="61"/>
-      <c r="I13" s="61"/>
-      <c r="J13" s="61"/>
-      <c r="K13" s="61"/>
-      <c r="L13" s="61"/>
-      <c r="M13" s="61"/>
-      <c r="N13" s="61"/>
-      <c r="O13" s="61"/>
-      <c r="P13" s="61"/>
-      <c r="Q13" s="61"/>
-      <c r="S13" s="58"/>
-      <c r="T13" s="58"/>
-      <c r="U13" s="58"/>
-      <c r="W13" s="57"/>
-      <c r="X13" s="57"/>
+      <c r="E13" s="61"/>
+      <c r="F13" s="64"/>
+      <c r="G13" s="64"/>
+      <c r="H13" s="64"/>
+      <c r="I13" s="64"/>
+      <c r="J13" s="64"/>
+      <c r="K13" s="64"/>
+      <c r="L13" s="64"/>
+      <c r="M13" s="64"/>
+      <c r="N13" s="64"/>
+      <c r="O13" s="64"/>
+      <c r="P13" s="64"/>
+      <c r="Q13" s="64"/>
+      <c r="S13" s="61"/>
+      <c r="T13" s="61"/>
+      <c r="U13" s="61"/>
+      <c r="W13" s="65"/>
+      <c r="X13" s="65"/>
     </row>
     <row r="14" spans="5:24" x14ac:dyDescent="0.25">
-      <c r="E14" s="58"/>
-      <c r="F14" s="61"/>
-      <c r="G14" s="61"/>
-      <c r="H14" s="61"/>
-      <c r="I14" s="61"/>
-      <c r="J14" s="61"/>
-      <c r="K14" s="61"/>
-      <c r="L14" s="61"/>
-      <c r="M14" s="61"/>
-      <c r="N14" s="61"/>
-      <c r="O14" s="61"/>
-      <c r="P14" s="61"/>
-      <c r="Q14" s="61"/>
-      <c r="S14" s="58"/>
-      <c r="T14" s="58"/>
-      <c r="U14" s="58"/>
-      <c r="W14" s="57"/>
-      <c r="X14" s="57"/>
+      <c r="E14" s="61"/>
+      <c r="F14" s="64"/>
+      <c r="G14" s="64"/>
+      <c r="H14" s="64"/>
+      <c r="I14" s="64"/>
+      <c r="J14" s="64"/>
+      <c r="K14" s="64"/>
+      <c r="L14" s="64"/>
+      <c r="M14" s="64"/>
+      <c r="N14" s="64"/>
+      <c r="O14" s="64"/>
+      <c r="P14" s="64"/>
+      <c r="Q14" s="64"/>
+      <c r="S14" s="61"/>
+      <c r="T14" s="61"/>
+      <c r="U14" s="61"/>
+      <c r="W14" s="65"/>
+      <c r="X14" s="65"/>
     </row>
     <row r="15" spans="5:24" x14ac:dyDescent="0.25">
-      <c r="E15" s="58"/>
-      <c r="F15" s="61"/>
-      <c r="G15" s="61"/>
-      <c r="H15" s="61"/>
-      <c r="I15" s="61"/>
-      <c r="J15" s="61"/>
-      <c r="K15" s="61"/>
-      <c r="L15" s="61"/>
-      <c r="M15" s="61"/>
-      <c r="N15" s="61"/>
-      <c r="O15" s="61"/>
-      <c r="P15" s="61"/>
-      <c r="Q15" s="61"/>
-      <c r="S15" s="58"/>
-      <c r="T15" s="58"/>
-      <c r="U15" s="58"/>
-      <c r="W15" s="57"/>
-      <c r="X15" s="57"/>
+      <c r="E15" s="61"/>
+      <c r="F15" s="64"/>
+      <c r="G15" s="64"/>
+      <c r="H15" s="64"/>
+      <c r="I15" s="64"/>
+      <c r="J15" s="64"/>
+      <c r="K15" s="64"/>
+      <c r="L15" s="64"/>
+      <c r="M15" s="64"/>
+      <c r="N15" s="64"/>
+      <c r="O15" s="64"/>
+      <c r="P15" s="64"/>
+      <c r="Q15" s="64"/>
+      <c r="S15" s="61"/>
+      <c r="T15" s="61"/>
+      <c r="U15" s="61"/>
+      <c r="W15" s="65"/>
+      <c r="X15" s="65"/>
     </row>
     <row r="16" spans="5:24" x14ac:dyDescent="0.25">
-      <c r="E16" s="58"/>
-      <c r="F16" s="61"/>
-      <c r="G16" s="61"/>
-      <c r="H16" s="61"/>
-      <c r="I16" s="61"/>
-      <c r="J16" s="61"/>
-      <c r="K16" s="61"/>
-      <c r="L16" s="61"/>
-      <c r="M16" s="61"/>
-      <c r="N16" s="61"/>
-      <c r="O16" s="61"/>
-      <c r="P16" s="61"/>
-      <c r="Q16" s="61"/>
-      <c r="S16" s="58"/>
-      <c r="T16" s="58"/>
-      <c r="U16" s="58"/>
-      <c r="W16" s="57"/>
-      <c r="X16" s="57"/>
+      <c r="E16" s="61"/>
+      <c r="F16" s="64"/>
+      <c r="G16" s="64"/>
+      <c r="H16" s="64"/>
+      <c r="I16" s="64"/>
+      <c r="J16" s="64"/>
+      <c r="K16" s="64"/>
+      <c r="L16" s="64"/>
+      <c r="M16" s="64"/>
+      <c r="N16" s="64"/>
+      <c r="O16" s="64"/>
+      <c r="P16" s="64"/>
+      <c r="Q16" s="64"/>
+      <c r="S16" s="61"/>
+      <c r="T16" s="61"/>
+      <c r="U16" s="61"/>
+      <c r="W16" s="65"/>
+      <c r="X16" s="65"/>
     </row>
     <row r="17" spans="5:24" x14ac:dyDescent="0.25">
-      <c r="E17" s="58"/>
-      <c r="F17" s="61"/>
-      <c r="G17" s="61"/>
-      <c r="H17" s="61"/>
-      <c r="I17" s="61"/>
-      <c r="J17" s="61"/>
-      <c r="K17" s="61"/>
-      <c r="L17" s="61"/>
-      <c r="M17" s="61"/>
-      <c r="N17" s="61"/>
-      <c r="O17" s="61"/>
-      <c r="P17" s="61"/>
-      <c r="Q17" s="61"/>
-      <c r="S17" s="58"/>
-      <c r="T17" s="58"/>
-      <c r="U17" s="58"/>
-      <c r="W17" s="57"/>
-      <c r="X17" s="57"/>
+      <c r="E17" s="61"/>
+      <c r="F17" s="64"/>
+      <c r="G17" s="64"/>
+      <c r="H17" s="64"/>
+      <c r="I17" s="64"/>
+      <c r="J17" s="64"/>
+      <c r="K17" s="64"/>
+      <c r="L17" s="64"/>
+      <c r="M17" s="64"/>
+      <c r="N17" s="64"/>
+      <c r="O17" s="64"/>
+      <c r="P17" s="64"/>
+      <c r="Q17" s="64"/>
+      <c r="S17" s="61"/>
+      <c r="T17" s="61"/>
+      <c r="U17" s="61"/>
+      <c r="W17" s="65"/>
+      <c r="X17" s="65"/>
     </row>
     <row r="18" spans="5:24" x14ac:dyDescent="0.25">
-      <c r="E18" s="58"/>
-      <c r="F18" s="61"/>
-      <c r="G18" s="61"/>
-      <c r="H18" s="61"/>
-      <c r="I18" s="61"/>
-      <c r="J18" s="61"/>
-      <c r="K18" s="61"/>
-      <c r="L18" s="61"/>
-      <c r="M18" s="61"/>
-      <c r="N18" s="61"/>
-      <c r="O18" s="61"/>
-      <c r="P18" s="61"/>
-      <c r="Q18" s="61"/>
-      <c r="S18" s="58"/>
-      <c r="T18" s="58"/>
-      <c r="U18" s="58"/>
-      <c r="W18" s="57"/>
-      <c r="X18" s="57"/>
+      <c r="E18" s="61"/>
+      <c r="F18" s="64"/>
+      <c r="G18" s="64"/>
+      <c r="H18" s="64"/>
+      <c r="I18" s="64"/>
+      <c r="J18" s="64"/>
+      <c r="K18" s="64"/>
+      <c r="L18" s="64"/>
+      <c r="M18" s="64"/>
+      <c r="N18" s="64"/>
+      <c r="O18" s="64"/>
+      <c r="P18" s="64"/>
+      <c r="Q18" s="64"/>
+      <c r="S18" s="61"/>
+      <c r="T18" s="61"/>
+      <c r="U18" s="61"/>
+      <c r="W18" s="65"/>
+      <c r="X18" s="65"/>
     </row>
     <row r="19" spans="5:24" x14ac:dyDescent="0.25">
-      <c r="E19" s="58"/>
-      <c r="F19" s="61"/>
-      <c r="G19" s="61"/>
-      <c r="H19" s="61"/>
-      <c r="I19" s="61"/>
-      <c r="J19" s="61"/>
-      <c r="K19" s="61"/>
-      <c r="L19" s="61"/>
-      <c r="M19" s="61"/>
-      <c r="N19" s="61"/>
-      <c r="O19" s="61"/>
-      <c r="P19" s="61"/>
-      <c r="Q19" s="61"/>
-      <c r="S19" s="58"/>
-      <c r="T19" s="58"/>
-      <c r="U19" s="58"/>
-      <c r="W19" s="57"/>
-      <c r="X19" s="57"/>
+      <c r="E19" s="61"/>
+      <c r="F19" s="64"/>
+      <c r="G19" s="64"/>
+      <c r="H19" s="64"/>
+      <c r="I19" s="64"/>
+      <c r="J19" s="64"/>
+      <c r="K19" s="64"/>
+      <c r="L19" s="64"/>
+      <c r="M19" s="64"/>
+      <c r="N19" s="64"/>
+      <c r="O19" s="64"/>
+      <c r="P19" s="64"/>
+      <c r="Q19" s="64"/>
+      <c r="S19" s="61"/>
+      <c r="T19" s="61"/>
+      <c r="U19" s="61"/>
+      <c r="W19" s="65"/>
+      <c r="X19" s="65"/>
     </row>
     <row r="20" spans="5:24" x14ac:dyDescent="0.25">
-      <c r="E20" s="58"/>
-      <c r="F20" s="61"/>
-      <c r="G20" s="61"/>
-      <c r="H20" s="61"/>
-      <c r="I20" s="61"/>
-      <c r="J20" s="61"/>
-      <c r="K20" s="61"/>
-      <c r="L20" s="61"/>
-      <c r="M20" s="61"/>
-      <c r="N20" s="61"/>
-      <c r="O20" s="61"/>
-      <c r="P20" s="61"/>
-      <c r="Q20" s="61"/>
-      <c r="S20" s="58"/>
-      <c r="T20" s="58"/>
-      <c r="U20" s="58"/>
-      <c r="W20" s="57"/>
-      <c r="X20" s="57"/>
+      <c r="E20" s="61"/>
+      <c r="F20" s="64"/>
+      <c r="G20" s="64"/>
+      <c r="H20" s="64"/>
+      <c r="I20" s="64"/>
+      <c r="J20" s="64"/>
+      <c r="K20" s="64"/>
+      <c r="L20" s="64"/>
+      <c r="M20" s="64"/>
+      <c r="N20" s="64"/>
+      <c r="O20" s="64"/>
+      <c r="P20" s="64"/>
+      <c r="Q20" s="64"/>
+      <c r="S20" s="61"/>
+      <c r="T20" s="61"/>
+      <c r="U20" s="61"/>
+      <c r="W20" s="65"/>
+      <c r="X20" s="65"/>
     </row>
     <row r="21" spans="5:24" x14ac:dyDescent="0.25">
-      <c r="E21" s="58"/>
-      <c r="F21" s="61"/>
-      <c r="G21" s="61"/>
-      <c r="H21" s="61"/>
-      <c r="I21" s="61"/>
-      <c r="J21" s="61"/>
-      <c r="K21" s="61"/>
-      <c r="L21" s="61"/>
-      <c r="M21" s="61"/>
-      <c r="N21" s="61"/>
-      <c r="O21" s="61"/>
-      <c r="P21" s="61"/>
-      <c r="Q21" s="61"/>
-      <c r="S21" s="58"/>
-      <c r="T21" s="58"/>
-      <c r="U21" s="58"/>
-      <c r="W21" s="57"/>
-      <c r="X21" s="57"/>
+      <c r="E21" s="61"/>
+      <c r="F21" s="64"/>
+      <c r="G21" s="64"/>
+      <c r="H21" s="64"/>
+      <c r="I21" s="64"/>
+      <c r="J21" s="64"/>
+      <c r="K21" s="64"/>
+      <c r="L21" s="64"/>
+      <c r="M21" s="64"/>
+      <c r="N21" s="64"/>
+      <c r="O21" s="64"/>
+      <c r="P21" s="64"/>
+      <c r="Q21" s="64"/>
+      <c r="S21" s="61"/>
+      <c r="T21" s="61"/>
+      <c r="U21" s="61"/>
+      <c r="W21" s="65"/>
+      <c r="X21" s="65"/>
     </row>
     <row r="22" spans="5:24" x14ac:dyDescent="0.25">
-      <c r="E22" s="58"/>
-      <c r="F22" s="61"/>
-      <c r="G22" s="61"/>
-      <c r="H22" s="61"/>
-      <c r="I22" s="61"/>
-      <c r="J22" s="61"/>
-      <c r="K22" s="61"/>
-      <c r="L22" s="61"/>
-      <c r="M22" s="61"/>
-      <c r="N22" s="61"/>
-      <c r="O22" s="61"/>
-      <c r="P22" s="61"/>
-      <c r="Q22" s="61"/>
-      <c r="S22" s="58"/>
-      <c r="T22" s="58"/>
-      <c r="U22" s="58"/>
-      <c r="W22" s="57"/>
-      <c r="X22" s="57"/>
+      <c r="E22" s="61"/>
+      <c r="F22" s="64"/>
+      <c r="G22" s="64"/>
+      <c r="H22" s="64"/>
+      <c r="I22" s="64"/>
+      <c r="J22" s="64"/>
+      <c r="K22" s="64"/>
+      <c r="L22" s="64"/>
+      <c r="M22" s="64"/>
+      <c r="N22" s="64"/>
+      <c r="O22" s="64"/>
+      <c r="P22" s="64"/>
+      <c r="Q22" s="64"/>
+      <c r="S22" s="61"/>
+      <c r="T22" s="61"/>
+      <c r="U22" s="61"/>
+      <c r="W22" s="65"/>
+      <c r="X22" s="65"/>
     </row>
     <row r="23" spans="5:24" x14ac:dyDescent="0.25">
-      <c r="E23" s="58"/>
-      <c r="F23" s="61"/>
-      <c r="G23" s="61"/>
-      <c r="H23" s="61"/>
-      <c r="I23" s="61"/>
-      <c r="J23" s="61"/>
-      <c r="K23" s="61"/>
-      <c r="L23" s="61"/>
-      <c r="M23" s="61"/>
-      <c r="N23" s="61"/>
-      <c r="O23" s="61"/>
-      <c r="P23" s="61"/>
-      <c r="Q23" s="61"/>
-      <c r="S23" s="58"/>
-      <c r="T23" s="58"/>
-      <c r="U23" s="58"/>
-      <c r="W23" s="57"/>
-      <c r="X23" s="57"/>
+      <c r="E23" s="61"/>
+      <c r="F23" s="64"/>
+      <c r="G23" s="64"/>
+      <c r="H23" s="64"/>
+      <c r="I23" s="64"/>
+      <c r="J23" s="64"/>
+      <c r="K23" s="64"/>
+      <c r="L23" s="64"/>
+      <c r="M23" s="64"/>
+      <c r="N23" s="64"/>
+      <c r="O23" s="64"/>
+      <c r="P23" s="64"/>
+      <c r="Q23" s="64"/>
+      <c r="S23" s="61"/>
+      <c r="T23" s="61"/>
+      <c r="U23" s="61"/>
+      <c r="W23" s="65"/>
+      <c r="X23" s="65"/>
     </row>
     <row r="24" spans="5:24" x14ac:dyDescent="0.25">
-      <c r="E24" s="58"/>
-      <c r="F24" s="61"/>
-      <c r="G24" s="61"/>
-      <c r="H24" s="61"/>
-      <c r="I24" s="61"/>
-      <c r="J24" s="61"/>
-      <c r="K24" s="61"/>
-      <c r="L24" s="61"/>
-      <c r="M24" s="61"/>
-      <c r="N24" s="61"/>
-      <c r="O24" s="61"/>
-      <c r="P24" s="61"/>
-      <c r="Q24" s="61"/>
-      <c r="S24" s="58"/>
-      <c r="T24" s="58"/>
-      <c r="U24" s="58"/>
-      <c r="W24" s="57"/>
-      <c r="X24" s="57"/>
+      <c r="E24" s="61"/>
+      <c r="F24" s="64"/>
+      <c r="G24" s="64"/>
+      <c r="H24" s="64"/>
+      <c r="I24" s="64"/>
+      <c r="J24" s="64"/>
+      <c r="K24" s="64"/>
+      <c r="L24" s="64"/>
+      <c r="M24" s="64"/>
+      <c r="N24" s="64"/>
+      <c r="O24" s="64"/>
+      <c r="P24" s="64"/>
+      <c r="Q24" s="64"/>
+      <c r="S24" s="61"/>
+      <c r="T24" s="61"/>
+      <c r="U24" s="61"/>
+      <c r="W24" s="65"/>
+      <c r="X24" s="65"/>
     </row>
     <row r="25" spans="5:24" x14ac:dyDescent="0.25">
-      <c r="E25" s="58"/>
-      <c r="F25" s="61"/>
-      <c r="G25" s="61"/>
-      <c r="H25" s="61"/>
-      <c r="I25" s="61"/>
-      <c r="J25" s="61"/>
-      <c r="K25" s="61"/>
-      <c r="L25" s="61"/>
-      <c r="M25" s="61"/>
-      <c r="N25" s="61"/>
-      <c r="O25" s="61"/>
-      <c r="P25" s="61"/>
-      <c r="Q25" s="61"/>
-      <c r="S25" s="58"/>
-      <c r="T25" s="58"/>
-      <c r="U25" s="58"/>
-      <c r="W25" s="57"/>
-      <c r="X25" s="57"/>
+      <c r="E25" s="61"/>
+      <c r="F25" s="64"/>
+      <c r="G25" s="64"/>
+      <c r="H25" s="64"/>
+      <c r="I25" s="64"/>
+      <c r="J25" s="64"/>
+      <c r="K25" s="64"/>
+      <c r="L25" s="64"/>
+      <c r="M25" s="64"/>
+      <c r="N25" s="64"/>
+      <c r="O25" s="64"/>
+      <c r="P25" s="64"/>
+      <c r="Q25" s="64"/>
+      <c r="S25" s="61"/>
+      <c r="T25" s="61"/>
+      <c r="U25" s="61"/>
+      <c r="W25" s="65"/>
+      <c r="X25" s="65"/>
     </row>
     <row r="26" spans="5:24" x14ac:dyDescent="0.25">
-      <c r="E26" s="58"/>
-      <c r="F26" s="61"/>
-      <c r="G26" s="61"/>
-      <c r="H26" s="61"/>
-      <c r="I26" s="61"/>
-      <c r="J26" s="61"/>
-      <c r="K26" s="61"/>
-      <c r="L26" s="61"/>
-      <c r="M26" s="61"/>
-      <c r="N26" s="61"/>
-      <c r="O26" s="61"/>
-      <c r="P26" s="61"/>
-      <c r="Q26" s="61"/>
-      <c r="S26" s="58"/>
-      <c r="T26" s="58"/>
-      <c r="U26" s="58"/>
-      <c r="W26" s="57"/>
-      <c r="X26" s="57"/>
+      <c r="E26" s="61"/>
+      <c r="F26" s="64"/>
+      <c r="G26" s="64"/>
+      <c r="H26" s="64"/>
+      <c r="I26" s="64"/>
+      <c r="J26" s="64"/>
+      <c r="K26" s="64"/>
+      <c r="L26" s="64"/>
+      <c r="M26" s="64"/>
+      <c r="N26" s="64"/>
+      <c r="O26" s="64"/>
+      <c r="P26" s="64"/>
+      <c r="Q26" s="64"/>
+      <c r="S26" s="61"/>
+      <c r="T26" s="61"/>
+      <c r="U26" s="61"/>
+      <c r="W26" s="65"/>
+      <c r="X26" s="65"/>
     </row>
     <row r="27" spans="5:24" x14ac:dyDescent="0.25">
-      <c r="E27" s="58"/>
-      <c r="F27" s="61"/>
-      <c r="G27" s="61"/>
-      <c r="H27" s="61"/>
-      <c r="I27" s="61"/>
-      <c r="J27" s="61"/>
-      <c r="K27" s="61"/>
-      <c r="L27" s="61"/>
-      <c r="M27" s="61"/>
-      <c r="N27" s="61"/>
-      <c r="O27" s="61"/>
-      <c r="P27" s="61"/>
-      <c r="Q27" s="61"/>
-      <c r="S27" s="58"/>
-      <c r="T27" s="58"/>
-      <c r="U27" s="58"/>
-      <c r="W27" s="57"/>
-      <c r="X27" s="57"/>
+      <c r="E27" s="61"/>
+      <c r="F27" s="64"/>
+      <c r="G27" s="64"/>
+      <c r="H27" s="64"/>
+      <c r="I27" s="64"/>
+      <c r="J27" s="64"/>
+      <c r="K27" s="64"/>
+      <c r="L27" s="64"/>
+      <c r="M27" s="64"/>
+      <c r="N27" s="64"/>
+      <c r="O27" s="64"/>
+      <c r="P27" s="64"/>
+      <c r="Q27" s="64"/>
+      <c r="S27" s="61"/>
+      <c r="T27" s="61"/>
+      <c r="U27" s="61"/>
+      <c r="W27" s="65"/>
+      <c r="X27" s="65"/>
     </row>
     <row r="28" spans="5:24" x14ac:dyDescent="0.25">
-      <c r="E28" s="58"/>
-      <c r="F28" s="61"/>
-      <c r="G28" s="61"/>
-      <c r="H28" s="61"/>
-      <c r="I28" s="61"/>
-      <c r="J28" s="61"/>
-      <c r="K28" s="61"/>
-      <c r="L28" s="61"/>
-      <c r="M28" s="61"/>
-      <c r="N28" s="61"/>
-      <c r="O28" s="61"/>
-      <c r="P28" s="61"/>
-      <c r="Q28" s="61"/>
-      <c r="S28" s="58"/>
-      <c r="T28" s="58"/>
-      <c r="U28" s="58"/>
-      <c r="W28" s="57"/>
-      <c r="X28" s="57"/>
+      <c r="E28" s="61"/>
+      <c r="F28" s="64"/>
+      <c r="G28" s="64"/>
+      <c r="H28" s="64"/>
+      <c r="I28" s="64"/>
+      <c r="J28" s="64"/>
+      <c r="K28" s="64"/>
+      <c r="L28" s="64"/>
+      <c r="M28" s="64"/>
+      <c r="N28" s="64"/>
+      <c r="O28" s="64"/>
+      <c r="P28" s="64"/>
+      <c r="Q28" s="64"/>
+      <c r="S28" s="61"/>
+      <c r="T28" s="61"/>
+      <c r="U28" s="61"/>
+      <c r="W28" s="65"/>
+      <c r="X28" s="65"/>
     </row>
     <row r="29" spans="5:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E29" s="58">
+      <c r="E29" s="61">
         <v>4</v>
       </c>
-      <c r="F29" s="60" t="s">
+      <c r="F29" s="63" t="s">
         <v>54</v>
       </c>
-      <c r="G29" s="61"/>
-      <c r="H29" s="61"/>
-      <c r="I29" s="61"/>
-      <c r="J29" s="61"/>
-      <c r="K29" s="61"/>
-      <c r="L29" s="61"/>
-      <c r="M29" s="61"/>
-      <c r="N29" s="61"/>
-      <c r="O29" s="61"/>
-      <c r="P29" s="61"/>
-      <c r="Q29" s="61"/>
-      <c r="S29" s="58" t="s">
+      <c r="G29" s="64"/>
+      <c r="H29" s="64"/>
+      <c r="I29" s="64"/>
+      <c r="J29" s="64"/>
+      <c r="K29" s="64"/>
+      <c r="L29" s="64"/>
+      <c r="M29" s="64"/>
+      <c r="N29" s="64"/>
+      <c r="O29" s="64"/>
+      <c r="P29" s="64"/>
+      <c r="Q29" s="64"/>
+      <c r="S29" s="61" t="s">
         <v>58</v>
       </c>
-      <c r="T29" s="58"/>
-      <c r="U29" s="58"/>
-      <c r="W29" s="57" t="s">
+      <c r="T29" s="61"/>
+      <c r="U29" s="61"/>
+      <c r="W29" s="65" t="s">
         <v>65</v>
       </c>
-      <c r="X29" s="57"/>
+      <c r="X29" s="65"/>
     </row>
     <row r="30" spans="5:24" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E30" s="58"/>
-      <c r="F30" s="61"/>
-      <c r="G30" s="61"/>
-      <c r="H30" s="61"/>
-      <c r="I30" s="61"/>
-      <c r="J30" s="61"/>
-      <c r="K30" s="61"/>
-      <c r="L30" s="61"/>
-      <c r="M30" s="61"/>
-      <c r="N30" s="61"/>
-      <c r="O30" s="61"/>
-      <c r="P30" s="61"/>
-      <c r="Q30" s="61"/>
-      <c r="S30" s="58"/>
-      <c r="T30" s="58"/>
-      <c r="U30" s="58"/>
-      <c r="W30" s="57"/>
-      <c r="X30" s="57"/>
+      <c r="E30" s="61"/>
+      <c r="F30" s="64"/>
+      <c r="G30" s="64"/>
+      <c r="H30" s="64"/>
+      <c r="I30" s="64"/>
+      <c r="J30" s="64"/>
+      <c r="K30" s="64"/>
+      <c r="L30" s="64"/>
+      <c r="M30" s="64"/>
+      <c r="N30" s="64"/>
+      <c r="O30" s="64"/>
+      <c r="P30" s="64"/>
+      <c r="Q30" s="64"/>
+      <c r="S30" s="61"/>
+      <c r="T30" s="61"/>
+      <c r="U30" s="61"/>
+      <c r="W30" s="65"/>
+      <c r="X30" s="65"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="W3:X7"/>
+    <mergeCell ref="W8:X9"/>
+    <mergeCell ref="W29:X30"/>
+    <mergeCell ref="W10:W28"/>
+    <mergeCell ref="X10:X28"/>
     <mergeCell ref="S3:U7"/>
     <mergeCell ref="S8:U9"/>
     <mergeCell ref="S10:U28"/>
@@ -4460,11 +4526,6 @@
     <mergeCell ref="F10:H28"/>
     <mergeCell ref="I10:Q28"/>
     <mergeCell ref="F29:Q30"/>
-    <mergeCell ref="W3:X7"/>
-    <mergeCell ref="W8:X9"/>
-    <mergeCell ref="W29:X30"/>
-    <mergeCell ref="W10:W28"/>
-    <mergeCell ref="X10:X28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>